<commit_message>
Getting description, initial art, and embeds out of the way
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Mining Pick</t>
   </si>
@@ -69,9 +69,6 @@
     <t>VP</t>
   </si>
   <si>
-    <t xml:space="preserve">Description    </t>
-  </si>
-  <si>
     <t>Snark</t>
   </si>
   <si>
@@ -85,6 +82,15 @@
   </si>
   <si>
     <t>The power of purchase.</t>
+  </si>
+  <si>
+    <t>Two free Stone may be used in this turn's Make</t>
+  </si>
+  <si>
+    <t>We'll strike gold one of these days!</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -447,7 +453,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -460,7 +466,7 @@
     <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -490,10 +496,10 @@
         <v>8</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -507,10 +513,10 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
         <v>20</v>
-      </c>
-      <c r="J2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -527,7 +533,7 @@
         <v>11</v>
       </c>
       <c r="J3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -544,7 +550,7 @@
         <v>9</v>
       </c>
       <c r="J4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -561,7 +567,7 @@
         <v>10</v>
       </c>
       <c r="J5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -588,6 +594,12 @@
       </c>
       <c r="H6" t="s">
         <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Getting costs and vp onto the card
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -453,7 +453,7 @@
   <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +590,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="5">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Expanded out the game design into a playable prototype
Time taken: about 2.5 hours.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
   <si>
     <t>Mining Pick</t>
   </si>
@@ -84,13 +84,166 @@
     <t>The power of purchase.</t>
   </si>
   <si>
-    <t>Two free Stone may be used in this turn's Make</t>
-  </si>
-  <si>
     <t>We'll strike gold one of these days!</t>
   </si>
   <si>
     <t>Description</t>
+  </si>
+  <si>
+    <t>Wood Axe</t>
+  </si>
+  <si>
+    <t>wood-axe</t>
+  </si>
+  <si>
+    <t>And my axe.</t>
+  </si>
+  <si>
+    <t>scales</t>
+  </si>
+  <si>
+    <t>Two free Gold may be used in a Make</t>
+  </si>
+  <si>
+    <t>Three free Wood may be used in a Make</t>
+  </si>
+  <si>
+    <t>Two free Stone may be used in a Make</t>
+  </si>
+  <si>
+    <t>Shiny things! I like shiny things.</t>
+  </si>
+  <si>
+    <t>Smelter</t>
+  </si>
+  <si>
+    <t>How does smelting actually CREATE things?</t>
+  </si>
+  <si>
+    <t>Wheelbarrow</t>
+  </si>
+  <si>
+    <t>wheelbarrow</t>
+  </si>
+  <si>
+    <t>You may keep 2 Resources until the next turn (these do not count against your limit of 5)</t>
+  </si>
+  <si>
+    <t>spade</t>
+  </si>
+  <si>
+    <t>Most people just call this a shovel.</t>
+  </si>
+  <si>
+    <t>Spade</t>
+  </si>
+  <si>
+    <t>Magnet</t>
+  </si>
+  <si>
+    <t>magnet</t>
+  </si>
+  <si>
+    <t>Robot Golem</t>
+  </si>
+  <si>
+    <t>Chalice</t>
+  </si>
+  <si>
+    <t>jeweled-chalice</t>
+  </si>
+  <si>
+    <t>robot-golem</t>
+  </si>
+  <si>
+    <t>Take 2 Steel from the Trash, if available.</t>
+  </si>
+  <si>
+    <t>Medieval Turret</t>
+  </si>
+  <si>
+    <t>Steel may be used for any Resource</t>
+  </si>
+  <si>
+    <t>stone-tower</t>
+  </si>
+  <si>
+    <t>Galleon</t>
+  </si>
+  <si>
+    <t>galleon</t>
+  </si>
+  <si>
+    <t>Wood may be used for any Resource.</t>
+  </si>
+  <si>
+    <t>Three free Steel may be used in a Make</t>
+  </si>
+  <si>
+    <t>axe-in-stump</t>
+  </si>
+  <si>
+    <t>Draw a card from your deck, if it's Wood, draw two more cards.</t>
+  </si>
+  <si>
+    <t>Lumberjack</t>
+  </si>
+  <si>
+    <t>stone-spear</t>
+  </si>
+  <si>
+    <t>Gold may be used for any Three Resources.</t>
+  </si>
+  <si>
+    <t>Stone may be used for any Two Resources.</t>
+  </si>
+  <si>
+    <t>Rockslide</t>
+  </si>
+  <si>
+    <t>falling-rocks</t>
+  </si>
+  <si>
+    <t>Take one Stone from the Trash, if available.</t>
+  </si>
+  <si>
+    <t>Super Spade</t>
+  </si>
+  <si>
+    <t>Draw two cards from your deck.</t>
+  </si>
+  <si>
+    <t>Draw one two cards from your deck.</t>
+  </si>
+  <si>
+    <t>sword-spade</t>
+  </si>
+  <si>
+    <t>thrown-charcoal</t>
+  </si>
+  <si>
+    <t>Spear</t>
+  </si>
+  <si>
+    <t>Gold Merchant</t>
+  </si>
+  <si>
+    <t>locked-chest</t>
+  </si>
+  <si>
+    <t>Draw 1 card and take 2 Gold from the Trash (if available).</t>
+  </si>
+  <si>
+    <t>War Chest</t>
+  </si>
+  <si>
+    <t>Barrel</t>
+  </si>
+  <si>
+    <t>barrel</t>
+  </si>
+  <si>
+    <t>You may keep 3 Resources until the next turn (these do not count against your limit of 5).</t>
   </si>
 </sst>
 </file>
@@ -134,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -148,6 +301,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -450,15 +612,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B2" sqref="B2:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="5"/>
     <col min="3" max="3" width="10" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.140625" style="3" bestFit="1" customWidth="1"/>
@@ -466,8 +628,8 @@
     <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="40" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -495,10 +657,10 @@
       <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="I1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>17</v>
       </c>
     </row>
@@ -507,7 +669,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G2" s="5">
         <v>0</v>
@@ -515,7 +677,7 @@
       <c r="H2" t="s">
         <v>19</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -524,7 +686,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="5">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="G3" s="5">
         <v>0</v>
@@ -532,7 +694,7 @@
       <c r="H3" t="s">
         <v>11</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="8" t="s">
         <v>20</v>
       </c>
     </row>
@@ -541,7 +703,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
@@ -549,7 +711,7 @@
       <c r="H4" t="s">
         <v>9</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="8" t="s">
         <v>18</v>
       </c>
     </row>
@@ -558,7 +720,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
@@ -566,7 +728,7 @@
       <c r="H5" t="s">
         <v>10</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="8" t="s">
         <v>21</v>
       </c>
     </row>
@@ -595,11 +757,421 @@
       <c r="H6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>23</v>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2</v>
+      </c>
+      <c r="H7" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5">
+        <v>2</v>
+      </c>
+      <c r="H8" t="s">
+        <v>27</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="5">
+        <v>1</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="5">
+        <v>3</v>
+      </c>
+      <c r="H9" t="s">
+        <v>67</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="5">
+        <v>2</v>
+      </c>
+      <c r="H10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
+        <v>1</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="5">
+        <v>2</v>
+      </c>
+      <c r="H11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="J11" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
+        <v>1</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="5">
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>41</v>
+      </c>
+      <c r="I12" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="5">
+        <v>2</v>
+      </c>
+      <c r="H13" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
+        <v>1</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="5">
+        <v>2</v>
+      </c>
+      <c r="H14" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="5">
+        <v>2</v>
+      </c>
+      <c r="H15" t="s">
+        <v>61</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>2</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5">
+        <v>2</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="5">
+        <v>5</v>
+      </c>
+      <c r="H16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>73</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="5">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="5">
+        <v>5</v>
+      </c>
+      <c r="H17" t="s">
+        <v>74</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B18" s="5">
+        <v>1</v>
+      </c>
+      <c r="C18" s="5">
+        <v>3</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="5">
+        <v>5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>70</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" s="5">
+        <v>7</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="5">
+        <v>7</v>
+      </c>
+      <c r="H19" t="s">
+        <v>45</v>
+      </c>
+      <c r="I19" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="5">
+        <v>1</v>
+      </c>
+      <c r="C20" s="5">
+        <v>6</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5">
+        <v>9</v>
+      </c>
+      <c r="H20" t="s">
+        <v>44</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>47</v>
+      </c>
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" s="5">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="5">
+        <v>7</v>
+      </c>
+      <c r="H21" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <v>7</v>
+      </c>
+      <c r="H22" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Some new cards. VP point calculations
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -7,16 +7,15 @@
     <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="12330"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Deck" sheetId="1" r:id="rId1"/>
+    <sheet name="VPs" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
   <si>
     <t>Mining Pick</t>
   </si>
@@ -244,6 +243,42 @@
   </si>
   <si>
     <t>You may keep 3 Resources until the next turn (these do not count against your limit of 5).</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>VP Rate</t>
+  </si>
+  <si>
+    <t>Throne</t>
+  </si>
+  <si>
+    <t>stone-throne</t>
+  </si>
+  <si>
+    <t>Anvil</t>
+  </si>
+  <si>
+    <t>anvil</t>
+  </si>
+  <si>
+    <t>Stone Tablet</t>
+  </si>
+  <si>
+    <t>stone-tablet</t>
+  </si>
+  <si>
+    <t>Crossbow</t>
+  </si>
+  <si>
+    <t>crossbow</t>
+  </si>
+  <si>
+    <t>Baseball Bat</t>
+  </si>
+  <si>
+    <t>baseball-bat</t>
   </si>
 </sst>
 </file>
@@ -612,10 +647,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B22"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -752,7 +787,8 @@
         <v>2</v>
       </c>
       <c r="G6" s="5">
-        <v>2</v>
+        <f>ROUND(C6*VLOOKUP(D6,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F6,VPs!A$2:B$6,2,FALSE)),0,E6*VLOOKUP(F6,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>3</v>
       </c>
       <c r="H6" t="s">
         <v>12</v>
@@ -784,7 +820,8 @@
         <v>3</v>
       </c>
       <c r="G7" s="5">
-        <v>2</v>
+        <f>ROUND(C7*VLOOKUP(D7,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F7,VPs!A$2:B$6,2,FALSE)),0,E7*VLOOKUP(F7,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>3</v>
       </c>
       <c r="H7" t="s">
         <v>25</v>
@@ -810,6 +847,7 @@
         <v>4</v>
       </c>
       <c r="G8" s="5">
+        <f>ROUND(C8*VLOOKUP(D8,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F8,VPs!A$2:B$6,2,FALSE)),0,E8*VLOOKUP(F8,VPs!A$2:B$6,2,FALSE)),0)</f>
         <v>2</v>
       </c>
       <c r="H8" t="s">
@@ -842,6 +880,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="5">
+        <f>ROUND(C9*VLOOKUP(D9,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F9,VPs!A$2:B$6,2,FALSE)),0,E9*VLOOKUP(F9,VPs!A$2:B$6,2,FALSE)),0)</f>
         <v>3</v>
       </c>
       <c r="H9" t="s">
@@ -868,7 +907,8 @@
         <v>1</v>
       </c>
       <c r="G10" s="5">
-        <v>2</v>
+        <f>ROUND(C10*VLOOKUP(D10,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F10,VPs!A$2:B$6,2,FALSE)),0,E10*VLOOKUP(F10,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>3</v>
       </c>
       <c r="H10" t="s">
         <v>35</v>
@@ -897,7 +937,8 @@
         <v>2</v>
       </c>
       <c r="G11" s="5">
-        <v>2</v>
+        <f>ROUND(C11*VLOOKUP(D11,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F11,VPs!A$2:B$6,2,FALSE)),0,E11*VLOOKUP(F11,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>3</v>
       </c>
       <c r="H11" t="s">
         <v>37</v>
@@ -923,6 +964,7 @@
         <v>2</v>
       </c>
       <c r="G12" s="5">
+        <f>ROUND(C12*VLOOKUP(D12,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F12,VPs!A$2:B$6,2,FALSE)),0,E12*VLOOKUP(F12,VPs!A$2:B$6,2,FALSE)),0)</f>
         <v>1</v>
       </c>
       <c r="H12" t="s">
@@ -946,6 +988,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="5">
+        <f>ROUND(C13*VLOOKUP(D13,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F13,VPs!A$2:B$6,2,FALSE)),0,E13*VLOOKUP(F13,VPs!A$2:B$6,2,FALSE)),0)</f>
         <v>2</v>
       </c>
       <c r="H13" t="s">
@@ -975,7 +1018,8 @@
         <v>3</v>
       </c>
       <c r="G14" s="5">
-        <v>2</v>
+        <f>ROUND(C14*VLOOKUP(D14,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F14,VPs!A$2:B$6,2,FALSE)),0,E14*VLOOKUP(F14,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>3</v>
       </c>
       <c r="H14" t="s">
         <v>57</v>
@@ -998,6 +1042,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="5">
+        <f>ROUND(C15*VLOOKUP(D15,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F15,VPs!A$2:B$6,2,FALSE)),0,E15*VLOOKUP(F15,VPs!A$2:B$6,2,FALSE)),0)</f>
         <v>2</v>
       </c>
       <c r="H15" t="s">
@@ -1009,7 +1054,7 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="B16" s="5">
         <v>1</v>
@@ -1018,50 +1063,46 @@
         <v>2</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E16" s="5">
         <v>2</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G16" s="5">
-        <v>5</v>
+        <f>ROUND(C16*VLOOKUP(D16,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F16,VPs!A$2:B$6,2,FALSE)),0,E16*VLOOKUP(F16,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>66</v>
-      </c>
-      <c r="I16" s="8" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
       </c>
       <c r="C17" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G17" s="5">
+        <f>ROUND(C17*VLOOKUP(D17,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F17,VPs!A$2:B$6,2,FALSE)),0,E17*VLOOKUP(F17,VPs!A$2:B$6,2,FALSE)),0)</f>
         <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>74</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -1070,107 +1111,235 @@
         <v>3</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="5">
+        <f>ROUND(C18*VLOOKUP(D18,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F18,VPs!A$2:B$6,2,FALSE)),0,E18*VLOOKUP(F18,VPs!A$2:B$6,2,FALSE)),0)</f>
         <v>4</v>
       </c>
-      <c r="G18" s="5">
-        <v>5</v>
-      </c>
       <c r="H18" t="s">
-        <v>70</v>
-      </c>
-      <c r="I18" s="8" t="s">
-        <v>71</v>
+        <v>81</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>86</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
       </c>
       <c r="C19" s="5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="5">
-        <v>7</v>
+        <f>ROUND(C19*VLOOKUP(D19,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F19,VPs!A$2:B$6,2,FALSE)),0,E19*VLOOKUP(F19,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>45</v>
-      </c>
-      <c r="I19" s="8" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>84</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
       </c>
       <c r="C20" s="5">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
+      </c>
+      <c r="E20" s="5">
+        <v>2</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="G20" s="5">
-        <v>9</v>
+        <f>ROUND(C20*VLOOKUP(D20,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F20,VPs!A$2:B$6,2,FALSE)),0,E20*VLOOKUP(F20,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>44</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>58</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
       </c>
       <c r="C21" s="5">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5">
+        <v>2</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="5">
+        <f>ROUND(C21*VLOOKUP(D21,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F21,VPs!A$2:B$6,2,FALSE)),0,E21*VLOOKUP(F21,VPs!A$2:B$6,2,FALSE)),0)</f>
         <v>6</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G21" s="5">
-        <v>7</v>
-      </c>
       <c r="H21" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="5">
+        <v>1</v>
+      </c>
+      <c r="C22" s="5">
+        <v>4</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G22" s="5">
+        <f>ROUND(C22*VLOOKUP(D22,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F22,VPs!A$2:B$6,2,FALSE)),0,E22*VLOOKUP(F22,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>5</v>
+      </c>
+      <c r="H22" t="s">
+        <v>74</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>72</v>
+      </c>
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23" s="5">
+        <v>3</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="5">
+        <f>ROUND(C23*VLOOKUP(D23,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F23,VPs!A$2:B$6,2,FALSE)),0,E23*VLOOKUP(F23,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>5</v>
+      </c>
+      <c r="H23" t="s">
+        <v>70</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>42</v>
+      </c>
+      <c r="B24" s="5">
+        <v>1</v>
+      </c>
+      <c r="C24" s="5">
+        <v>7</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" s="5">
+        <f>ROUND(C24*VLOOKUP(D24,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F24,VPs!A$2:B$6,2,FALSE)),0,E24*VLOOKUP(F24,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>10</v>
+      </c>
+      <c r="H24" t="s">
+        <v>45</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="5">
+        <v>1</v>
+      </c>
+      <c r="C25" s="5">
+        <v>6</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="5">
+        <f>ROUND(C25*VLOOKUP(D25,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F25,VPs!A$2:B$6,2,FALSE)),0,E25*VLOOKUP(F25,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>10</v>
+      </c>
+      <c r="H25" t="s">
+        <v>44</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" s="5">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5">
+        <v>6</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="5">
+        <f>ROUND(C26*VLOOKUP(D26,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F26,VPs!A$2:B$6,2,FALSE)),0,E26*VLOOKUP(F26,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>9</v>
+      </c>
+      <c r="H26" t="s">
+        <v>49</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>50</v>
       </c>
-      <c r="B22" s="5">
-        <v>1</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="B27" s="5">
+        <v>1</v>
+      </c>
+      <c r="C27" s="5">
         <v>7</v>
       </c>
-      <c r="D22" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="G22" s="5">
-        <v>7</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="D27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" s="5">
+        <f>ROUND(C27*VLOOKUP(D27,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F27,VPs!A$2:B$6,2,FALSE)),0,E27*VLOOKUP(F27,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <v>9</v>
+      </c>
+      <c r="H27" t="s">
         <v>51</v>
       </c>
-      <c r="I22" s="8" t="s">
+      <c r="I27" s="8" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1181,24 +1350,63 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="7.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1.4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Balance tweaks and pdf creation
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Deck" sheetId="1" r:id="rId1"/>
     <sheet name="VPs" sheetId="2" r:id="rId2"/>
+    <sheet name="Economy" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
   <si>
     <t>Mining Pick</t>
   </si>
@@ -179,15 +180,9 @@
     <t>Three free Steel may be used in a Make</t>
   </si>
   <si>
-    <t>axe-in-stump</t>
-  </si>
-  <si>
     <t>Draw a card from your deck, if it's Wood, draw two more cards.</t>
   </si>
   <si>
-    <t>Lumberjack</t>
-  </si>
-  <si>
     <t>stone-spear</t>
   </si>
   <si>
@@ -279,6 +274,18 @@
   </si>
   <si>
     <t>baseball-bat</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t># Cards Costing</t>
+  </si>
+  <si>
+    <t>Ladder</t>
+  </si>
+  <si>
+    <t>hole-ladder</t>
   </si>
 </sst>
 </file>
@@ -650,7 +657,7 @@
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -835,7 +842,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
@@ -884,7 +891,7 @@
         <v>3</v>
       </c>
       <c r="H9" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="I9" s="8" t="s">
         <v>53</v>
@@ -944,7 +951,7 @@
         <v>37</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J11" s="8" t="s">
         <v>38</v>
@@ -976,7 +983,7 @@
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>56</v>
+        <v>88</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -985,22 +992,22 @@
         <v>1</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G13" s="5">
         <f>ROUND(C13*VLOOKUP(D13,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F13,VPs!A$2:B$6,2,FALSE)),0,E13*VLOOKUP(F13,VPs!A$2:B$6,2,FALSE)),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H13" t="s">
+        <v>89</v>
+      </c>
+      <c r="I13" s="8" t="s">
         <v>54</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -1022,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="H14" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>30</v>
@@ -1030,7 +1037,7 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
@@ -1046,15 +1053,15 @@
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B16" s="5">
         <v>1</v>
@@ -1076,12 +1083,12 @@
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
@@ -1097,12 +1104,12 @@
         <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
@@ -1118,12 +1125,12 @@
         <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
@@ -1139,12 +1146,12 @@
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -1166,12 +1173,12 @@
         <v>5</v>
       </c>
       <c r="H20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
@@ -1193,15 +1200,15 @@
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="I21" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B22" s="5">
         <v>1</v>
@@ -1217,15 +1224,15 @@
         <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
@@ -1241,10 +1248,10 @@
         <v>5</v>
       </c>
       <c r="H23" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="I23" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -1292,7 +1299,7 @@
         <v>44</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -1316,7 +1323,7 @@
         <v>49</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -1363,10 +1370,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1404,6 +1411,88 @@
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3">
+        <f>COUNTIF(Deck!D:D,Economy!A2) + COUNTIF(Deck!F:F,Economy!A2)</f>
+        <v>10</v>
+      </c>
+      <c r="C2" s="3">
+        <f>SUMIF(Deck!D:D,Economy!A2,Deck!C:C) + SUMIF(Deck!F:F,Economy!A2,Deck!E:E)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3">
+        <f>COUNTIF(Deck!D:D,Economy!A3) + COUNTIF(Deck!F:F,Economy!A3)</f>
+        <v>8</v>
+      </c>
+      <c r="C3" s="3">
+        <f>SUMIF(Deck!D:D,Economy!A3,Deck!C:C) + SUMIF(Deck!F:F,Economy!A3,Deck!E:E)</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3">
+        <f>COUNTIF(Deck!D:D,Economy!A4) + COUNTIF(Deck!F:F,Economy!A4)</f>
+        <v>8</v>
+      </c>
+      <c r="C4" s="3">
+        <f>SUMIF(Deck!D:D,Economy!A4,Deck!C:C) + SUMIF(Deck!F:F,Economy!A4,Deck!E:E)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <f>COUNTIF(Deck!D:D,Economy!A5) + COUNTIF(Deck!F:F,Economy!A5)</f>
+        <v>4</v>
+      </c>
+      <c r="C5" s="3">
+        <f>SUMIF(Deck!D:D,Economy!A5,Deck!C:C) + SUMIF(Deck!F:F,Economy!A5,Deck!E:E)</f>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Switched to bonus-per-space instead
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -11,12 +11,19 @@
     <sheet name="VPs" sheetId="2" r:id="rId2"/>
     <sheet name="Economy" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="GoldVP">VPs!$B$5</definedName>
+    <definedName name="SteelVP">VPs!$B$3</definedName>
+    <definedName name="StoneVP">VPs!$B$4</definedName>
+    <definedName name="WoodValue">VPs!$B$2</definedName>
+    <definedName name="WoodVP">VPs!$B$2</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
   <si>
     <t>Mining Pick</t>
   </si>
@@ -33,15 +40,6 @@
     <t>Gold</t>
   </si>
   <si>
-    <t>Cost1Type</t>
-  </si>
-  <si>
-    <t>Cost2Amt</t>
-  </si>
-  <si>
-    <t>Cost2Type</t>
-  </si>
-  <si>
     <t>GameIcon</t>
   </si>
   <si>
@@ -63,9 +61,6 @@
     <t>Qty</t>
   </si>
   <si>
-    <t>Cost1Amt</t>
-  </si>
-  <si>
     <t>VP</t>
   </si>
   <si>
@@ -286,6 +281,24 @@
   </si>
   <si>
     <t>hole-ladder</t>
+  </si>
+  <si>
+    <t>Dog Statue</t>
+  </si>
+  <si>
+    <t>hound</t>
+  </si>
+  <si>
+    <t>Ancient Pyramid</t>
+  </si>
+  <si>
+    <t>mayan-pyramid</t>
+  </si>
+  <si>
+    <t>Windmill</t>
+  </si>
+  <si>
+    <t>windmill</t>
   </si>
 </sst>
 </file>
@@ -359,6 +372,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF732D"/>
+      <color rgb="FF702500"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -654,20 +673,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" style="5"/>
-    <col min="3" max="3" width="10" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="5"/>
     <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="43.7109375" style="8" bestFit="1" customWidth="1"/>
@@ -676,34 +695,34 @@
   <sheetData>
     <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>13</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -713,14 +732,17 @@
       <c r="B2" s="5">
         <v>12</v>
       </c>
+      <c r="C2" s="5">
+        <v>1</v>
+      </c>
       <c r="G2" s="5">
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -730,14 +752,17 @@
       <c r="B3" s="5">
         <v>12</v>
       </c>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
       <c r="G3" s="5">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -747,14 +772,17 @@
       <c r="B4" s="5">
         <v>10</v>
       </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
       <c r="G4" s="5">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -764,14 +792,17 @@
       <c r="B5" s="5">
         <v>6</v>
       </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
       <c r="G5" s="5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -784,32 +815,26 @@
       <c r="C6" s="5">
         <v>1</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
+      <c r="D6" s="5">
+        <v>1</v>
       </c>
       <c r="G6" s="5">
-        <f>ROUND(C6*VLOOKUP(D6,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F6,VPs!A$2:B$6,2,FALSE)),0,E6*VLOOKUP(F6,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C6*WoodVP+D6*SteelVP+E6*StoneVP+F6*GoldVP,0)</f>
         <v>3</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
@@ -817,92 +842,77 @@
       <c r="C7" s="5">
         <v>1</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="E7" s="5">
         <v>1</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="5">
+        <f>ROUND(C7*WoodVP+D7*SteelVP+E7*StoneVP+F7*GoldVP,0)</f>
         <v>3</v>
       </c>
-      <c r="G7" s="5">
-        <f>ROUND(C7*VLOOKUP(D7,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F7,VPs!A$2:B$6,2,FALSE)),0,E7*VLOOKUP(F7,VPs!A$2:B$6,2,FALSE)),0)</f>
-        <v>3</v>
-      </c>
       <c r="H7" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>29</v>
-      </c>
       <c r="J7" s="6" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="C8" s="5">
-        <v>1</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>4</v>
+      <c r="F8" s="5">
+        <v>1</v>
       </c>
       <c r="G8" s="5">
-        <f>ROUND(C8*VLOOKUP(D8,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F8,VPs!A$2:B$6,2,FALSE)),0,E8*VLOOKUP(F8,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0)</f>
         <v>2</v>
       </c>
       <c r="H8" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="8" t="s">
         <v>27</v>
-      </c>
-      <c r="I8" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
-      <c r="C9" s="5">
-        <v>1</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>2</v>
+      <c r="D9" s="5">
+        <v>1</v>
       </c>
       <c r="E9" s="5">
         <v>1</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="5">
+        <f>ROUND(C9*WoodVP+D9*SteelVP+E9*StoneVP+F9*GoldVP,0)</f>
         <v>3</v>
       </c>
-      <c r="G9" s="5">
-        <f>ROUND(C9*VLOOKUP(D9,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F9,VPs!A$2:B$6,2,FALSE)),0,E9*VLOOKUP(F9,VPs!A$2:B$6,2,FALSE)),0)</f>
-        <v>3</v>
-      </c>
       <c r="H9" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
@@ -910,23 +920,20 @@
       <c r="C10" s="5">
         <v>2</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="G10" s="5">
-        <f>ROUND(C10*VLOOKUP(D10,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F10,VPs!A$2:B$6,2,FALSE)),0,E10*VLOOKUP(F10,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C10*WoodVP+D10*SteelVP+E10*StoneVP+F10*GoldVP,0)</f>
         <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
@@ -934,56 +941,47 @@
       <c r="C11" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="5">
-        <v>1</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>2</v>
+      <c r="D11" s="5">
+        <v>1</v>
       </c>
       <c r="G11" s="5">
-        <f>ROUND(C11*VLOOKUP(D11,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F11,VPs!A$2:B$6,2,FALSE)),0,E11*VLOOKUP(F11,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C11*WoodVP+D11*SteelVP+E11*StoneVP+F11*GoldVP,0)</f>
         <v>3</v>
       </c>
       <c r="H11" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B12" s="5">
         <v>1</v>
       </c>
-      <c r="C12" s="5">
-        <v>1</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>2</v>
+      <c r="D12" s="5">
+        <v>1</v>
       </c>
       <c r="G12" s="5">
-        <f>ROUND(C12*VLOOKUP(D12,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F12,VPs!A$2:B$6,2,FALSE)),0,E12*VLOOKUP(F12,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C12*WoodVP+D12*SteelVP+E12*StoneVP+F12*GoldVP,0)</f>
         <v>1</v>
       </c>
       <c r="H12" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
@@ -991,23 +989,20 @@
       <c r="C13" s="5">
         <v>1</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="G13" s="5">
-        <f>ROUND(C13*VLOOKUP(D13,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F13,VPs!A$2:B$6,2,FALSE)),0,E13*VLOOKUP(F13,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C13*WoodVP+D13*SteelVP+E13*StoneVP+F13*GoldVP,0)</f>
         <v>1</v>
       </c>
       <c r="H13" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
@@ -1015,122 +1010,101 @@
       <c r="C14" s="5">
         <v>1</v>
       </c>
-      <c r="D14" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="E14" s="5">
         <v>1</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="5">
+        <f>ROUND(C14*WoodVP+D14*SteelVP+E14*StoneVP+F14*GoldVP,0)</f>
         <v>3</v>
       </c>
-      <c r="G14" s="5">
-        <f>ROUND(C14*VLOOKUP(D14,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F14,VPs!A$2:B$6,2,FALSE)),0,E14*VLOOKUP(F14,VPs!A$2:B$6,2,FALSE)),0)</f>
-        <v>3</v>
-      </c>
       <c r="H14" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
       </c>
-      <c r="C15" s="5">
-        <v>1</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>3</v>
+      <c r="E15" s="5">
+        <v>1</v>
       </c>
       <c r="G15" s="5">
-        <f>ROUND(C15*VLOOKUP(D15,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F15,VPs!A$2:B$6,2,FALSE)),0,E15*VLOOKUP(F15,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C15*WoodVP+D15*SteelVP+E15*StoneVP+F15*GoldVP,0)</f>
         <v>2</v>
       </c>
       <c r="H15" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B16" s="5">
         <v>1</v>
-      </c>
-      <c r="C16" s="5">
-        <v>2</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>3</v>
       </c>
       <c r="E16" s="5">
         <v>2</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>4</v>
+      <c r="F16" s="5">
+        <v>2</v>
       </c>
       <c r="G16" s="5">
-        <f>ROUND(C16*VLOOKUP(D16,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F16,VPs!A$2:B$6,2,FALSE)),0,E16*VLOOKUP(F16,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C16*WoodVP+D16*SteelVP+E16*StoneVP+F16*GoldVP,0)</f>
         <v>6</v>
       </c>
       <c r="H16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
       </c>
-      <c r="C17" s="5">
+      <c r="E17" s="5">
         <v>3</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="G17" s="5">
-        <f>ROUND(C17*VLOOKUP(D17,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F17,VPs!A$2:B$6,2,FALSE)),0,E17*VLOOKUP(F17,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C17*WoodVP+D17*SteelVP+E17*StoneVP+F17*GoldVP,0)</f>
         <v>5</v>
       </c>
       <c r="H17" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
       </c>
-      <c r="C18" s="5">
+      <c r="D18" s="5">
         <v>3</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="G18" s="5">
-        <f>ROUND(C18*VLOOKUP(D18,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F18,VPs!A$2:B$6,2,FALSE)),0,E18*VLOOKUP(F18,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C18*WoodVP+D18*SteelVP+E18*StoneVP+F18*GoldVP,0)</f>
         <v>4</v>
       </c>
       <c r="H18" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
@@ -1138,216 +1112,255 @@
       <c r="C19" s="5">
         <v>3</v>
       </c>
-      <c r="D19" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="G19" s="5">
-        <f>ROUND(C19*VLOOKUP(D19,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F19,VPs!A$2:B$6,2,FALSE)),0,E19*VLOOKUP(F19,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C19*WoodVP+D19*SteelVP+E19*StoneVP+F19*GoldVP,0)</f>
         <v>4</v>
       </c>
       <c r="H19" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
       </c>
       <c r="C20" s="5">
-        <v>2</v>
-      </c>
-      <c r="D20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="5">
         <v>1</v>
       </c>
       <c r="E20" s="5">
-        <v>2</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F20" s="5">
+        <v>1</v>
       </c>
       <c r="G20" s="5">
-        <f>ROUND(C20*VLOOKUP(D20,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F20,VPs!A$2:B$6,2,FALSE)),0,E20*VLOOKUP(F20,VPs!A$2:B$6,2,FALSE)),0)</f>
-        <v>5</v>
+        <f>ROUND(C20*WoodVP+D20*SteelVP+E20*StoneVP+F20*GoldVP,0)</f>
+        <v>6</v>
       </c>
       <c r="H20" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>88</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
       </c>
-      <c r="C21" s="5">
-        <v>2</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>2</v>
+      <c r="D21" s="5">
+        <v>1</v>
       </c>
       <c r="E21" s="5">
         <v>2</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>3</v>
+      <c r="F21" s="5">
+        <v>1</v>
       </c>
       <c r="G21" s="5">
-        <f>ROUND(C21*VLOOKUP(D21,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F21,VPs!A$2:B$6,2,FALSE)),0,E21*VLOOKUP(F21,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C21*WoodVP+D21*SteelVP+E21*StoneVP+F21*GoldVP,0)</f>
         <v>6</v>
       </c>
       <c r="H21" t="s">
-        <v>64</v>
-      </c>
-      <c r="I21" s="8" t="s">
-        <v>62</v>
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B22" s="5">
         <v>1</v>
       </c>
       <c r="C22" s="5">
-        <v>4</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="D22" s="5">
+        <v>2</v>
       </c>
       <c r="G22" s="5">
-        <f>ROUND(C22*VLOOKUP(D22,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F22,VPs!A$2:B$6,2,FALSE)),0,E22*VLOOKUP(F22,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C22*WoodVP+D22*SteelVP+E22*StoneVP+F22*GoldVP,0)</f>
         <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>72</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
       </c>
       <c r="C23" s="5">
-        <v>3</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="D23" s="5">
+        <v>2</v>
       </c>
       <c r="G23" s="5">
-        <f>ROUND(C23*VLOOKUP(D23,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F23,VPs!A$2:B$6,2,FALSE)),0,E23*VLOOKUP(F23,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C23*WoodVP+D23*SteelVP+E23*StoneVP+F23*GoldVP,0)</f>
         <v>5</v>
       </c>
       <c r="H23" t="s">
-        <v>68</v>
-      </c>
-      <c r="I23" s="8" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
       </c>
-      <c r="C24" s="5">
-        <v>7</v>
-      </c>
-      <c r="D24" s="3" t="s">
+      <c r="D24" s="5">
         <v>2</v>
       </c>
+      <c r="E24" s="5">
+        <v>2</v>
+      </c>
       <c r="G24" s="5">
-        <f>ROUND(C24*VLOOKUP(D24,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F24,VPs!A$2:B$6,2,FALSE)),0,E24*VLOOKUP(F24,VPs!A$2:B$6,2,FALSE)),0)</f>
-        <v>10</v>
+        <f>ROUND(C24*WoodVP+D24*SteelVP+E24*StoneVP+F24*GoldVP,0)</f>
+        <v>6</v>
       </c>
       <c r="H24" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="I24" s="8" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>43</v>
+        <v>67</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>6</v>
-      </c>
-      <c r="D25" s="3" t="s">
         <v>4</v>
       </c>
       <c r="G25" s="5">
-        <f>ROUND(C25*VLOOKUP(D25,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F25,VPs!A$2:B$6,2,FALSE)),0,E25*VLOOKUP(F25,VPs!A$2:B$6,2,FALSE)),0)</f>
-        <v>10</v>
+        <f>ROUND(C25*WoodVP+D25*SteelVP+E25*StoneVP+F25*GoldVP,0)</f>
+        <v>5</v>
       </c>
       <c r="H25" t="s">
-        <v>44</v>
+        <v>68</v>
       </c>
       <c r="I25" s="8" t="s">
-        <v>56</v>
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
       </c>
-      <c r="C26" s="5">
-        <v>6</v>
-      </c>
-      <c r="D26" s="3" t="s">
+      <c r="F26" s="5">
         <v>3</v>
       </c>
       <c r="G26" s="5">
-        <f>ROUND(C26*VLOOKUP(D26,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F26,VPs!A$2:B$6,2,FALSE)),0,E26*VLOOKUP(F26,VPs!A$2:B$6,2,FALSE)),0)</f>
-        <v>9</v>
+        <f>ROUND(C26*WoodVP+D26*SteelVP+E26*StoneVP+F26*GoldVP,0)</f>
+        <v>5</v>
       </c>
       <c r="H26" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>38</v>
       </c>
       <c r="B27" s="5">
         <v>1</v>
       </c>
-      <c r="C27" s="5">
+      <c r="D27" s="5">
         <v>7</v>
       </c>
-      <c r="D27" s="3" t="s">
-        <v>1</v>
-      </c>
       <c r="G27" s="5">
-        <f>ROUND(C27*VLOOKUP(D27,VPs!A$2:B$5,2,FALSE) + IF(ISNA(VLOOKUP(F27,VPs!A$2:B$6,2,FALSE)),0,E27*VLOOKUP(F27,VPs!A$2:B$6,2,FALSE)),0)</f>
+        <f>ROUND(C27*WoodVP+D27*SteelVP+E27*StoneVP+F27*GoldVP,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H27" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>39</v>
+      </c>
+      <c r="B28" s="5">
+        <v>1</v>
+      </c>
+      <c r="F28" s="5">
+        <v>6</v>
+      </c>
+      <c r="G28" s="5">
+        <f>ROUND(C28*WoodVP+D28*SteelVP+E28*StoneVP+F28*GoldVP,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H28" t="s">
+        <v>40</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="5">
+        <v>1</v>
+      </c>
+      <c r="E29" s="5">
+        <v>6</v>
+      </c>
+      <c r="G29" s="5">
+        <f>ROUND(C29*WoodVP+D29*SteelVP+E29*StoneVP+F29*GoldVP,0)</f>
         <v>9</v>
       </c>
-      <c r="H27" t="s">
-        <v>51</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>52</v>
+      <c r="H29" t="s">
+        <v>45</v>
+      </c>
+      <c r="I29" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="5">
+        <v>1</v>
+      </c>
+      <c r="C30" s="5">
+        <v>7</v>
+      </c>
+      <c r="G30" s="5">
+        <f>ROUND(C30*WoodVP+D30*SteelVP+E30*StoneVP+F30*GoldVP,0)</f>
+        <v>9</v>
+      </c>
+      <c r="H30" t="s">
+        <v>47</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1357,10 +1370,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1370,10 +1383,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1406,11 +1419,6 @@
       </c>
       <c r="B5">
         <v>1.6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -1423,7 +1431,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1434,65 +1442,65 @@
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
-        <f>COUNTIF(Deck!D:D,Economy!A2) + COUNTIF(Deck!F:F,Economy!A2)</f>
-        <v>10</v>
-      </c>
-      <c r="C2" s="3">
-        <f>SUMIF(Deck!D:D,Economy!A2,Deck!C:C) + SUMIF(Deck!F:F,Economy!A2,Deck!E:E)</f>
-        <v>23</v>
+      <c r="B2" s="3" t="e">
+        <f>COUNTIF(Deck!#REF!,Economy!A2) + COUNTIF(Deck!#REF!,Economy!A2)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C2" s="3" t="e">
+        <f>SUMIF(Deck!#REF!,Economy!A2,Deck!#REF!) + SUMIF(Deck!#REF!,Economy!A2,Deck!#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <f>COUNTIF(Deck!D:D,Economy!A3) + COUNTIF(Deck!F:F,Economy!A3)</f>
-        <v>8</v>
-      </c>
-      <c r="C3" s="3">
-        <f>SUMIF(Deck!D:D,Economy!A3,Deck!C:C) + SUMIF(Deck!F:F,Economy!A3,Deck!E:E)</f>
-        <v>18</v>
+      <c r="B3" s="3" t="e">
+        <f>COUNTIF(Deck!#REF!,Economy!A3) + COUNTIF(Deck!#REF!,Economy!A3)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C3" s="3" t="e">
+        <f>SUMIF(Deck!#REF!,Economy!A3,Deck!#REF!) + SUMIF(Deck!#REF!,Economy!A3,Deck!#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <f>COUNTIF(Deck!D:D,Economy!A4) + COUNTIF(Deck!F:F,Economy!A4)</f>
-        <v>8</v>
-      </c>
-      <c r="C4" s="3">
-        <f>SUMIF(Deck!D:D,Economy!A4,Deck!C:C) + SUMIF(Deck!F:F,Economy!A4,Deck!E:E)</f>
-        <v>17</v>
+      <c r="B4" s="3" t="e">
+        <f>COUNTIF(Deck!#REF!,Economy!A4) + COUNTIF(Deck!#REF!,Economy!A4)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C4" s="3" t="e">
+        <f>SUMIF(Deck!#REF!,Economy!A4,Deck!#REF!) + SUMIF(Deck!#REF!,Economy!A4,Deck!#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
-        <f>COUNTIF(Deck!D:D,Economy!A5) + COUNTIF(Deck!F:F,Economy!A5)</f>
-        <v>4</v>
-      </c>
-      <c r="C5" s="3">
-        <f>SUMIF(Deck!D:D,Economy!A5,Deck!C:C) + SUMIF(Deck!F:F,Economy!A5,Deck!E:E)</f>
-        <v>12</v>
+      <c r="B5" s="3" t="e">
+        <f>COUNTIF(Deck!#REF!,Economy!A5) + COUNTIF(Deck!#REF!,Economy!A5)</f>
+        <v>#REF!</v>
+      </c>
+      <c r="C5" s="3" t="e">
+        <f>SUMIF(Deck!#REF!,Economy!A5,Deck!#REF!) + SUMIF(Deck!#REF!,Economy!A5,Deck!#REF!)</f>
+        <v>#REF!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Game balance after first playtest (many more cards overall)
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="117">
   <si>
     <t>Mining Pick</t>
   </si>
@@ -70,9 +70,6 @@
     <t>Build it strong, build it right.</t>
   </si>
   <si>
-    <t>planks</t>
-  </si>
-  <si>
     <t>Building must start somewhere.</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Most people just call this a shovel.</t>
   </si>
   <si>
-    <t>Spade</t>
-  </si>
-  <si>
     <t>Magnet</t>
   </si>
   <si>
@@ -175,9 +169,6 @@
     <t>Three free Steel may be used in a Make</t>
   </si>
   <si>
-    <t>Draw a card from your deck, if it's Wood, draw two more cards.</t>
-  </si>
-  <si>
     <t>stone-spear</t>
   </si>
   <si>
@@ -202,9 +193,6 @@
     <t>Draw two cards from your deck.</t>
   </si>
   <si>
-    <t>Draw one two cards from your deck.</t>
-  </si>
-  <si>
     <t>sword-spade</t>
   </si>
   <si>
@@ -271,9 +259,6 @@
     <t>baseball-bat</t>
   </si>
   <si>
-    <t>Total Cost</t>
-  </si>
-  <si>
     <t># Cards Costing</t>
   </si>
   <si>
@@ -283,12 +268,6 @@
     <t>hole-ladder</t>
   </si>
   <si>
-    <t>Dog Statue</t>
-  </si>
-  <si>
-    <t>hound</t>
-  </si>
-  <si>
     <t>Ancient Pyramid</t>
   </si>
   <si>
@@ -299,6 +278,102 @@
   </si>
   <si>
     <t>windmill</t>
+  </si>
+  <si>
+    <t>A Log</t>
+  </si>
+  <si>
+    <t>Bunch of Logs</t>
+  </si>
+  <si>
+    <t>log</t>
+  </si>
+  <si>
+    <t>wood-pile</t>
+  </si>
+  <si>
+    <t>Necklace</t>
+  </si>
+  <si>
+    <t>gem-chain</t>
+  </si>
+  <si>
+    <t>gem-pendant</t>
+  </si>
+  <si>
+    <t>Pendant</t>
+  </si>
+  <si>
+    <t>Normal Spade</t>
+  </si>
+  <si>
+    <t>Stone Spade</t>
+  </si>
+  <si>
+    <t>Draw one card from your deck.</t>
+  </si>
+  <si>
+    <t>Solid Spade</t>
+  </si>
+  <si>
+    <t>Pile of Nails</t>
+  </si>
+  <si>
+    <t>A Stone</t>
+  </si>
+  <si>
+    <t>A Gold Bar</t>
+  </si>
+  <si>
+    <t>Crate</t>
+  </si>
+  <si>
+    <t>wooden-crate</t>
+  </si>
+  <si>
+    <t>Chains</t>
+  </si>
+  <si>
+    <t>wavy-chains</t>
+  </si>
+  <si>
+    <t>Total Economy</t>
+  </si>
+  <si>
+    <t>Lumbermill</t>
+  </si>
+  <si>
+    <t>bolt-saw</t>
+  </si>
+  <si>
+    <t>At game end, 1 VP per "A Log" and 2 VP per "Bunch of Logs"</t>
+  </si>
+  <si>
+    <t>Boots</t>
+  </si>
+  <si>
+    <t>boots</t>
+  </si>
+  <si>
+    <t>Upon purchase, draw two cards and place them directly in your discard pile.</t>
+  </si>
+  <si>
+    <t>Awesome Armor</t>
+  </si>
+  <si>
+    <t>overlord-helm</t>
+  </si>
+  <si>
+    <t>Screwdriver</t>
+  </si>
+  <si>
+    <t>screwdriver</t>
+  </si>
+  <si>
+    <t>Draw a card from your deck, if it's only Wood (no bonuses), draw one more card.</t>
+  </si>
+  <si>
+    <t>Draw a card from your deck, if it's only Steel or only Stone (no bonuses), draw one more card.</t>
   </si>
 </sst>
 </file>
@@ -673,10 +748,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,7 +794,7 @@
         <v>5</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>13</v>
@@ -727,10 +802,10 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>85</v>
       </c>
       <c r="B2" s="5">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C2" s="5">
         <v>1</v>
@@ -739,230 +814,205 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>15</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="B3" s="5">
-        <v>12</v>
-      </c>
-      <c r="D3" s="5">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
       </c>
       <c r="G3" s="5">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" s="8" t="s">
-        <v>16</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>97</v>
       </c>
       <c r="B4" s="5">
-        <v>10</v>
-      </c>
-      <c r="E4" s="5">
+        <v>8</v>
+      </c>
+      <c r="D4" s="5">
         <v>1</v>
       </c>
       <c r="G4" s="5">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>98</v>
       </c>
       <c r="B5" s="5">
-        <v>6</v>
-      </c>
-      <c r="F5" s="5">
+        <v>8</v>
+      </c>
+      <c r="E5" s="5">
         <v>1</v>
       </c>
       <c r="G5" s="5">
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="5">
+        <v>6</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="5">
         <v>0</v>
       </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="G6" s="5">
-        <f>ROUND(C6*WoodVP+D6*SteelVP+E6*StoneVP+F6*GoldVP,0)</f>
-        <v>3</v>
-      </c>
       <c r="H6" t="s">
-        <v>9</v>
-      </c>
-      <c r="I6" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="J6" s="6" t="s">
-        <v>18</v>
+        <v>7</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
       </c>
-      <c r="C7" s="5">
-        <v>1</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="D7" s="5">
         <v>1</v>
       </c>
       <c r="G7" s="5">
         <f>ROUND(C7*WoodVP+D7*SteelVP+E7*StoneVP+F7*GoldVP,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="6" t="s">
-        <v>22</v>
+        <v>35</v>
+      </c>
+      <c r="I7" s="8" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>63</v>
+        <v>79</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
-      <c r="F8" s="5">
+      <c r="C8" s="5">
         <v>1</v>
       </c>
       <c r="G8" s="5">
         <f>ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H8" t="s">
-        <v>23</v>
+        <v>80</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="J8" s="8" t="s">
-        <v>27</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
       <c r="B9" s="5">
         <v>1</v>
       </c>
       <c r="D9" s="5">
-        <v>1</v>
-      </c>
-      <c r="E9" s="5">
         <v>1</v>
       </c>
       <c r="G9" s="5">
         <f>ROUND(C9*WoodVP+D9*SteelVP+E9*StoneVP+F9*GoldVP,0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>61</v>
+        <v>114</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J9" s="6" t="s">
-        <v>29</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>59</v>
       </c>
       <c r="B10" s="5">
         <v>1</v>
       </c>
-      <c r="C10" s="5">
-        <v>2</v>
+      <c r="F10" s="5">
+        <v>1</v>
       </c>
       <c r="G10" s="5">
         <f>ROUND(C10*WoodVP+D10*SteelVP+E10*StoneVP+F10*GoldVP,0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H10" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="J10" s="8" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="B11" s="5">
         <v>1</v>
       </c>
-      <c r="C11" s="5">
-        <v>1</v>
-      </c>
-      <c r="D11" s="5">
+      <c r="E11" s="5">
         <v>1</v>
       </c>
       <c r="G11" s="5">
         <f>ROUND(C11*WoodVP+D11*SteelVP+E11*StoneVP+F11*GoldVP,0)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H11" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>34</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>0</v>
       </c>
       <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
         <v>1</v>
       </c>
       <c r="D12" s="5">
@@ -970,44 +1020,53 @@
       </c>
       <c r="G12" s="5">
         <f>ROUND(C12*WoodVP+D12*SteelVP+E12*StoneVP+F12*GoldVP,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H12" t="s">
-        <v>37</v>
+        <v>9</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>42</v>
+        <v>25</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="B13" s="5">
         <v>1</v>
       </c>
       <c r="C13" s="5">
+        <v>1</v>
+      </c>
+      <c r="E13" s="5">
         <v>1</v>
       </c>
       <c r="G13" s="5">
         <f>ROUND(C13*WoodVP+D13*SteelVP+E13*StoneVP+F13*GoldVP,0)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H13" t="s">
-        <v>85</v>
-      </c>
-      <c r="I13" s="8" t="s">
-        <v>50</v>
+        <v>20</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>62</v>
+        <v>27</v>
       </c>
       <c r="B14" s="5">
         <v>1</v>
       </c>
-      <c r="C14" s="5">
+      <c r="D14" s="5">
         <v>1</v>
       </c>
       <c r="E14" s="5">
@@ -1018,111 +1077,138 @@
         <v>3</v>
       </c>
       <c r="H14" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="I14" s="8" t="s">
-        <v>26</v>
+        <v>47</v>
+      </c>
+      <c r="J14" s="6" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>54</v>
+        <v>29</v>
       </c>
       <c r="B15" s="5">
         <v>1</v>
       </c>
-      <c r="E15" s="5">
-        <v>1</v>
+      <c r="C15" s="5">
+        <v>2</v>
       </c>
       <c r="G15" s="5">
         <f>ROUND(C15*WoodVP+D15*SteelVP+E15*StoneVP+F15*GoldVP,0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H15" t="s">
-        <v>55</v>
+        <v>30</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>72</v>
+        <v>94</v>
       </c>
       <c r="B16" s="5">
         <v>1</v>
       </c>
+      <c r="D16" s="5">
+        <v>1</v>
+      </c>
       <c r="E16" s="5">
-        <v>2</v>
-      </c>
-      <c r="F16" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16" s="5">
         <f>ROUND(C16*WoodVP+D16*SteelVP+E16*StoneVP+F16*GoldVP,0)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="B17" s="5">
         <v>1</v>
       </c>
-      <c r="E17" s="5">
-        <v>3</v>
+      <c r="C17" s="5">
+        <v>1</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1</v>
       </c>
       <c r="G17" s="5">
         <f>ROUND(C17*WoodVP+D17*SteelVP+E17*StoneVP+F17*GoldVP,0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H17" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="J17" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>74</v>
+        <v>96</v>
       </c>
       <c r="B18" s="5">
         <v>1</v>
       </c>
       <c r="D18" s="5">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
       </c>
       <c r="G18" s="5">
         <f>ROUND(C18*WoodVP+D18*SteelVP+E18*StoneVP+F18*GoldVP,0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H18" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="I18" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B19" s="5">
         <v>1</v>
       </c>
-      <c r="C19" s="5">
-        <v>3</v>
+      <c r="E19" s="5">
+        <v>1</v>
+      </c>
+      <c r="F19" s="5">
+        <v>1</v>
       </c>
       <c r="G19" s="5">
         <f>ROUND(C19*WoodVP+D19*SteelVP+E19*StoneVP+F19*GoldVP,0)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H19" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>86</v>
+        <v>58</v>
       </c>
       <c r="B20" s="5">
         <v>1</v>
@@ -1130,240 +1216,441 @@
       <c r="C20" s="5">
         <v>1</v>
       </c>
-      <c r="D20" s="5">
-        <v>1</v>
-      </c>
       <c r="E20" s="5">
-        <v>1</v>
-      </c>
-      <c r="F20" s="5">
         <v>1</v>
       </c>
       <c r="G20" s="5">
         <f>ROUND(C20*WoodVP+D20*SteelVP+E20*StoneVP+F20*GoldVP,0)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H20" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B21" s="5">
         <v>1</v>
       </c>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
-      <c r="E21" s="5">
-        <v>2</v>
-      </c>
       <c r="F21" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G21" s="5">
         <f>ROUND(C21*WoodVP+D21*SteelVP+E21*StoneVP+F21*GoldVP,0)</f>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H21" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="B22" s="5">
         <v>1</v>
       </c>
       <c r="C22" s="5">
-        <v>2</v>
-      </c>
-      <c r="D22" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G22" s="5">
         <f>ROUND(C22*WoodVP+D22*SteelVP+E22*StoneVP+F22*GoldVP,0)</f>
         <v>5</v>
       </c>
       <c r="H22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>78</v>
+        <v>102</v>
       </c>
       <c r="B23" s="5">
         <v>1</v>
-      </c>
-      <c r="C23" s="5">
-        <v>2</v>
       </c>
       <c r="D23" s="5">
         <v>2</v>
       </c>
       <c r="G23" s="5">
         <f>ROUND(C23*WoodVP+D23*SteelVP+E23*StoneVP+F23*GoldVP,0)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H23" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
       <c r="B24" s="5">
         <v>1</v>
       </c>
       <c r="D24" s="5">
-        <v>2</v>
-      </c>
-      <c r="E24" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G24" s="5">
         <f>ROUND(C24*WoodVP+D24*SteelVP+E24*StoneVP+F24*GoldVP,0)</f>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="H24" t="s">
-        <v>60</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="B25" s="5">
         <v>1</v>
       </c>
       <c r="C25" s="5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G25" s="5">
         <f>ROUND(C25*WoodVP+D25*SteelVP+E25*StoneVP+F25*GoldVP,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H25" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>108</v>
       </c>
       <c r="B26" s="5">
         <v>1</v>
       </c>
-      <c r="F26" s="5">
-        <v>3</v>
+      <c r="C26" s="5">
+        <v>1</v>
+      </c>
+      <c r="D26" s="5">
+        <v>1</v>
+      </c>
+      <c r="E26" s="5">
+        <v>1</v>
       </c>
       <c r="G26" s="5">
         <f>ROUND(C26*WoodVP+D26*SteelVP+E26*StoneVP+F26*GoldVP,0)</f>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H26" t="s">
-        <v>64</v>
+        <v>109</v>
       </c>
       <c r="I26" s="8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B27" s="5">
-        <v>1</v>
-      </c>
-      <c r="D27" s="5">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="E27" s="5">
+        <v>3</v>
       </c>
       <c r="G27" s="5">
         <f>ROUND(C27*WoodVP+D27*SteelVP+E27*StoneVP+F27*GoldVP,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H27" t="s">
-        <v>41</v>
-      </c>
-      <c r="I27" s="8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>83</v>
       </c>
       <c r="B28" s="5">
         <v>1</v>
       </c>
-      <c r="F28" s="5">
-        <v>6</v>
+      <c r="C28" s="5">
+        <v>2</v>
+      </c>
+      <c r="D28" s="5">
+        <v>2</v>
       </c>
       <c r="G28" s="5">
         <f>ROUND(C28*WoodVP+D28*SteelVP+E28*StoneVP+F28*GoldVP,0)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="H28" t="s">
-        <v>40</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="B29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="5">
-        <v>6</v>
+      <c r="C29" s="5">
+        <v>2</v>
+      </c>
+      <c r="D29" s="5">
+        <v>2</v>
       </c>
       <c r="G29" s="5">
         <f>ROUND(C29*WoodVP+D29*SteelVP+E29*StoneVP+F29*GoldVP,0)</f>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="H29" t="s">
-        <v>45</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="B30" s="5">
         <v>1</v>
       </c>
       <c r="C30" s="5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G30" s="5">
         <f>ROUND(C30*WoodVP+D30*SteelVP+E30*StoneVP+F30*GoldVP,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H30" t="s">
+        <v>64</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="5">
+        <v>1</v>
+      </c>
+      <c r="F31" s="5">
+        <v>3</v>
+      </c>
+      <c r="G31" s="5">
+        <f>ROUND(C31*WoodVP+D31*SteelVP+E31*StoneVP+F31*GoldVP,0)</f>
+        <v>5</v>
+      </c>
+      <c r="H31" t="s">
+        <v>60</v>
+      </c>
+      <c r="I31" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>105</v>
+      </c>
+      <c r="B32" s="5">
+        <v>1</v>
+      </c>
+      <c r="D32" s="5">
+        <v>2</v>
+      </c>
+      <c r="E32" s="5">
+        <v>2</v>
+      </c>
+      <c r="G32" s="5">
+        <f>ROUND(C32*WoodVP+D32*SteelVP+E32*StoneVP+F32*GoldVP,0)</f>
+        <v>6</v>
+      </c>
+      <c r="H32" t="s">
+        <v>106</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>68</v>
+      </c>
+      <c r="B33" s="5">
+        <v>1</v>
+      </c>
+      <c r="E33" s="5">
+        <v>2</v>
+      </c>
+      <c r="F33" s="5">
+        <v>2</v>
+      </c>
+      <c r="G33" s="5">
+        <f>ROUND(C33*WoodVP+D33*SteelVP+E33*StoneVP+F33*GoldVP,0)</f>
+        <v>6</v>
+      </c>
+      <c r="H33" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>111</v>
+      </c>
+      <c r="B34" s="5">
+        <v>1</v>
+      </c>
+      <c r="D34" s="5">
+        <v>3</v>
+      </c>
+      <c r="F34" s="5">
+        <v>1</v>
+      </c>
+      <c r="G34" s="5">
+        <f>ROUND(C34*WoodVP+D34*SteelVP+E34*StoneVP+F34*GoldVP,0)</f>
+        <v>6</v>
+      </c>
+      <c r="H34" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>81</v>
+      </c>
+      <c r="B35" s="5">
+        <v>1</v>
+      </c>
+      <c r="D35" s="5">
+        <v>1</v>
+      </c>
+      <c r="E35" s="5">
+        <v>2</v>
+      </c>
+      <c r="F35" s="5">
+        <v>1</v>
+      </c>
+      <c r="G35" s="5">
+        <f>ROUND(C35*WoodVP+D35*SteelVP+E35*StoneVP+F35*GoldVP,0)</f>
+        <v>6</v>
+      </c>
+      <c r="H35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="5">
+        <v>1</v>
+      </c>
+      <c r="D36" s="5">
+        <v>2</v>
+      </c>
+      <c r="E36" s="5">
+        <v>2</v>
+      </c>
+      <c r="G36" s="5">
+        <f>ROUND(C36*WoodVP+D36*SteelVP+E36*StoneVP+F36*GoldVP,0)</f>
+        <v>6</v>
+      </c>
+      <c r="H36" t="s">
+        <v>56</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>41</v>
+      </c>
+      <c r="B37" s="5">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5">
+        <v>6</v>
+      </c>
+      <c r="G37" s="5">
+        <f>ROUND(C37*WoodVP+D37*SteelVP+E37*StoneVP+F37*GoldVP,0)</f>
         <v>9</v>
       </c>
-      <c r="H30" t="s">
-        <v>47</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>48</v>
+      <c r="H37" t="s">
+        <v>43</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>44</v>
+      </c>
+      <c r="B38" s="5">
+        <v>1</v>
+      </c>
+      <c r="C38" s="5">
+        <v>7</v>
+      </c>
+      <c r="G38" s="5">
+        <f>ROUND(C38*WoodVP+D38*SteelVP+E38*StoneVP+F38*GoldVP,0)</f>
+        <v>9</v>
+      </c>
+      <c r="H38" t="s">
+        <v>45</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="5">
+        <v>1</v>
+      </c>
+      <c r="D39" s="5">
+        <v>7</v>
+      </c>
+      <c r="G39" s="5">
+        <f>ROUND(C39*WoodVP+D39*SteelVP+E39*StoneVP+F39*GoldVP,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H39" t="s">
+        <v>39</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="5">
+        <v>1</v>
+      </c>
+      <c r="F40" s="5">
+        <v>6</v>
+      </c>
+      <c r="G40" s="5">
+        <f>ROUND(C40*WoodVP+D40*SteelVP+E40*StoneVP+F40*GoldVP,0)</f>
+        <v>10</v>
+      </c>
+      <c r="H40" t="s">
+        <v>38</v>
+      </c>
+      <c r="I40" s="8" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:J31">
+    <sortCondition ref="G2:G31"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1383,10 +1670,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1431,76 +1718,76 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="e">
-        <f>COUNTIF(Deck!#REF!,Economy!A2) + COUNTIF(Deck!#REF!,Economy!A2)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C2" s="3" t="e">
-        <f>SUMIF(Deck!#REF!,Economy!A2,Deck!#REF!) + SUMIF(Deck!#REF!,Economy!A2,Deck!#REF!)</f>
-        <v>#REF!</v>
+      <c r="B2" s="3">
+        <f>COUNTA(Deck!C2:C104)</f>
+        <v>15</v>
+      </c>
+      <c r="C2" s="3">
+        <f>SUM(Deck!C2:C103)</f>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="e">
-        <f>COUNTIF(Deck!#REF!,Economy!A3) + COUNTIF(Deck!#REF!,Economy!A3)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C3" s="3" t="e">
-        <f>SUMIF(Deck!#REF!,Economy!A3,Deck!#REF!) + SUMIF(Deck!#REF!,Economy!A3,Deck!#REF!)</f>
-        <v>#REF!</v>
+      <c r="B3" s="3">
+        <f>COUNTA(Deck!D2:D104)</f>
+        <v>18</v>
+      </c>
+      <c r="C3" s="3">
+        <f>SUM(Deck!D2:D103)</f>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="e">
-        <f>COUNTIF(Deck!#REF!,Economy!A4) + COUNTIF(Deck!#REF!,Economy!A4)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C4" s="3" t="e">
-        <f>SUMIF(Deck!#REF!,Economy!A4,Deck!#REF!) + SUMIF(Deck!#REF!,Economy!A4,Deck!#REF!)</f>
-        <v>#REF!</v>
+      <c r="B4" s="3">
+        <f>COUNTA(Deck!E2:E104)</f>
+        <v>15</v>
+      </c>
+      <c r="C4" s="3">
+        <f>SUM(Deck!E2:E103)</f>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="e">
-        <f>COUNTIF(Deck!#REF!,Economy!A5) + COUNTIF(Deck!#REF!,Economy!A5)</f>
-        <v>#REF!</v>
-      </c>
-      <c r="C5" s="3" t="e">
-        <f>SUMIF(Deck!#REF!,Economy!A5,Deck!#REF!) + SUMIF(Deck!#REF!,Economy!A5,Deck!#REF!)</f>
-        <v>#REF!</v>
+      <c r="B5" s="3">
+        <f>COUNTA(Deck!F2:F104)</f>
+        <v>9</v>
+      </c>
+      <c r="C5" s="3">
+        <f>SUM(Deck!F2:F104)</f>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Downplaying VP on bonus cards, other small adjustments
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -79,9 +79,6 @@
     <t>wood-pile</t>
   </si>
   <si>
-    <t>Gears</t>
-  </si>
-  <si>
     <t>gears</t>
   </si>
   <si>
@@ -412,13 +409,16 @@
     <t>Total Economy</t>
   </si>
   <si>
-    <t>Upon purchase, you may reorder the cards on one row.</t>
-  </si>
-  <si>
-    <t>At game end, you may scrap two cards (not this one) and gain 2 VP per Wood.</t>
-  </si>
-  <si>
     <t>-1 Stone per turn</t>
+  </si>
+  <si>
+    <t>Rusted Gears</t>
+  </si>
+  <si>
+    <t>At game end, 1 VP per Wood in any cards except this one.</t>
+  </si>
+  <si>
+    <t>Upon purchase, you may reorder the cards on one row or column.</t>
   </si>
 </sst>
 </file>
@@ -797,10 +797,10 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +908,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>129</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
@@ -921,7 +921,7 @@
         <v>0</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J4" t="s">
         <v>14</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B5" s="9">
         <v>6</v>
@@ -944,7 +944,7 @@
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J5" t="s">
         <v>14</v>
@@ -956,7 +956,7 @@
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="9">
         <v>8</v>
@@ -968,19 +968,19 @@
         <v>0</v>
       </c>
       <c r="I6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J6" t="s">
         <v>14</v>
       </c>
       <c r="K6"/>
       <c r="L6" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" s="9">
         <v>6</v>
@@ -993,49 +993,49 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J7" t="s">
         <v>14</v>
       </c>
       <c r="K7"/>
       <c r="L7" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <f>ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
         <v>28</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="E8" s="9">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9">
-        <f t="shared" ref="G8:G41" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
-        <v>6</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>29</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>30</v>
-      </c>
-      <c r="K8" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9" s="9">
         <v>1</v>
@@ -1051,106 +1051,112 @@
         <v>1</v>
       </c>
       <c r="G9" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C9*WoodVP+D9*SteelVP+E9*StoneVP+F9*GoldVP,0) + H9</f>
         <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J9" t="s">
+        <v>29</v>
+      </c>
+      <c r="K9" t="s">
         <v>30</v>
-      </c>
-      <c r="K9" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
+        <f>ROUND(C10*WoodVP+D10*SteelVP+E10*StoneVP+F10*GoldVP,0) + H10</f>
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I10" t="s">
-        <v>35</v>
-      </c>
       <c r="J10" t="s">
+        <v>29</v>
+      </c>
+      <c r="K10" t="s">
         <v>30</v>
-      </c>
-      <c r="K10" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <f>ROUND(C11*WoodVP+D11*SteelVP+E11*StoneVP+F11*GoldVP,0) + H11</f>
+        <v>2</v>
+      </c>
+      <c r="H11" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I11" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="D11" s="9">
-        <v>1</v>
-      </c>
-      <c r="F11" s="9">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>37</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1</v>
+      </c>
+      <c r="F12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9">
+        <f>ROUND(C12*WoodVP+D12*SteelVP+E12*StoneVP+F12*GoldVP,0) + H12</f>
+        <v>2</v>
+      </c>
+      <c r="H12" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="9">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
+        <v>37</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="J12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B13" s="9">
         <v>1</v>
@@ -1160,23 +1166,26 @@
       </c>
       <c r="E13" s="10"/>
       <c r="G13" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(C13*WoodVP+D13*SteelVP+E13*StoneVP+F13*GoldVP,0) + H13</f>
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>-1</v>
       </c>
       <c r="I13" t="s">
+        <v>43</v>
+      </c>
+      <c r="J13" t="s">
         <v>44</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>46</v>
       </c>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="9">
         <v>1</v>
@@ -1186,53 +1195,59 @@
       </c>
       <c r="E14" s="10"/>
       <c r="G14" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(C14*WoodVP+D14*SteelVP+E14*StoneVP+F14*GoldVP,0) + H14</f>
+        <v>2</v>
+      </c>
+      <c r="H14" s="1">
+        <v>-1</v>
       </c>
       <c r="I14" t="s">
+        <v>47</v>
+      </c>
+      <c r="J14" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="J14" t="s">
-        <v>45</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="L14"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>49</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9">
+        <f>ROUND(C15*WoodVP+D15*SteelVP+E15*StoneVP+F15*GoldVP,0) + H15</f>
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I15" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="9">
-        <v>1</v>
-      </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
+        <v>44</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J15" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="6" t="s">
+      <c r="L15" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="9">
         <v>1</v>
@@ -1245,25 +1260,28 @@
       </c>
       <c r="E16" s="10"/>
       <c r="G16" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(C16*WoodVP+D16*SteelVP+E16*StoneVP+F16*GoldVP,0) + H16</f>
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>-1</v>
       </c>
       <c r="I16" t="s">
+        <v>50</v>
+      </c>
+      <c r="J16" t="s">
+        <v>44</v>
+      </c>
+      <c r="K16" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J16" t="s">
-        <v>45</v>
-      </c>
-      <c r="K16" s="6" t="s">
+      <c r="L16" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="9">
         <v>1</v>
@@ -1275,25 +1293,28 @@
         <v>1</v>
       </c>
       <c r="G17" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(C17*WoodVP+D17*SteelVP+E17*StoneVP+F17*GoldVP,0) + H17</f>
+        <v>2</v>
+      </c>
+      <c r="H17" s="1">
+        <v>-1</v>
       </c>
       <c r="I17" t="s">
+        <v>50</v>
+      </c>
+      <c r="J17" t="s">
+        <v>44</v>
+      </c>
+      <c r="K17" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="J17" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" s="6" t="s">
+      <c r="L17" s="6" t="s">
         <v>52</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
@@ -1303,25 +1324,25 @@
         <v>1</v>
       </c>
       <c r="G18" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C18*WoodVP+D18*SteelVP+E18*StoneVP+F18*GoldVP,0) + H18</f>
         <v>2</v>
       </c>
       <c r="I18" t="s">
+        <v>56</v>
+      </c>
+      <c r="J18" t="s">
         <v>57</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="L18" s="6" t="s">
         <v>59</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B19" s="9">
         <v>1</v>
@@ -1331,22 +1352,25 @@
         <v>2</v>
       </c>
       <c r="G19" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(C19*WoodVP+D19*SteelVP+E19*StoneVP+F19*GoldVP,0) + H19</f>
+        <v>2</v>
+      </c>
+      <c r="H19" s="1">
+        <v>-1</v>
       </c>
       <c r="I19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" t="s">
+        <v>57</v>
+      </c>
+      <c r="K19" t="s">
         <v>62</v>
-      </c>
-      <c r="J19" t="s">
-        <v>58</v>
-      </c>
-      <c r="K19" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B20" s="9">
         <v>1</v>
@@ -1356,25 +1380,25 @@
         <v>4</v>
       </c>
       <c r="G20" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C20*WoodVP+D20*SteelVP+E20*StoneVP+F20*GoldVP,0) + H20</f>
         <v>5</v>
       </c>
       <c r="H20" s="1">
         <v>-1</v>
       </c>
       <c r="I20" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="9">
         <v>1</v>
@@ -1384,20 +1408,20 @@
         <v>3</v>
       </c>
       <c r="G21" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C21*WoodVP+D21*SteelVP+E21*StoneVP+F21*GoldVP,0) + H21</f>
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K21"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="9">
         <v>1</v>
@@ -1407,23 +1431,23 @@
         <v>6</v>
       </c>
       <c r="G22" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C22*WoodVP+D22*SteelVP+E22*StoneVP+F22*GoldVP,0) + H22</f>
         <v>13</v>
       </c>
       <c r="H22" s="1">
         <v>3</v>
       </c>
       <c r="I22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="J22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
@@ -1433,23 +1457,26 @@
       </c>
       <c r="E23" s="10"/>
       <c r="G23" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(C23*WoodVP+D23*SteelVP+E23*StoneVP+F23*GoldVP,0) + H23</f>
+        <v>2</v>
+      </c>
+      <c r="H23" s="1">
+        <v>-1</v>
       </c>
       <c r="I23" t="s">
+        <v>70</v>
+      </c>
+      <c r="J23" t="s">
         <v>71</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" s="6" t="s">
         <v>72</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>73</v>
       </c>
       <c r="L23"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
@@ -1462,22 +1489,22 @@
       </c>
       <c r="E24" s="10"/>
       <c r="G24" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C24*WoodVP+D24*SteelVP+E24*StoneVP+F24*GoldVP,0) + H24</f>
         <v>5</v>
       </c>
       <c r="I24" t="s">
+        <v>74</v>
+      </c>
+      <c r="J24" t="s">
+        <v>71</v>
+      </c>
+      <c r="K24" s="6" t="s">
         <v>75</v>
-      </c>
-      <c r="J24" t="s">
-        <v>72</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>77</v>
+        <v>120</v>
       </c>
       <c r="B25" s="9">
         <v>1</v>
@@ -1485,434 +1512,437 @@
       <c r="C25" s="9">
         <v>2</v>
       </c>
-      <c r="E25" s="10"/>
+      <c r="D25" s="9">
+        <v>2</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9">
+        <v>1</v>
+      </c>
       <c r="G25" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>78</v>
+        <f>ROUND(C25*WoodVP+D25*SteelVP+E25*StoneVP+F25*GoldVP,0) + H25</f>
+        <v>9</v>
+      </c>
+      <c r="I25" t="s">
+        <v>121</v>
       </c>
       <c r="J25" t="s">
-        <v>79</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L25"/>
+        <v>122</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
       </c>
-      <c r="E26" s="9">
-        <v>2</v>
-      </c>
+      <c r="C26" s="9">
+        <v>2</v>
+      </c>
+      <c r="E26" s="10"/>
       <c r="G26" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C26*WoodVP+D26*SteelVP+E26*StoneVP+F26*GoldVP,0) + H26</f>
         <v>3</v>
       </c>
-      <c r="I26" t="s">
-        <v>82</v>
+      <c r="I26" s="7" t="s">
+        <v>77</v>
       </c>
       <c r="J26" t="s">
+        <v>78</v>
+      </c>
+      <c r="K26" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="K26" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>84</v>
-      </c>
+      <c r="L26"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B27" s="9">
-        <v>2</v>
-      </c>
-      <c r="D27" s="9">
-        <v>2</v>
-      </c>
-      <c r="E27" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>2</v>
+      </c>
       <c r="G27" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C27*WoodVP+D27*SteelVP+E27*StoneVP+F27*GoldVP,0) + H27</f>
         <v>3</v>
       </c>
       <c r="I27" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="J27" t="s">
-        <v>79</v>
-      </c>
-      <c r="K27"/>
+        <v>78</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B28" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D28" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E28" s="10"/>
       <c r="G28" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>ROUND(C28*WoodVP+D28*SteelVP+E28*StoneVP+F28*GoldVP,0) + H28</f>
+        <v>3</v>
       </c>
       <c r="I28" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J28" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K28"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B29" s="9">
         <v>1</v>
       </c>
       <c r="D29" s="9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E29" s="10"/>
       <c r="G29" s="9">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f>ROUND(C29*WoodVP+D29*SteelVP+E29*StoneVP+F29*GoldVP,0) + H29</f>
+        <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="J29" t="s">
-        <v>79</v>
-      </c>
-      <c r="K29" s="6" t="s">
-        <v>91</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="K29"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B30" s="9">
         <v>1</v>
       </c>
       <c r="D30" s="9">
-        <v>3</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E30" s="10"/>
       <c r="G30" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>ROUND(C30*WoodVP+D30*SteelVP+E30*StoneVP+F30*GoldVP,0) + H30</f>
+        <v>10</v>
       </c>
       <c r="I30" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="J30" t="s">
-        <v>94</v>
-      </c>
-      <c r="K30" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="L30"/>
+        <v>78</v>
+      </c>
+      <c r="K30" s="6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B31" s="9">
         <v>1</v>
       </c>
       <c r="C31" s="9">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9">
+        <v>1</v>
+      </c>
+      <c r="G31" s="9">
+        <f>ROUND(C31*WoodVP+D31*SteelVP+E31*StoneVP+F31*GoldVP,0) + H31</f>
         <v>3</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="G31" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
       <c r="I31" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="J31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K31" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="L31" s="6" t="s">
-        <v>97</v>
+        <v>128</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B32" s="9">
         <v>1</v>
       </c>
-      <c r="C32" s="9">
-        <v>1</v>
-      </c>
-      <c r="E32" s="9">
-        <v>1</v>
+      <c r="D32" s="9">
+        <v>3</v>
       </c>
       <c r="G32" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
+        <f>ROUND(C32*WoodVP+D32*SteelVP+E32*StoneVP+F32*GoldVP,0) + H32</f>
+        <v>4</v>
       </c>
       <c r="I32" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="J32" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="K32" s="11" t="s">
-        <v>131</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="L32"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B33" s="9">
-        <v>2</v>
-      </c>
-      <c r="E33" s="9">
+        <v>1</v>
+      </c>
+      <c r="C33" s="9">
         <v>3</v>
       </c>
+      <c r="E33" s="10"/>
       <c r="G33" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>ROUND(C33*WoodVP+D33*SteelVP+E33*StoneVP+F33*GoldVP,0) + H33</f>
+        <v>4</v>
       </c>
       <c r="I33" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="J33" t="s">
-        <v>94</v>
-      </c>
-      <c r="K33"/>
+        <v>93</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="L33" s="6" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B34" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G34" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>ROUND(C34*WoodVP+D34*SteelVP+E34*StoneVP+F34*GoldVP,0) + H34</f>
+        <v>5</v>
       </c>
       <c r="I34" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="J34" t="s">
-        <v>94</v>
-      </c>
-      <c r="K34" s="6" t="s">
-        <v>104</v>
-      </c>
+        <v>93</v>
+      </c>
+      <c r="K34"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B35" s="9">
         <v>1</v>
       </c>
-      <c r="C35" s="9">
-        <v>2</v>
-      </c>
-      <c r="D35" s="9">
-        <v>1</v>
-      </c>
-      <c r="E35" s="10"/>
+      <c r="E35" s="9">
+        <v>6</v>
+      </c>
       <c r="G35" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>ROUND(C35*WoodVP+D35*SteelVP+E35*StoneVP+F35*GoldVP,0) + H35</f>
+        <v>9</v>
       </c>
       <c r="I35" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="J35" t="s">
-        <v>107</v>
-      </c>
-      <c r="K35" t="s">
-        <v>129</v>
+        <v>93</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
       </c>
       <c r="C36" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D36" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E36" s="10"/>
       <c r="G36" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C36*WoodVP+D36*SteelVP+E36*StoneVP+F36*GoldVP,0) + H36</f>
         <v>4</v>
       </c>
       <c r="I36" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J36" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="K36" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B37" s="9">
         <v>1</v>
       </c>
-      <c r="E37" s="9">
-        <v>1</v>
-      </c>
+      <c r="C37" s="9">
+        <v>1</v>
+      </c>
+      <c r="D37" s="9">
+        <v>2</v>
+      </c>
+      <c r="E37" s="10"/>
       <c r="G37" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f>ROUND(C37*WoodVP+D37*SteelVP+E37*StoneVP+F37*GoldVP,0) + H37</f>
+        <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J37" t="s">
-        <v>112</v>
-      </c>
-      <c r="K37" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="L37" s="6" t="s">
-        <v>114</v>
+        <v>106</v>
+      </c>
+      <c r="K37" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B38" s="9">
         <v>1</v>
       </c>
-      <c r="C38" s="9">
-        <v>3</v>
-      </c>
-      <c r="E38" s="10"/>
+      <c r="E38" s="9">
+        <v>1</v>
+      </c>
       <c r="G38" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f>ROUND(C38*WoodVP+D38*SteelVP+E38*StoneVP+F38*GoldVP,0) + H38</f>
+        <v>2</v>
       </c>
       <c r="I38" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J38" t="s">
+        <v>111</v>
+      </c>
+      <c r="K38" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="K38"/>
+      <c r="L38" s="6" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B39" s="9">
         <v>1</v>
       </c>
       <c r="C39" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E39" s="10"/>
       <c r="G39" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f>ROUND(C39*WoodVP+D39*SteelVP+E39*StoneVP+F39*GoldVP,0) + H39</f>
+        <v>4</v>
       </c>
       <c r="I39" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="J39" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="K39"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B40" s="9">
         <v>1</v>
       </c>
       <c r="C40" s="9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E40" s="10"/>
       <c r="G40" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f>ROUND(C40*WoodVP+D40*SteelVP+E40*StoneVP+F40*GoldVP,0) + H40</f>
+        <v>5</v>
       </c>
       <c r="I40" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J40" t="s">
-        <v>112</v>
-      </c>
-      <c r="K40" s="6" t="s">
-        <v>130</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="K40"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B41" s="9">
         <v>1</v>
       </c>
       <c r="C41" s="9">
-        <v>2</v>
-      </c>
-      <c r="D41" s="9">
-        <v>2</v>
-      </c>
-      <c r="E41" s="9">
-        <v>1</v>
-      </c>
-      <c r="F41" s="9">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E41" s="10"/>
       <c r="G41" s="9">
-        <f t="shared" si="0"/>
+        <f>ROUND(C41*WoodVP+D41*SteelVP+E41*StoneVP+F41*GoldVP,0) + H41</f>
         <v>9</v>
       </c>
       <c r="I41" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J41" t="s">
-        <v>123</v>
-      </c>
-      <c r="K41" s="2" t="s">
-        <v>124</v>
+        <v>111</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:L41">
+    <sortCondition ref="J2:J41"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
@@ -1935,10 +1965,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>125</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1997,13 +2027,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>127</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Gold bars are now a wildcard resource
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="134">
   <si>
     <t>Name</t>
   </si>
@@ -103,9 +103,6 @@
     <t>gold-bar</t>
   </si>
   <si>
-    <t>The power of purchase.</t>
-  </si>
-  <si>
     <t>Ancient Throne</t>
   </si>
   <si>
@@ -419,6 +416,15 @@
   </si>
   <si>
     <t>Upon purchase, you may reorder the cards on one row or column.</t>
+  </si>
+  <si>
+    <t>May also be used for any 1 Resource.</t>
+  </si>
+  <si>
+    <t>Lest we forget, steampunk is a fantasy.</t>
+  </si>
+  <si>
+    <t>Behold the power of purchase.</t>
   </si>
 </sst>
 </file>
@@ -797,10 +803,10 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -908,7 +914,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
@@ -927,7 +933,9 @@
         <v>14</v>
       </c>
       <c r="K4"/>
-      <c r="L4"/>
+      <c r="L4" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -998,44 +1006,46 @@
       <c r="J7" t="s">
         <v>14</v>
       </c>
-      <c r="K7"/>
+      <c r="K7" t="s">
+        <v>131</v>
+      </c>
       <c r="L7" s="6" t="s">
-        <v>26</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" ref="G8:G41" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="E8" s="9">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9">
-        <f>ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
-        <v>6</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>28</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>29</v>
-      </c>
-      <c r="K8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B9" s="9">
         <v>1</v>
@@ -1051,52 +1061,52 @@
         <v>1</v>
       </c>
       <c r="G9" s="9">
-        <f>ROUND(C9*WoodVP+D9*SteelVP+E9*StoneVP+F9*GoldVP,0) + H9</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J9" t="s">
+        <v>28</v>
+      </c>
+      <c r="K9" t="s">
         <v>29</v>
-      </c>
-      <c r="K9" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9">
-        <f>ROUND(C10*WoodVP+D10*SteelVP+E10*StoneVP+F10*GoldVP,0) + H10</f>
-        <v>6</v>
-      </c>
-      <c r="I10" t="s">
-        <v>34</v>
-      </c>
       <c r="J10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" t="s">
         <v>29</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11" s="9">
         <v>1</v>
@@ -1108,25 +1118,25 @@
         <v>1</v>
       </c>
       <c r="G11" s="9">
-        <f>ROUND(C11*WoodVP+D11*SteelVP+E11*StoneVP+F11*GoldVP,0) + H11</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H11" s="1">
         <v>-1</v>
       </c>
       <c r="I11" t="s">
+        <v>35</v>
+      </c>
+      <c r="J11" t="s">
         <v>36</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B12" s="9">
         <v>1</v>
@@ -1138,25 +1148,25 @@
         <v>1</v>
       </c>
       <c r="G12" s="9">
-        <f>ROUND(C12*WoodVP+D12*SteelVP+E12*StoneVP+F12*GoldVP,0) + H12</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H12" s="1">
         <v>-1</v>
       </c>
       <c r="I12" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="J12" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" s="9">
         <v>1</v>
@@ -1166,26 +1176,26 @@
       </c>
       <c r="E13" s="10"/>
       <c r="G13" s="9">
-        <f>ROUND(C13*WoodVP+D13*SteelVP+E13*StoneVP+F13*GoldVP,0) + H13</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H13" s="1">
         <v>-1</v>
       </c>
       <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" t="s">
         <v>43</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" s="6" t="s">
         <v>44</v>
-      </c>
-      <c r="K13" s="6" t="s">
-        <v>45</v>
       </c>
       <c r="L13"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="9">
         <v>1</v>
@@ -1195,26 +1205,26 @@
       </c>
       <c r="E14" s="10"/>
       <c r="G14" s="9">
-        <f>ROUND(C14*WoodVP+D14*SteelVP+E14*StoneVP+F14*GoldVP,0) + H14</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H14" s="1">
         <v>-1</v>
       </c>
       <c r="I14" t="s">
+        <v>46</v>
+      </c>
+      <c r="J14" t="s">
+        <v>43</v>
+      </c>
+      <c r="K14" s="6" t="s">
         <v>47</v>
-      </c>
-      <c r="J14" t="s">
-        <v>44</v>
-      </c>
-      <c r="K14" s="6" t="s">
-        <v>48</v>
       </c>
       <c r="L14"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="9">
         <v>1</v>
@@ -1226,28 +1236,28 @@
         <v>1</v>
       </c>
       <c r="G15" s="9">
-        <f>ROUND(C15*WoodVP+D15*SteelVP+E15*StoneVP+F15*GoldVP,0) + H15</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H15" s="1">
         <v>-1</v>
       </c>
       <c r="I15" t="s">
+        <v>49</v>
+      </c>
+      <c r="J15" t="s">
+        <v>43</v>
+      </c>
+      <c r="K15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J15" t="s">
-        <v>44</v>
-      </c>
-      <c r="K15" s="6" t="s">
+      <c r="L15" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="9">
         <v>1</v>
@@ -1260,28 +1270,28 @@
       </c>
       <c r="E16" s="10"/>
       <c r="G16" s="9">
-        <f>ROUND(C16*WoodVP+D16*SteelVP+E16*StoneVP+F16*GoldVP,0) + H16</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H16" s="1">
         <v>-1</v>
       </c>
       <c r="I16" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" t="s">
+        <v>43</v>
+      </c>
+      <c r="K16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J16" t="s">
-        <v>44</v>
-      </c>
-      <c r="K16" s="6" t="s">
+      <c r="L16" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B17" s="9">
         <v>1</v>
@@ -1293,28 +1303,28 @@
         <v>1</v>
       </c>
       <c r="G17" s="9">
-        <f>ROUND(C17*WoodVP+D17*SteelVP+E17*StoneVP+F17*GoldVP,0) + H17</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H17" s="1">
         <v>-1</v>
       </c>
       <c r="I17" t="s">
+        <v>49</v>
+      </c>
+      <c r="J17" t="s">
+        <v>43</v>
+      </c>
+      <c r="K17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="J17" t="s">
-        <v>44</v>
-      </c>
-      <c r="K17" s="6" t="s">
+      <c r="L17" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
@@ -1324,25 +1334,25 @@
         <v>1</v>
       </c>
       <c r="G18" s="9">
-        <f>ROUND(C18*WoodVP+D18*SteelVP+E18*StoneVP+F18*GoldVP,0) + H18</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="I18" t="s">
+        <v>55</v>
+      </c>
+      <c r="J18" t="s">
         <v>56</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="L18" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="9">
         <v>1</v>
@@ -1352,25 +1362,25 @@
         <v>2</v>
       </c>
       <c r="G19" s="9">
-        <f>ROUND(C19*WoodVP+D19*SteelVP+E19*StoneVP+F19*GoldVP,0) + H19</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="H19" s="1">
         <v>-1</v>
       </c>
       <c r="I19" t="s">
+        <v>60</v>
+      </c>
+      <c r="J19" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" t="s">
         <v>61</v>
-      </c>
-      <c r="J19" t="s">
-        <v>57</v>
-      </c>
-      <c r="K19" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="9">
         <v>1</v>
@@ -1380,25 +1390,25 @@
         <v>4</v>
       </c>
       <c r="G20" s="9">
-        <f>ROUND(C20*WoodVP+D20*SteelVP+E20*StoneVP+F20*GoldVP,0) + H20</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>6</v>
       </c>
       <c r="H20" s="1">
         <v>-1</v>
       </c>
       <c r="I20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K20" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B21" s="9">
         <v>1</v>
@@ -1408,20 +1418,20 @@
         <v>3</v>
       </c>
       <c r="G21" s="9">
-        <f>ROUND(C21*WoodVP+D21*SteelVP+E21*StoneVP+F21*GoldVP,0) + H21</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="J21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K21"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B22" s="9">
         <v>1</v>
@@ -1431,23 +1441,23 @@
         <v>6</v>
       </c>
       <c r="G22" s="9">
-        <f>ROUND(C22*WoodVP+D22*SteelVP+E22*StoneVP+F22*GoldVP,0) + H22</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="H22" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
@@ -1457,26 +1467,26 @@
       </c>
       <c r="E23" s="10"/>
       <c r="G23" s="9">
-        <f>ROUND(C23*WoodVP+D23*SteelVP+E23*StoneVP+F23*GoldVP,0) + H23</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="H23" s="1">
         <v>-1</v>
       </c>
       <c r="I23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J23" t="s">
         <v>70</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="L23"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
@@ -1489,55 +1499,55 @@
       </c>
       <c r="E24" s="10"/>
       <c r="G24" s="9">
-        <f>ROUND(C24*WoodVP+D24*SteelVP+E24*StoneVP+F24*GoldVP,0) + H24</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I24" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" t="s">
+        <v>70</v>
+      </c>
+      <c r="K24" s="6" t="s">
         <v>74</v>
-      </c>
-      <c r="J24" t="s">
-        <v>71</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>119</v>
+      </c>
+      <c r="B25" s="9">
+        <v>1</v>
+      </c>
+      <c r="C25" s="9">
+        <v>2</v>
+      </c>
+      <c r="D25" s="9">
+        <v>2</v>
+      </c>
+      <c r="E25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9">
+        <v>1</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I25" t="s">
         <v>120</v>
       </c>
-      <c r="B25" s="9">
-        <v>1</v>
-      </c>
-      <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="D25" s="9">
-        <v>2</v>
-      </c>
-      <c r="E25" s="9">
-        <v>1</v>
-      </c>
-      <c r="F25" s="9">
-        <v>1</v>
-      </c>
-      <c r="G25" s="9">
-        <f>ROUND(C25*WoodVP+D25*SteelVP+E25*StoneVP+F25*GoldVP,0) + H25</f>
-        <v>9</v>
-      </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>121</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
@@ -1547,50 +1557,50 @@
       </c>
       <c r="E26" s="10"/>
       <c r="G26" s="9">
-        <f>ROUND(C26*WoodVP+D26*SteelVP+E26*StoneVP+F26*GoldVP,0) + H26</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I26" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="J26" t="s">
         <v>77</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="L26"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>2</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="9">
-        <v>1</v>
-      </c>
-      <c r="E27" s="9">
-        <v>2</v>
-      </c>
-      <c r="G27" s="9">
-        <f>ROUND(C27*WoodVP+D27*SteelVP+E27*StoneVP+F27*GoldVP,0) + H27</f>
-        <v>3</v>
-      </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
+        <v>77</v>
+      </c>
+      <c r="K27" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="J27" t="s">
-        <v>78</v>
-      </c>
-      <c r="K27" s="6" t="s">
+      <c r="L27" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B28" s="9">
         <v>2</v>
@@ -1600,20 +1610,20 @@
       </c>
       <c r="E28" s="10"/>
       <c r="G28" s="9">
-        <f>ROUND(C28*WoodVP+D28*SteelVP+E28*StoneVP+F28*GoldVP,0) + H28</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J28" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K28"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B29" s="9">
         <v>1</v>
@@ -1623,20 +1633,20 @@
       </c>
       <c r="E29" s="10"/>
       <c r="G29" s="9">
-        <f>ROUND(C29*WoodVP+D29*SteelVP+E29*StoneVP+F29*GoldVP,0) + H29</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J29" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="K29"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B30" s="9">
         <v>1</v>
@@ -1646,49 +1656,49 @@
       </c>
       <c r="E30" s="10"/>
       <c r="G30" s="9">
-        <f>ROUND(C30*WoodVP+D30*SteelVP+E30*StoneVP+F30*GoldVP,0) + H30</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="I30" t="s">
+        <v>88</v>
+      </c>
+      <c r="J30" t="s">
+        <v>77</v>
+      </c>
+      <c r="K30" s="6" t="s">
         <v>89</v>
-      </c>
-      <c r="J30" t="s">
-        <v>78</v>
-      </c>
-      <c r="K30" s="6" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>96</v>
+      </c>
+      <c r="B31" s="9">
+        <v>1</v>
+      </c>
+      <c r="C31" s="9">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9">
+        <v>1</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I31" t="s">
         <v>97</v>
       </c>
-      <c r="B31" s="9">
-        <v>1</v>
-      </c>
-      <c r="C31" s="9">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9">
-        <v>1</v>
-      </c>
-      <c r="G31" s="9">
-        <f>ROUND(C31*WoodVP+D31*SteelVP+E31*StoneVP+F31*GoldVP,0) + H31</f>
-        <v>3</v>
-      </c>
-      <c r="I31" t="s">
-        <v>98</v>
-      </c>
       <c r="J31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K31" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B32" s="9">
         <v>1</v>
@@ -1697,23 +1707,23 @@
         <v>3</v>
       </c>
       <c r="G32" s="9">
-        <f>ROUND(C32*WoodVP+D32*SteelVP+E32*StoneVP+F32*GoldVP,0) + H32</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I32" t="s">
+        <v>91</v>
+      </c>
+      <c r="J32" t="s">
         <v>92</v>
       </c>
-      <c r="J32" t="s">
-        <v>93</v>
-      </c>
       <c r="K32" s="11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L32"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
@@ -1723,25 +1733,25 @@
       </c>
       <c r="E33" s="10"/>
       <c r="G33" s="9">
-        <f>ROUND(C33*WoodVP+D33*SteelVP+E33*StoneVP+F33*GoldVP,0) + H33</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I33" t="s">
+        <v>94</v>
+      </c>
+      <c r="J33" t="s">
+        <v>92</v>
+      </c>
+      <c r="K33" s="11" t="s">
+        <v>127</v>
+      </c>
+      <c r="L33" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="J33" t="s">
-        <v>93</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B34" s="9">
         <v>2</v>
@@ -1750,20 +1760,20 @@
         <v>3</v>
       </c>
       <c r="G34" s="9">
-        <f>ROUND(C34*WoodVP+D34*SteelVP+E34*StoneVP+F34*GoldVP,0) + H34</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I34" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J34" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K34"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B35" s="9">
         <v>1</v>
@@ -1772,22 +1782,22 @@
         <v>6</v>
       </c>
       <c r="G35" s="9">
-        <f>ROUND(C35*WoodVP+D35*SteelVP+E35*StoneVP+F35*GoldVP,0) + H35</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="I35" t="s">
+        <v>101</v>
+      </c>
+      <c r="J35" t="s">
+        <v>92</v>
+      </c>
+      <c r="K35" s="6" t="s">
         <v>102</v>
-      </c>
-      <c r="J35" t="s">
-        <v>93</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
@@ -1800,22 +1810,22 @@
       </c>
       <c r="E36" s="10"/>
       <c r="G36" s="9">
-        <f>ROUND(C36*WoodVP+D36*SteelVP+E36*StoneVP+F36*GoldVP,0) + H36</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I36" t="s">
+        <v>104</v>
+      </c>
+      <c r="J36" t="s">
         <v>105</v>
       </c>
-      <c r="J36" t="s">
-        <v>106</v>
-      </c>
       <c r="K36" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B37" s="9">
         <v>1</v>
@@ -1828,49 +1838,49 @@
       </c>
       <c r="E37" s="10"/>
       <c r="G37" s="9">
-        <f>ROUND(C37*WoodVP+D37*SteelVP+E37*StoneVP+F37*GoldVP,0) + H37</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J37" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="9">
+        <v>1</v>
+      </c>
+      <c r="E38" s="9">
+        <v>1</v>
+      </c>
+      <c r="G38" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I38" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="9">
-        <v>1</v>
-      </c>
-      <c r="E38" s="9">
-        <v>1</v>
-      </c>
-      <c r="G38" s="9">
-        <f>ROUND(C38*WoodVP+D38*SteelVP+E38*StoneVP+F38*GoldVP,0) + H38</f>
-        <v>2</v>
-      </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>110</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="K38" s="6" t="s">
+      <c r="L38" s="6" t="s">
         <v>112</v>
-      </c>
-      <c r="L38" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B39" s="9">
         <v>1</v>
@@ -1880,20 +1890,20 @@
       </c>
       <c r="E39" s="10"/>
       <c r="G39" s="9">
-        <f>ROUND(C39*WoodVP+D39*SteelVP+E39*StoneVP+F39*GoldVP,0) + H39</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I39" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="J39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K39"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B40" s="9">
         <v>1</v>
@@ -1903,20 +1913,20 @@
       </c>
       <c r="E40" s="10"/>
       <c r="G40" s="9">
-        <f>ROUND(C40*WoodVP+D40*SteelVP+E40*StoneVP+F40*GoldVP,0) + H40</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="I40" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="J40" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K40"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B41" s="9">
         <v>1</v>
@@ -1926,17 +1936,17 @@
       </c>
       <c r="E41" s="10"/>
       <c r="G41" s="9">
-        <f>ROUND(C41*WoodVP+D41*SteelVP+E41*StoneVP+F41*GoldVP,0) + H41</f>
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="I41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="J41" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="K41" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -1953,7 +1963,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1965,10 +1975,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2000,7 +2010,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>1.6</v>
+        <v>1.8</v>
       </c>
     </row>
   </sheetData>
@@ -2014,7 +2024,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2027,13 +2037,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Players start with 14 cards, not 15 (removed nails)
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -803,10 +803,10 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -942,7 +942,7 @@
         <v>19</v>
       </c>
       <c r="B5" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>

</xml_diff>

<commit_message>
Balance: add early game cards to prolong initial buildup gameplay
* Added Necklace to make the gold path a little smoother
* Chalice -->Crown, and then Chalice is now its own thing
* Additional Necklace, made a 4vp to be early game too
* Additional Screwdriver
* Chains and anvils are more useful now
* Added Steel Axe to fill out symmetry
* Baseball Bat --> Small Crate
* Added Large Crate
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="140">
   <si>
     <t>Name</t>
   </si>
@@ -220,9 +220,6 @@
     <t>Necklace</t>
   </si>
   <si>
-    <t>gem-chain</t>
-  </si>
-  <si>
     <t>Chalice</t>
   </si>
   <si>
@@ -364,15 +361,6 @@
     <t>And my axe.</t>
   </si>
   <si>
-    <t>Baseball Bat</t>
-  </si>
-  <si>
-    <t>baseball-bat</t>
-  </si>
-  <si>
-    <t>Crate</t>
-  </si>
-  <si>
     <t>wooden-crate</t>
   </si>
   <si>
@@ -425,6 +413,36 @@
   </si>
   <si>
     <t>Behold the power of purchase.</t>
+  </si>
+  <si>
+    <t>Small Crate</t>
+  </si>
+  <si>
+    <t>Medium Crate</t>
+  </si>
+  <si>
+    <t>Steel Axe</t>
+  </si>
+  <si>
+    <t>-1 Wood per turn</t>
+  </si>
+  <si>
+    <t>Can be purchased for 2 Steel</t>
+  </si>
+  <si>
+    <t>Can be purchased for 3 Steel</t>
+  </si>
+  <si>
+    <t>gem-necklace</t>
+  </si>
+  <si>
+    <t>Crown</t>
+  </si>
+  <si>
+    <t>crown</t>
+  </si>
+  <si>
+    <t>Woah, this really is heavy.</t>
   </si>
 </sst>
 </file>
@@ -800,13 +818,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,7 +932,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
@@ -934,7 +952,7 @@
       </c>
       <c r="K4"/>
       <c r="L4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1007,10 +1025,10 @@
         <v>14</v>
       </c>
       <c r="K7" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="L7" s="6" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -1030,7 +1048,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" ref="G8:G41" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
+        <f t="shared" ref="G8:G43" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
         <v>6</v>
       </c>
       <c r="I8" t="s">
@@ -1380,141 +1398,142 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B20" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="9">
+        <v>3</v>
+      </c>
+      <c r="G20" s="9">
+        <f t="shared" si="0"/>
         <v>4</v>
-      </c>
-      <c r="G20" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
       <c r="H20" s="1">
         <v>-1</v>
       </c>
       <c r="I20" t="s">
-        <v>63</v>
+        <v>136</v>
       </c>
       <c r="J20" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="6" t="s">
-        <v>61</v>
-      </c>
+      <c r="K20"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B21" s="9">
         <v>1</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G21" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="H21" s="1">
+        <v>-1</v>
       </c>
       <c r="I21" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J21" t="s">
         <v>56</v>
       </c>
-      <c r="K21"/>
+      <c r="K21" s="6" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B22" s="9">
         <v>1</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G22" s="9">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="H22" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J22" t="s">
         <v>56</v>
       </c>
-      <c r="K22" s="6"/>
+      <c r="K22"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>68</v>
+        <v>137</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
       </c>
-      <c r="C23" s="9">
-        <v>2</v>
-      </c>
       <c r="E23" s="10"/>
+      <c r="F23" s="9">
+        <v>6</v>
+      </c>
       <c r="G23" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="H23" s="1">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I23" t="s">
-        <v>69</v>
+        <v>138</v>
       </c>
       <c r="J23" t="s">
-        <v>70</v>
-      </c>
-      <c r="K23" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="L23"/>
+        <v>56</v>
+      </c>
+      <c r="K23" s="6"/>
+      <c r="L23" s="2" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
       </c>
       <c r="C24" s="9">
-        <v>2</v>
-      </c>
-      <c r="D24" s="9">
         <v>2</v>
       </c>
       <c r="E24" s="10"/>
       <c r="G24" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
+      </c>
+      <c r="H24" s="1">
+        <v>-1</v>
       </c>
       <c r="I24" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J24" t="s">
+        <v>69</v>
+      </c>
+      <c r="K24" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="K24" s="6" t="s">
-        <v>74</v>
-      </c>
+      <c r="L24"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>119</v>
+        <v>71</v>
       </c>
       <c r="B25" s="9">
         <v>1</v>
@@ -1525,29 +1544,24 @@
       <c r="D25" s="9">
         <v>2</v>
       </c>
-      <c r="E25" s="9">
-        <v>1</v>
-      </c>
-      <c r="F25" s="9">
-        <v>1</v>
-      </c>
+      <c r="E25" s="10"/>
       <c r="G25" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I25" t="s">
-        <v>120</v>
+        <v>72</v>
       </c>
       <c r="J25" t="s">
-        <v>121</v>
-      </c>
-      <c r="K25" s="2" t="s">
-        <v>122</v>
+        <v>69</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
@@ -1555,78 +1569,88 @@
       <c r="C26" s="9">
         <v>2</v>
       </c>
-      <c r="E26" s="10"/>
+      <c r="D26" s="9">
+        <v>2</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
+      <c r="F26" s="9">
+        <v>1</v>
+      </c>
       <c r="G26" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I26" s="7" t="s">
-        <v>76</v>
+        <v>9</v>
+      </c>
+      <c r="I26" t="s">
+        <v>116</v>
       </c>
       <c r="J26" t="s">
-        <v>77</v>
-      </c>
-      <c r="K26" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="L26"/>
+        <v>117</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="B27" s="9">
-        <v>1</v>
-      </c>
-      <c r="E27" s="9">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C27" s="9">
+        <v>2</v>
+      </c>
+      <c r="E27" s="10"/>
       <c r="G27" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I27" t="s">
-        <v>80</v>
+      <c r="I27" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="J27" t="s">
+        <v>76</v>
+      </c>
+      <c r="K27" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="K27" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>82</v>
-      </c>
+      <c r="L27"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B28" s="9">
-        <v>2</v>
-      </c>
-      <c r="D28" s="9">
-        <v>2</v>
-      </c>
-      <c r="E28" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>2</v>
+      </c>
       <c r="G28" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I28" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="J28" t="s">
-        <v>77</v>
-      </c>
-      <c r="K28"/>
+        <v>76</v>
+      </c>
+      <c r="K28" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>81</v>
+      </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B29" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D29" s="9">
         <v>3</v>
@@ -1637,204 +1661,203 @@
         <v>4</v>
       </c>
       <c r="I29" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="J29" t="s">
-        <v>77</v>
-      </c>
-      <c r="K29"/>
+        <v>76</v>
+      </c>
+      <c r="K29" s="6" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="B30" s="9">
         <v>1</v>
       </c>
       <c r="D30" s="9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E30" s="10"/>
       <c r="G30" s="9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="I30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="J30" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B31" s="9">
         <v>1</v>
       </c>
-      <c r="C31" s="9">
-        <v>1</v>
-      </c>
-      <c r="E31" s="9">
-        <v>1</v>
-      </c>
+      <c r="D31" s="9">
+        <v>7</v>
+      </c>
+      <c r="E31" s="10"/>
       <c r="G31" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I31" t="s">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="J31" t="s">
-        <v>92</v>
-      </c>
-      <c r="K31" s="11" t="s">
-        <v>127</v>
+        <v>76</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="B32" s="9">
         <v>1</v>
       </c>
-      <c r="D32" s="9">
+      <c r="C32" s="9">
+        <v>1</v>
+      </c>
+      <c r="E32" s="9">
+        <v>1</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G32" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
       <c r="I32" t="s">
+        <v>96</v>
+      </c>
+      <c r="J32" t="s">
         <v>91</v>
       </c>
-      <c r="J32" t="s">
-        <v>92</v>
-      </c>
       <c r="K32" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="L32"/>
+        <v>123</v>
+      </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
       </c>
-      <c r="C33" s="9">
+      <c r="D33" s="9">
         <v>3</v>
       </c>
-      <c r="E33" s="10"/>
       <c r="G33" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I33" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K33" s="11" t="s">
-        <v>127</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>95</v>
-      </c>
+        <v>123</v>
+      </c>
+      <c r="L33"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="B34" s="9">
-        <v>2</v>
-      </c>
-      <c r="E34" s="9">
+        <v>1</v>
+      </c>
+      <c r="C34" s="9">
         <v>3</v>
       </c>
+      <c r="E34" s="10"/>
       <c r="G34" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I34" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="J34" t="s">
-        <v>92</v>
-      </c>
-      <c r="K34"/>
+        <v>91</v>
+      </c>
+      <c r="K34" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B35" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="G35" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I35" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J35" t="s">
-        <v>92</v>
-      </c>
-      <c r="K35" s="6" t="s">
-        <v>102</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="K35"/>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
       </c>
-      <c r="C36" s="9">
-        <v>2</v>
-      </c>
-      <c r="D36" s="9">
-        <v>1</v>
-      </c>
-      <c r="E36" s="10"/>
+      <c r="E36" s="9">
+        <v>6</v>
+      </c>
       <c r="G36" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I36" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="J36" t="s">
-        <v>105</v>
-      </c>
-      <c r="K36" t="s">
-        <v>130</v>
+        <v>91</v>
+      </c>
+      <c r="K36" s="6" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B37" s="9">
         <v>1</v>
       </c>
       <c r="C37" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D37" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E37" s="10"/>
       <c r="G37" s="9">
@@ -1842,111 +1865,170 @@
         <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J37" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K37" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B38" s="9">
         <v>1</v>
       </c>
-      <c r="E38" s="9">
-        <v>1</v>
-      </c>
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+      <c r="D38" s="9">
+        <v>2</v>
+      </c>
+      <c r="E38" s="10"/>
       <c r="G38" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J38" t="s">
-        <v>110</v>
-      </c>
-      <c r="K38" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="L38" s="6" t="s">
-        <v>112</v>
+        <v>104</v>
+      </c>
+      <c r="K38" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>113</v>
+        <v>132</v>
       </c>
       <c r="B39" s="9">
         <v>1</v>
       </c>
-      <c r="C39" s="9">
-        <v>3</v>
+      <c r="D39" s="9">
+        <v>1</v>
       </c>
       <c r="E39" s="10"/>
       <c r="G39" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I39" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="J39" t="s">
-        <v>110</v>
-      </c>
-      <c r="K39"/>
+        <v>109</v>
+      </c>
+      <c r="K39" s="11" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B40" s="9">
         <v>1</v>
       </c>
-      <c r="C40" s="9">
-        <v>4</v>
-      </c>
-      <c r="E40" s="10"/>
+      <c r="E40" s="9">
+        <v>1</v>
+      </c>
       <c r="G40" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I40" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="J40" t="s">
+        <v>109</v>
+      </c>
+      <c r="K40" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="K40"/>
+      <c r="L40" s="6" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B41" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C41" s="9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E41" s="10"/>
       <c r="G41" s="9">
         <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I41" t="s">
+        <v>112</v>
+      </c>
+      <c r="J41" t="s">
+        <v>109</v>
+      </c>
+      <c r="K41"/>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>131</v>
+      </c>
+      <c r="B42" s="9">
+        <v>2</v>
+      </c>
+      <c r="C42" s="9">
+        <v>4</v>
+      </c>
+      <c r="E42" s="10"/>
+      <c r="G42" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H42" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>112</v>
+      </c>
+      <c r="J42" t="s">
+        <v>109</v>
+      </c>
+      <c r="K42"/>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>113</v>
+      </c>
+      <c r="B43" s="9">
+        <v>1</v>
+      </c>
+      <c r="C43" s="9">
+        <v>7</v>
+      </c>
+      <c r="E43" s="10"/>
+      <c r="G43" s="9">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I41" t="s">
-        <v>118</v>
-      </c>
-      <c r="J41" t="s">
-        <v>110</v>
-      </c>
-      <c r="K41" s="6" t="s">
-        <v>129</v>
+      <c r="I43" t="s">
+        <v>114</v>
+      </c>
+      <c r="J43" t="s">
+        <v>109</v>
+      </c>
+      <c r="K43" s="6" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1975,10 +2057,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2037,13 +2119,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2051,11 +2133,11 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <f>COUNTA(Deck!C2:C101)</f>
+        <f>COUNTA(Deck!C2:C103)</f>
         <v>18</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(Deck!C2:C100)</f>
+        <f>SUM(Deck!C2:C102)</f>
         <v>40</v>
       </c>
     </row>
@@ -2064,12 +2146,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <f>COUNTA(Deck!D2:D101)</f>
-        <v>17</v>
+        <f>COUNTA(Deck!D2:D103)</f>
+        <v>18</v>
       </c>
       <c r="C3" s="1">
-        <f>SUM(Deck!D2:D100)</f>
-        <v>35</v>
+        <f>SUM(Deck!D2:D102)</f>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2077,11 +2159,11 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <f>COUNTA(Deck!E2:E101)</f>
+        <f>COUNTA(Deck!E2:E103)</f>
         <v>11</v>
       </c>
       <c r="C4" s="1">
-        <f>SUM(Deck!E2:E100)</f>
+        <f>SUM(Deck!E2:E102)</f>
         <v>19</v>
       </c>
     </row>
@@ -2090,12 +2172,12 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <f>COUNTA(Deck!F2:F101)</f>
-        <v>12</v>
+        <f>COUNTA(Deck!F2:F103)</f>
+        <v>13</v>
       </c>
       <c r="C5" s="1">
-        <f>SUM(Deck!F2:F101)</f>
-        <v>23</v>
+        <f>SUM(Deck!F2:F103)</f>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Chalice now has a place
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -824,7 +824,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H20" sqref="H20"/>
+      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1459,11 +1459,11 @@
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G22" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I22" t="s">
         <v>66</v>
@@ -2177,7 +2177,7 @@
       </c>
       <c r="C5" s="1">
         <f>SUM(Deck!F2:F103)</f>
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Game balance updates after playing with Brad
Broadly: a bunch more cards. Fill out the 7-8 VP cards to better head down a given path.

* Ladder is cheaper (1 Wood)
* New category: pass. Added Boomerang that passes from one player to another
* Gold Path: Added Gold Key to help with the Gold Path strategy
* Gold Path: Pendant got nerfed on the VP a bit
* Gold Path: Necklace got a real bonus so it's not useless
* Steel Path: Added Uzi for 7VP
* Steel Path: Added Battle Axe for 8VP
* Stone Path: Added two Stone Piles at 3VP to help get to Stone tablet at 5VP
* Stone Path: Added Rune Stone, a 7VP card with gold
* Wood Path: Added second Steel Axe to make Wood Path easier to get into
* Wood Path: Added Sign Post at 7VP, two of those cards
* Wood Path: Added Wizard Staff, which has some game-end scoring and requires Gold

This might be too many cards, which could extend the game.
But maybe we just dump a few of each at game beginning?
Either way, it's worth testing these out
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="160">
   <si>
     <t>Name</t>
   </si>
@@ -443,6 +443,66 @@
   </si>
   <si>
     <t>Woah, this really is heavy.</t>
+  </si>
+  <si>
+    <t>Uzi</t>
+  </si>
+  <si>
+    <t>uzi</t>
+  </si>
+  <si>
+    <t>Can be purchased for 4 Steel</t>
+  </si>
+  <si>
+    <t>Battle Axe</t>
+  </si>
+  <si>
+    <t>battle-axe</t>
+  </si>
+  <si>
+    <t>Gold Key</t>
+  </si>
+  <si>
+    <t>key</t>
+  </si>
+  <si>
+    <t>-1 Gold to build items consisting only of Gold</t>
+  </si>
+  <si>
+    <t>Stone Pile</t>
+  </si>
+  <si>
+    <t>stone-pile</t>
+  </si>
+  <si>
+    <t>rune-stone</t>
+  </si>
+  <si>
+    <t>Rune Stone</t>
+  </si>
+  <si>
+    <t>Sign Post</t>
+  </si>
+  <si>
+    <t>wooden-sign</t>
+  </si>
+  <si>
+    <t>Wizard Staff</t>
+  </si>
+  <si>
+    <t>At game end, 1 VP per two Wood in any cards except this one.</t>
+  </si>
+  <si>
+    <t>Boomerang</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>-1 Wood for the current turn. At end of turn, pass to left and place in opponent's hand.</t>
+  </si>
+  <si>
+    <t>boomerang</t>
   </si>
 </sst>
 </file>
@@ -818,13 +878,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L43"/>
+  <dimension ref="A1:L51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1048,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" ref="G8:G43" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
+        <f t="shared" ref="G8:G51" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
         <v>6</v>
       </c>
       <c r="I8" t="s">
@@ -1190,15 +1250,12 @@
         <v>1</v>
       </c>
       <c r="C13" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E13" s="10"/>
       <c r="G13" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H13" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I13" t="s">
         <v>42</v>
@@ -1342,226 +1399,222 @@
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>54</v>
+        <v>156</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
       </c>
-      <c r="E18" s="10"/>
-      <c r="F18" s="9">
+      <c r="C18" s="9">
         <v>1</v>
       </c>
       <c r="G18" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I18" t="s">
-        <v>55</v>
+        <v>159</v>
       </c>
       <c r="J18" t="s">
-        <v>56</v>
-      </c>
-      <c r="K18" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L18" s="6" t="s">
-        <v>58</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B19" s="9">
         <v>1</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H19" s="1">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J19" t="s">
         <v>56</v>
       </c>
-      <c r="K19" t="s">
-        <v>61</v>
+      <c r="K19" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L19" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>145</v>
       </c>
       <c r="B20" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G20" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H20" s="1">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I20" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
       <c r="J20" t="s">
         <v>56</v>
       </c>
-      <c r="K20"/>
+      <c r="K20" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="B21" s="9">
         <v>1</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G21" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H21" s="1">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="I21" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J21" t="s">
         <v>56</v>
       </c>
-      <c r="K21" s="6" t="s">
+      <c r="K21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="9">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G22" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
+      </c>
+      <c r="H22" s="1">
+        <v>-1</v>
       </c>
       <c r="I22" t="s">
-        <v>66</v>
+        <v>136</v>
       </c>
       <c r="J22" t="s">
         <v>56</v>
       </c>
-      <c r="K22"/>
+      <c r="K22" s="11" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="9">
+        <v>4</v>
+      </c>
+      <c r="G23" s="9">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G23" s="9">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
       <c r="H23" s="1">
-        <v>2</v>
+        <v>-1</v>
       </c>
       <c r="I23" t="s">
-        <v>138</v>
+        <v>63</v>
       </c>
       <c r="J23" t="s">
         <v>56</v>
       </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="2" t="s">
-        <v>139</v>
+      <c r="K23" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
       </c>
-      <c r="C24" s="9">
-        <v>2</v>
-      </c>
       <c r="E24" s="10"/>
+      <c r="F24" s="9">
+        <v>5</v>
+      </c>
       <c r="G24" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H24" s="1">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="I24" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="J24" t="s">
-        <v>69</v>
-      </c>
-      <c r="K24" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="L24"/>
+        <v>56</v>
+      </c>
+      <c r="K24"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>71</v>
+        <v>137</v>
       </c>
       <c r="B25" s="9">
         <v>1</v>
       </c>
-      <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="D25" s="9">
-        <v>2</v>
-      </c>
       <c r="E25" s="10"/>
+      <c r="F25" s="9">
+        <v>6</v>
+      </c>
       <c r="G25" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>13</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2</v>
       </c>
       <c r="I25" t="s">
-        <v>72</v>
+        <v>138</v>
       </c>
       <c r="J25" t="s">
-        <v>69</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>73</v>
+        <v>56</v>
+      </c>
+      <c r="K25" s="6"/>
+      <c r="L25" s="2" t="s">
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>115</v>
+        <v>67</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
@@ -1569,323 +1622,326 @@
       <c r="C26" s="9">
         <v>2</v>
       </c>
-      <c r="D26" s="9">
-        <v>2</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1</v>
-      </c>
-      <c r="F26" s="9">
-        <v>1</v>
-      </c>
+      <c r="E26" s="10"/>
       <c r="G26" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>2</v>
+      </c>
+      <c r="H26" s="1">
+        <v>-1</v>
       </c>
       <c r="I26" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="J26" t="s">
-        <v>117</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>118</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="L26"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B27" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" s="9">
+        <v>2</v>
+      </c>
+      <c r="D27" s="9">
         <v>2</v>
       </c>
       <c r="E27" s="10"/>
       <c r="G27" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I27" s="7" t="s">
-        <v>75</v>
+        <v>5</v>
+      </c>
+      <c r="I27" t="s">
+        <v>72</v>
       </c>
       <c r="J27" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="K27" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="L27"/>
+        <v>73</v>
+      </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>78</v>
+        <v>115</v>
       </c>
       <c r="B28" s="9">
         <v>1</v>
       </c>
+      <c r="C28" s="9">
+        <v>2</v>
+      </c>
+      <c r="D28" s="9">
+        <v>2</v>
+      </c>
       <c r="E28" s="9">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="F28" s="9">
+        <v>1</v>
       </c>
       <c r="G28" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I28" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="J28" t="s">
-        <v>76</v>
-      </c>
-      <c r="K28" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>81</v>
+        <v>117</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B29" s="9">
         <v>2</v>
       </c>
-      <c r="D29" s="9">
-        <v>3</v>
+      <c r="C29" s="9">
+        <v>2</v>
       </c>
       <c r="E29" s="10"/>
       <c r="G29" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I29" t="s">
-        <v>83</v>
+        <v>3</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>75</v>
       </c>
       <c r="J29" t="s">
         <v>76</v>
       </c>
       <c r="K29" s="6" t="s">
-        <v>134</v>
-      </c>
+        <v>77</v>
+      </c>
+      <c r="L29"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="B30" s="9">
         <v>1</v>
       </c>
-      <c r="D30" s="9">
-        <v>4</v>
-      </c>
-      <c r="E30" s="10"/>
+      <c r="E30" s="9">
+        <v>2</v>
+      </c>
       <c r="G30" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I30" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="J30" t="s">
         <v>76</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>135</v>
+        <v>80</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B31" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D31" s="9">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" s="9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="I31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="J31" t="s">
         <v>76</v>
       </c>
       <c r="K31" s="6" t="s">
-        <v>88</v>
+        <v>134</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="B32" s="9">
         <v>1</v>
       </c>
-      <c r="C32" s="9">
-        <v>1</v>
-      </c>
-      <c r="E32" s="9">
-        <v>1</v>
-      </c>
+      <c r="D32" s="9">
+        <v>4</v>
+      </c>
+      <c r="E32" s="10"/>
       <c r="G32" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I32" t="s">
-        <v>96</v>
+        <v>85</v>
       </c>
       <c r="J32" t="s">
-        <v>91</v>
-      </c>
-      <c r="K32" s="11" t="s">
-        <v>123</v>
+        <v>76</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>89</v>
+        <v>140</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
       </c>
       <c r="D33" s="9">
-        <v>3</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E33" s="10"/>
       <c r="G33" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I33" t="s">
-        <v>90</v>
+        <v>141</v>
       </c>
       <c r="J33" t="s">
-        <v>91</v>
-      </c>
-      <c r="K33" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="L33"/>
+        <v>76</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>142</v>
+      </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>92</v>
+        <v>143</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
       </c>
-      <c r="C34" s="9">
-        <v>3</v>
+      <c r="D34" s="9">
+        <v>5</v>
       </c>
       <c r="E34" s="10"/>
       <c r="G34" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>93</v>
+        <v>144</v>
       </c>
       <c r="J34" t="s">
-        <v>91</v>
-      </c>
-      <c r="K34" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="L34" s="6" t="s">
-        <v>94</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="K34" s="6"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>97</v>
+        <v>86</v>
       </c>
       <c r="B35" s="9">
-        <v>2</v>
-      </c>
-      <c r="E35" s="9">
-        <v>3</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="D35" s="9">
+        <v>7</v>
+      </c>
+      <c r="E35" s="10"/>
       <c r="G35" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I35" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="J35" t="s">
-        <v>91</v>
-      </c>
-      <c r="K35"/>
+        <v>76</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
       </c>
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
       <c r="E36" s="9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G36" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I36" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="J36" t="s">
         <v>91</v>
       </c>
-      <c r="K36" s="6" t="s">
-        <v>101</v>
+      <c r="K36" s="11" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="B37" s="9">
         <v>1</v>
       </c>
-      <c r="C37" s="9">
-        <v>2</v>
-      </c>
       <c r="D37" s="9">
-        <v>1</v>
-      </c>
-      <c r="E37" s="10"/>
+        <v>3</v>
+      </c>
       <c r="G37" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="I37" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="J37" t="s">
-        <v>104</v>
-      </c>
-      <c r="K37" t="s">
-        <v>126</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="K37" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L37"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="B38" s="9">
         <v>1</v>
       </c>
       <c r="C38" s="9">
-        <v>1</v>
-      </c>
-      <c r="D38" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E38" s="10"/>
       <c r="G38" s="9">
@@ -1893,141 +1949,349 @@
         <v>4</v>
       </c>
       <c r="I38" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="J38" t="s">
-        <v>104</v>
-      </c>
-      <c r="K38" t="s">
-        <v>126</v>
+        <v>91</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="L38" s="6" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
       <c r="B39" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D39" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="10"/>
       <c r="G39" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>108</v>
+        <v>149</v>
       </c>
       <c r="J39" t="s">
-        <v>109</v>
-      </c>
-      <c r="K39" s="11" t="s">
-        <v>133</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="K39" s="11"/>
+      <c r="L39" s="6"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B40" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G40" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I40" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="J40" t="s">
-        <v>109</v>
-      </c>
-      <c r="K40" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="L40" s="6" t="s">
-        <v>111</v>
-      </c>
+        <v>91</v>
+      </c>
+      <c r="K40"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>130</v>
+        <v>151</v>
       </c>
       <c r="B41" s="9">
-        <v>2</v>
-      </c>
-      <c r="C41" s="9">
-        <v>3</v>
-      </c>
-      <c r="E41" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="9">
+        <v>2</v>
+      </c>
+      <c r="F41" s="9">
+        <v>2</v>
+      </c>
       <c r="G41" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H41" s="1">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="I41" t="s">
-        <v>112</v>
+        <v>150</v>
       </c>
       <c r="J41" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
       <c r="K41"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>131</v>
+        <v>99</v>
       </c>
       <c r="B42" s="9">
-        <v>2</v>
-      </c>
-      <c r="C42" s="9">
-        <v>4</v>
-      </c>
-      <c r="E42" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="E42" s="9">
+        <v>6</v>
+      </c>
       <c r="G42" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H42" s="1">
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="I42" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="J42" t="s">
-        <v>109</v>
-      </c>
-      <c r="K42"/>
+        <v>91</v>
+      </c>
+      <c r="K42" s="6" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="B43" s="9">
         <v>1</v>
       </c>
       <c r="C43" s="9">
-        <v>7</v>
+        <v>2</v>
+      </c>
+      <c r="D43" s="9">
+        <v>1</v>
       </c>
       <c r="E43" s="10"/>
       <c r="G43" s="9">
         <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I43" t="s">
+        <v>103</v>
+      </c>
+      <c r="J43" t="s">
+        <v>104</v>
+      </c>
+      <c r="K43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>105</v>
+      </c>
+      <c r="B44" s="9">
+        <v>1</v>
+      </c>
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+      <c r="D44" s="9">
+        <v>2</v>
+      </c>
+      <c r="E44" s="10"/>
+      <c r="G44" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I44" t="s">
+        <v>106</v>
+      </c>
+      <c r="J44" t="s">
+        <v>104</v>
+      </c>
+      <c r="K44" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>132</v>
+      </c>
+      <c r="B45" s="9">
+        <v>2</v>
+      </c>
+      <c r="D45" s="9">
+        <v>1</v>
+      </c>
+      <c r="E45" s="10"/>
+      <c r="G45" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I45" t="s">
+        <v>108</v>
+      </c>
+      <c r="J45" t="s">
+        <v>109</v>
+      </c>
+      <c r="K45" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>107</v>
+      </c>
+      <c r="B46" s="9">
+        <v>1</v>
+      </c>
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
+      <c r="G46" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I46" t="s">
+        <v>108</v>
+      </c>
+      <c r="J46" t="s">
+        <v>109</v>
+      </c>
+      <c r="K46" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="L46" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>130</v>
+      </c>
+      <c r="B47" s="9">
+        <v>2</v>
+      </c>
+      <c r="C47" s="9">
+        <v>3</v>
+      </c>
+      <c r="E47" s="10"/>
+      <c r="G47" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H47" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I47" t="s">
+        <v>112</v>
+      </c>
+      <c r="J47" t="s">
+        <v>109</v>
+      </c>
+      <c r="K47"/>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>131</v>
+      </c>
+      <c r="B48" s="9">
+        <v>2</v>
+      </c>
+      <c r="C48" s="9">
+        <v>4</v>
+      </c>
+      <c r="E48" s="10"/>
+      <c r="G48" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H48" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I48" t="s">
+        <v>112</v>
+      </c>
+      <c r="J48" t="s">
+        <v>109</v>
+      </c>
+      <c r="K48"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>152</v>
+      </c>
+      <c r="B49" s="9">
+        <v>2</v>
+      </c>
+      <c r="C49" s="9">
+        <v>5</v>
+      </c>
+      <c r="E49" s="10"/>
+      <c r="G49" s="9">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I49" t="s">
+        <v>153</v>
+      </c>
+      <c r="J49" t="s">
+        <v>109</v>
+      </c>
+      <c r="K49"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>154</v>
+      </c>
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
+      <c r="C50" s="9">
+        <v>4</v>
+      </c>
+      <c r="E50" s="10"/>
+      <c r="F50" s="9">
+        <v>1</v>
+      </c>
+      <c r="G50" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H50" s="1">
+        <v>1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>153</v>
+      </c>
+      <c r="J50" t="s">
+        <v>109</v>
+      </c>
+      <c r="K50" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>113</v>
+      </c>
+      <c r="B51" s="9">
+        <v>1</v>
+      </c>
+      <c r="C51" s="9">
+        <v>7</v>
+      </c>
+      <c r="E51" s="10"/>
+      <c r="G51" s="9">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I51" t="s">
         <v>114</v>
       </c>
-      <c r="J43" t="s">
+      <c r="J51" t="s">
         <v>109</v>
       </c>
-      <c r="K43" s="6" t="s">
+      <c r="K51" s="6" t="s">
         <v>125</v>
       </c>
     </row>
@@ -2044,7 +2308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2106,7 +2370,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2133,12 +2397,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <f>COUNTA(Deck!C2:C103)</f>
-        <v>18</v>
+        <f>COUNTA(Deck!C2:C111)</f>
+        <v>21</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(Deck!C2:C102)</f>
-        <v>40</v>
+        <f>SUM(Deck!C2:C110)</f>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2146,12 +2410,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <f>COUNTA(Deck!D2:D103)</f>
-        <v>18</v>
+        <f>COUNTA(Deck!D2:D111)</f>
+        <v>21</v>
       </c>
       <c r="C3" s="1">
-        <f>SUM(Deck!D2:D102)</f>
-        <v>38</v>
+        <f>SUM(Deck!D2:D110)</f>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2159,12 +2423,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <f>COUNTA(Deck!E2:E103)</f>
-        <v>11</v>
+        <f>COUNTA(Deck!E2:E111)</f>
+        <v>12</v>
       </c>
       <c r="C4" s="1">
-        <f>SUM(Deck!E2:E102)</f>
-        <v>19</v>
+        <f>SUM(Deck!E2:E110)</f>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2172,12 +2436,12 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <f>COUNTA(Deck!F2:F103)</f>
-        <v>13</v>
+        <f>COUNTA(Deck!F2:F111)</f>
+        <v>16</v>
       </c>
       <c r="C5" s="1">
-        <f>SUM(Deck!F2:F103)</f>
-        <v>28</v>
+        <f>SUM(Deck!F2:F111)</f>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New card layout with negative space, added a survival element
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -18,12 +18,12 @@
     <definedName name="WoodValue">VPs!$B$2</definedName>
     <definedName name="WoodVP">VPs!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="145621" iterateDelta="1E-4"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="164">
   <si>
     <t>Name</t>
   </si>
@@ -503,6 +503,18 @@
   </si>
   <si>
     <t>boomerang</t>
+  </si>
+  <si>
+    <t>food</t>
+  </si>
+  <si>
+    <t>shelter</t>
+  </si>
+  <si>
+    <t>clothing</t>
+  </si>
+  <si>
+    <t>VPtype</t>
   </si>
 </sst>
 </file>
@@ -878,13 +890,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L51"/>
+  <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I18" sqref="I18"/>
+      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,14 +909,15 @@
     <col min="6" max="6" width="5.28515625" style="9"/>
     <col min="7" max="7" width="9.140625" style="9"/>
     <col min="8" max="8" width="6.140625" style="1"/>
-    <col min="9" max="9" width="14.85546875"/>
-    <col min="10" max="10" width="10.28515625"/>
-    <col min="11" max="11" width="73.5703125" style="2"/>
-    <col min="12" max="12" width="40" style="2"/>
-    <col min="13" max="1025" width="8.5703125"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="14.85546875"/>
+    <col min="11" max="11" width="10.28515625"/>
+    <col min="12" max="12" width="73.5703125" style="2"/>
+    <col min="13" max="13" width="40" style="2"/>
+    <col min="14" max="1026" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -929,20 +942,23 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -956,18 +972,21 @@
       <c r="G2" s="9">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>14</v>
       </c>
-      <c r="K2"/>
-      <c r="L2" s="6" t="s">
+      <c r="L2"/>
+      <c r="M2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -981,16 +1000,19 @@
       <c r="G3" s="9">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
+      <c r="I3" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>14</v>
       </c>
-      <c r="K3"/>
       <c r="L3"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>124</v>
       </c>
@@ -1004,18 +1026,21 @@
       <c r="G4" s="9">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
+      <c r="I4" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J4" t="s">
         <v>18</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>14</v>
       </c>
-      <c r="K4"/>
-      <c r="L4" t="s">
+      <c r="L4"/>
+      <c r="M4" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1029,18 +1054,21 @@
       <c r="G5" s="9">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
+      <c r="I5" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J5" t="s">
         <v>20</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>14</v>
       </c>
-      <c r="K5"/>
-      <c r="L5" s="6" t="s">
+      <c r="L5"/>
+      <c r="M5" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1053,18 +1081,21 @@
       <c r="G6" s="9">
         <v>0</v>
       </c>
-      <c r="I6" t="s">
+      <c r="I6" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J6" t="s">
         <v>22</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>14</v>
       </c>
-      <c r="K6"/>
-      <c r="L6" s="6" t="s">
+      <c r="L6"/>
+      <c r="M6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -1078,20 +1109,23 @@
       <c r="G7" s="9">
         <v>0</v>
       </c>
-      <c r="I7" t="s">
+      <c r="I7" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J7" t="s">
         <v>25</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>14</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>127</v>
       </c>
-      <c r="L7" s="6" t="s">
+      <c r="M7" s="6" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -1111,17 +1145,20 @@
         <f t="shared" ref="G8:G51" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
         <v>6</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J8" t="s">
         <v>27</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>28</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -1142,17 +1179,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I9" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J9" t="s">
         <v>31</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>28</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -1172,17 +1212,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I10" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J10" t="s">
         <v>33</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>28</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -1202,17 +1245,20 @@
       <c r="H11" s="1">
         <v>-1</v>
       </c>
-      <c r="I11" t="s">
+      <c r="I11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J11" t="s">
         <v>35</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>36</v>
       </c>
-      <c r="K11" s="6" t="s">
+      <c r="L11" s="6" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>38</v>
       </c>
@@ -1232,17 +1278,20 @@
       <c r="H12" s="1">
         <v>-1</v>
       </c>
-      <c r="I12" t="s">
+      <c r="I12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J12" t="s">
         <v>39</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>36</v>
       </c>
-      <c r="K12" s="6" t="s">
+      <c r="L12" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>41</v>
       </c>
@@ -1257,18 +1306,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I13" t="s">
+      <c r="I13" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J13" t="s">
         <v>42</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>43</v>
       </c>
-      <c r="K13" s="6" t="s">
+      <c r="L13" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>45</v>
       </c>
@@ -1286,18 +1338,21 @@
       <c r="H14" s="1">
         <v>-1</v>
       </c>
-      <c r="I14" t="s">
+      <c r="I14" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J14" t="s">
         <v>46</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>43</v>
       </c>
-      <c r="K14" s="6" t="s">
+      <c r="L14" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>48</v>
       </c>
@@ -1317,20 +1372,23 @@
       <c r="H15" s="1">
         <v>-1</v>
       </c>
-      <c r="I15" t="s">
+      <c r="I15" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J15" t="s">
         <v>49</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>43</v>
       </c>
-      <c r="K15" s="6" t="s">
+      <c r="L15" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="L15" s="6" t="s">
+      <c r="M15" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -1351,20 +1409,23 @@
       <c r="H16" s="1">
         <v>-1</v>
       </c>
-      <c r="I16" t="s">
+      <c r="I16" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J16" t="s">
         <v>49</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>43</v>
       </c>
-      <c r="K16" s="6" t="s">
+      <c r="L16" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="M16" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>53</v>
       </c>
@@ -1384,20 +1445,23 @@
       <c r="H17" s="1">
         <v>-1</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J17" t="s">
         <v>49</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="6" t="s">
+      <c r="L17" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="M17" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>156</v>
       </c>
@@ -1411,18 +1475,21 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J18" t="s">
         <v>159</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>157</v>
       </c>
-      <c r="K18" s="11" t="s">
+      <c r="L18" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="L18" s="6"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" s="6"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>54</v>
       </c>
@@ -1437,20 +1504,23 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J19" t="s">
         <v>55</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>56</v>
       </c>
-      <c r="K19" s="6" t="s">
+      <c r="L19" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="L19" s="6" t="s">
+      <c r="M19" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>145</v>
       </c>
@@ -1465,18 +1535,21 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J20" t="s">
         <v>146</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>56</v>
       </c>
-      <c r="K20" s="11" t="s">
+      <c r="L20" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="L20" s="6"/>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" s="6"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>59</v>
       </c>
@@ -1494,17 +1567,20 @@
       <c r="H21" s="1">
         <v>-2</v>
       </c>
-      <c r="I21" t="s">
+      <c r="I21" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J21" t="s">
         <v>60</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>56</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -1522,17 +1598,20 @@
       <c r="H22" s="1">
         <v>-1</v>
       </c>
-      <c r="I22" t="s">
+      <c r="I22" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J22" t="s">
         <v>136</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>56</v>
       </c>
-      <c r="K22" s="11" t="s">
+      <c r="L22" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>62</v>
       </c>
@@ -1550,17 +1629,20 @@
       <c r="H23" s="1">
         <v>-1</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J23" t="s">
         <v>63</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>56</v>
       </c>
-      <c r="K23" s="6" t="s">
+      <c r="L23" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>65</v>
       </c>
@@ -1575,15 +1657,18 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I24" t="s">
+      <c r="I24" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J24" t="s">
         <v>66</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>56</v>
       </c>
-      <c r="K24"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L24"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -1601,18 +1686,21 @@
       <c r="H25" s="1">
         <v>2</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I25" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J25" t="s">
         <v>138</v>
       </c>
-      <c r="J25" t="s">
+      <c r="K25" t="s">
         <v>56</v>
       </c>
-      <c r="K25" s="6"/>
-      <c r="L25" s="2" t="s">
+      <c r="L25" s="6"/>
+      <c r="M25" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -1630,18 +1718,21 @@
       <c r="H26" s="1">
         <v>-1</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J26" t="s">
         <v>68</v>
       </c>
-      <c r="J26" t="s">
+      <c r="K26" t="s">
         <v>69</v>
       </c>
-      <c r="K26" s="6" t="s">
+      <c r="L26" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>71</v>
       </c>
@@ -1659,17 +1750,20 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I27" t="s">
+      <c r="I27" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J27" t="s">
         <v>72</v>
       </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>69</v>
       </c>
-      <c r="K27" s="6" t="s">
+      <c r="L27" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>115</v>
       </c>
@@ -1692,17 +1786,20 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J28" t="s">
         <v>116</v>
       </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>117</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="L28" s="2" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>74</v>
       </c>
@@ -1717,18 +1814,21 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J29" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
         <v>76</v>
       </c>
-      <c r="K29" s="6" t="s">
+      <c r="L29" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>78</v>
       </c>
@@ -1742,20 +1842,23 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I30" t="s">
+      <c r="I30" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J30" t="s">
         <v>79</v>
       </c>
-      <c r="J30" t="s">
+      <c r="K30" t="s">
         <v>76</v>
       </c>
-      <c r="K30" s="6" t="s">
+      <c r="L30" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="L30" s="6" t="s">
+      <c r="M30" s="6" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>82</v>
       </c>
@@ -1770,17 +1873,20 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I31" t="s">
+      <c r="I31" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J31" t="s">
         <v>83</v>
       </c>
-      <c r="J31" t="s">
+      <c r="K31" t="s">
         <v>76</v>
       </c>
-      <c r="K31" s="6" t="s">
+      <c r="L31" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>84</v>
       </c>
@@ -1795,17 +1901,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I32" t="s">
+      <c r="I32" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J32" t="s">
         <v>85</v>
       </c>
-      <c r="J32" t="s">
+      <c r="K32" t="s">
         <v>76</v>
       </c>
-      <c r="K32" s="6" t="s">
+      <c r="L32" s="6" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>140</v>
       </c>
@@ -1820,17 +1929,20 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I33" t="s">
+      <c r="I33" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J33" t="s">
         <v>141</v>
       </c>
-      <c r="J33" t="s">
+      <c r="K33" t="s">
         <v>76</v>
       </c>
-      <c r="K33" s="6" t="s">
+      <c r="L33" s="6" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>143</v>
       </c>
@@ -1848,15 +1960,18 @@
       <c r="H34" s="1">
         <v>1</v>
       </c>
-      <c r="I34" t="s">
+      <c r="I34" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J34" t="s">
         <v>144</v>
       </c>
-      <c r="J34" t="s">
+      <c r="K34" t="s">
         <v>76</v>
       </c>
-      <c r="K34" s="6"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L34" s="6"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>86</v>
       </c>
@@ -1871,17 +1986,20 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="I35" t="s">
+      <c r="I35" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J35" t="s">
         <v>87</v>
       </c>
-      <c r="J35" t="s">
+      <c r="K35" t="s">
         <v>76</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="L35" s="6" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>95</v>
       </c>
@@ -1898,17 +2016,20 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I36" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J36" t="s">
         <v>96</v>
       </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>91</v>
       </c>
-      <c r="K36" s="11" t="s">
+      <c r="L36" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>89</v>
       </c>
@@ -1922,18 +2043,21 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J37" t="s">
         <v>90</v>
       </c>
-      <c r="J37" t="s">
+      <c r="K37" t="s">
         <v>91</v>
       </c>
-      <c r="K37" s="11" t="s">
+      <c r="L37" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="L37"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>92</v>
       </c>
@@ -1948,20 +2072,23 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J38" t="s">
         <v>93</v>
       </c>
-      <c r="J38" t="s">
+      <c r="K38" t="s">
         <v>91</v>
       </c>
-      <c r="K38" s="11" t="s">
+      <c r="L38" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="L38" s="6" t="s">
+      <c r="M38" s="6" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>148</v>
       </c>
@@ -1976,16 +2103,19 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I39" t="s">
+      <c r="I39" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J39" t="s">
         <v>149</v>
       </c>
-      <c r="J39" t="s">
+      <c r="K39" t="s">
         <v>91</v>
       </c>
-      <c r="K39" s="11"/>
-      <c r="L39" s="6"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L39" s="11"/>
+      <c r="M39" s="6"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>97</v>
       </c>
@@ -1999,15 +2129,18 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="I40" t="s">
+      <c r="I40" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J40" t="s">
         <v>98</v>
       </c>
-      <c r="J40" t="s">
+      <c r="K40" t="s">
         <v>91</v>
       </c>
-      <c r="K40"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L40"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>151</v>
       </c>
@@ -2024,15 +2157,18 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I41" t="s">
+      <c r="I41" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J41" t="s">
         <v>150</v>
       </c>
-      <c r="J41" t="s">
+      <c r="K41" t="s">
         <v>91</v>
       </c>
-      <c r="K41"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L41"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>99</v>
       </c>
@@ -2046,17 +2182,20 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I42" t="s">
+      <c r="I42" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J42" t="s">
         <v>100</v>
       </c>
-      <c r="J42" t="s">
+      <c r="K42" t="s">
         <v>91</v>
       </c>
-      <c r="K42" s="6" t="s">
+      <c r="L42" s="6" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>102</v>
       </c>
@@ -2074,17 +2213,20 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I43" t="s">
+      <c r="I43" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J43" t="s">
         <v>103</v>
       </c>
-      <c r="J43" t="s">
+      <c r="K43" t="s">
         <v>104</v>
       </c>
-      <c r="K43" t="s">
+      <c r="L43" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>105</v>
       </c>
@@ -2102,17 +2244,20 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="I44" t="s">
+      <c r="I44" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J44" t="s">
         <v>106</v>
       </c>
-      <c r="J44" t="s">
+      <c r="K44" t="s">
         <v>104</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>132</v>
       </c>
@@ -2127,17 +2272,20 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I45" t="s">
+      <c r="I45" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J45" t="s">
         <v>108</v>
       </c>
-      <c r="J45" t="s">
+      <c r="K45" t="s">
         <v>109</v>
       </c>
-      <c r="K45" s="11" t="s">
+      <c r="L45" s="11" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>107</v>
       </c>
@@ -2151,20 +2299,23 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I46" t="s">
+      <c r="I46" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J46" t="s">
         <v>108</v>
       </c>
-      <c r="J46" t="s">
+      <c r="K46" t="s">
         <v>109</v>
       </c>
-      <c r="K46" s="6" t="s">
+      <c r="L46" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="L46" s="6" t="s">
+      <c r="M46" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>130</v>
       </c>
@@ -2182,15 +2333,18 @@
       <c r="H47" s="1">
         <v>-1</v>
       </c>
-      <c r="I47" t="s">
+      <c r="I47" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J47" t="s">
         <v>112</v>
       </c>
-      <c r="J47" t="s">
+      <c r="K47" t="s">
         <v>109</v>
       </c>
-      <c r="K47"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L47"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>131</v>
       </c>
@@ -2208,15 +2362,18 @@
       <c r="H48" s="1">
         <v>-1</v>
       </c>
-      <c r="I48" t="s">
+      <c r="I48" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J48" t="s">
         <v>112</v>
       </c>
-      <c r="J48" t="s">
+      <c r="K48" t="s">
         <v>109</v>
       </c>
-      <c r="K48"/>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>152</v>
       </c>
@@ -2231,15 +2388,18 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I49" t="s">
+      <c r="I49" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="J49" t="s">
         <v>153</v>
       </c>
-      <c r="J49" t="s">
+      <c r="K49" t="s">
         <v>109</v>
       </c>
-      <c r="K49"/>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49"/>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>154</v>
       </c>
@@ -2260,17 +2420,20 @@
       <c r="H50" s="1">
         <v>1</v>
       </c>
-      <c r="I50" t="s">
+      <c r="I50" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="J50" t="s">
         <v>153</v>
       </c>
-      <c r="J50" t="s">
+      <c r="K50" t="s">
         <v>109</v>
       </c>
-      <c r="K50" t="s">
+      <c r="L50" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -2285,19 +2448,22 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="I51" t="s">
+      <c r="I51" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="J51" t="s">
         <v>114</v>
       </c>
-      <c r="J51" t="s">
+      <c r="K51" t="s">
         <v>109</v>
       </c>
-      <c r="K51" s="6" t="s">
+      <c r="L51" s="6" t="s">
         <v>125</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:L41">
-    <sortCondition ref="J2:J41"/>
+  <sortState ref="A2:M41">
+    <sortCondition ref="K2:K41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>

</xml_diff>

<commit_message>
Balance pass after playtest with Kelly
* Wrote tons of snarks - now every card has a snark
* Got rid of Golden Boots and Saw - never really bought them partly because I don't want to think about those bonuses
* Crossbow and Windmill can also be trashed to reorder again, which makes them quite powerful.
* Extra Pendant to help the Gold path and help
* LOTS of "May also be purchased for..." bonuses throughout. Helps out a lot of buying situations, and helps players essentially convert one resource to another for a cost (which then gets made up by those top-tier, single-resource purchases later)
* Added Barn - like a mini Obelisk with no gold
* New bonuses for top-tier cards
* Slight reduction on the number of "-2 X per turn" bonuses - not as great as they sound
* All premium purchases (e.g. Robot Golem, Galleon) have game-end bonuses, not in-game bonuses
*

Various other rewordings too.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="193">
   <si>
     <t>Name</t>
   </si>
@@ -127,27 +127,6 @@
     <t>mayan-pyramid</t>
   </si>
   <si>
-    <t>Golden Boots</t>
-  </si>
-  <si>
-    <t>boots</t>
-  </si>
-  <si>
-    <t>convert</t>
-  </si>
-  <si>
-    <t>Up to two Stone may be used for any resource</t>
-  </si>
-  <si>
-    <t>Golden Saw</t>
-  </si>
-  <si>
-    <t>bolt-saw</t>
-  </si>
-  <si>
-    <t>Up to two Wood may be used for any resource</t>
-  </si>
-  <si>
     <t>Ladder</t>
   </si>
   <si>
@@ -157,18 +136,12 @@
     <t>draw</t>
   </si>
   <si>
-    <t>Draw a card from your deck, if it contains  Wood, draw one more card.</t>
-  </si>
-  <si>
     <t>Magnet</t>
   </si>
   <si>
     <t>magnet</t>
   </si>
   <si>
-    <t>Draw a card from your deck, if it's contains Steel, draw one more card.</t>
-  </si>
-  <si>
     <t>Solid Spade</t>
   </si>
   <si>
@@ -271,12 +244,6 @@
     <t>How does smelting actually CREATE things?</t>
   </si>
   <si>
-    <t>Chains</t>
-  </si>
-  <si>
-    <t>wavy-chains</t>
-  </si>
-  <si>
     <t>Anvil</t>
   </si>
   <si>
@@ -289,9 +256,6 @@
     <t>robot-golem</t>
   </si>
   <si>
-    <t>-3 Steel on each Make.</t>
-  </si>
-  <si>
     <t>Rockslide</t>
   </si>
   <si>
@@ -328,9 +292,6 @@
     <t>stone-tower</t>
   </si>
   <si>
-    <t>1 Stone may be used for 1 of any Resource per turn</t>
-  </si>
-  <si>
     <t>Windmill</t>
   </si>
   <si>
@@ -346,9 +307,6 @@
     <t>crossbow</t>
   </si>
   <si>
-    <t>Wood Axe</t>
-  </si>
-  <si>
     <t>wood-axe</t>
   </si>
   <si>
@@ -379,9 +337,6 @@
     <t>small deck</t>
   </si>
   <si>
-    <t>At game end, 4 VP if your deck has 10 or fewer cards.</t>
-  </si>
-  <si>
     <t>Resource</t>
   </si>
   <si>
@@ -403,9 +358,6 @@
     <t>At game end, 1 VP per Wood in any cards except this one.</t>
   </si>
   <si>
-    <t>Upon purchase, you may reorder the cards on one row or column.</t>
-  </si>
-  <si>
     <t>May also be used for any 1 Resource.</t>
   </si>
   <si>
@@ -421,18 +373,6 @@
     <t>Medium Crate</t>
   </si>
   <si>
-    <t>Steel Axe</t>
-  </si>
-  <si>
-    <t>-1 Wood per turn</t>
-  </si>
-  <si>
-    <t>Can be purchased for 2 Steel</t>
-  </si>
-  <si>
-    <t>Can be purchased for 3 Steel</t>
-  </si>
-  <si>
     <t>gem-necklace</t>
   </si>
   <si>
@@ -442,18 +382,12 @@
     <t>crown</t>
   </si>
   <si>
-    <t>Woah, this really is heavy.</t>
-  </si>
-  <si>
     <t>Uzi</t>
   </si>
   <si>
     <t>uzi</t>
   </si>
   <si>
-    <t>Can be purchased for 4 Steel</t>
-  </si>
-  <si>
     <t>Battle Axe</t>
   </si>
   <si>
@@ -490,9 +424,6 @@
     <t>Wizard Staff</t>
   </si>
   <si>
-    <t>At game end, 1 VP per two Wood in any cards except this one.</t>
-  </si>
-  <si>
     <t>Boomerang</t>
   </si>
   <si>
@@ -515,6 +446,162 @@
   </si>
   <si>
     <t>VPtype</t>
+  </si>
+  <si>
+    <t>Can be purchased for 2 Gold</t>
+  </si>
+  <si>
+    <t>Can be purchased for 3 Gold</t>
+  </si>
+  <si>
+    <t>Draw a card from your deck. If it contains Steel, draw one more card.</t>
+  </si>
+  <si>
+    <t>Draw a card from your deck. If it contains Wood, draw one more card.</t>
+  </si>
+  <si>
+    <t>At game end, 3 VP if your deck has 10 or fewer cards.</t>
+  </si>
+  <si>
+    <t>At game end, 1 VP per card that contains Steel, including this one.</t>
+  </si>
+  <si>
+    <t>At game end, 1 VP for every three cards in deck</t>
+  </si>
+  <si>
+    <t>wizard-staff</t>
+  </si>
+  <si>
+    <t>At game end, 2 VP if deck contains 4 Wood besides this card.</t>
+  </si>
+  <si>
+    <t>May be purchased for 4 Steel or 3 Stone</t>
+  </si>
+  <si>
+    <t>We used the steel to collect the stones, duh!</t>
+  </si>
+  <si>
+    <t>May be purchased for 3 Steel</t>
+  </si>
+  <si>
+    <t>May be purchased for 2 Steel or 3 Wood</t>
+  </si>
+  <si>
+    <t>May be purchased for 3 Steel or 4 Wood</t>
+  </si>
+  <si>
+    <t>May be purchased for 4 Steel or 5 Wood</t>
+  </si>
+  <si>
+    <t>Stone Axe</t>
+  </si>
+  <si>
+    <t>Let's get started.</t>
+  </si>
+  <si>
+    <t>Let the wood times roll!</t>
+  </si>
+  <si>
+    <t>Just get out of the way of the flying shards.</t>
+  </si>
+  <si>
+    <t>This one messes up your small deck strategy.</t>
+  </si>
+  <si>
+    <t>To war!</t>
+  </si>
+  <si>
+    <t>Great for making decrees.</t>
+  </si>
+  <si>
+    <t>Just don't get tetanus.</t>
+  </si>
+  <si>
+    <t>Great for naps or eternal rest!</t>
+  </si>
+  <si>
+    <t>Are you ready for this kind of commitment?</t>
+  </si>
+  <si>
+    <t>Snag this while you can!</t>
+  </si>
+  <si>
+    <t>A good deal, indeed.</t>
+  </si>
+  <si>
+    <t>My money. Stay away.</t>
+  </si>
+  <si>
+    <t>A retirement plan you can drink from.</t>
+  </si>
+  <si>
+    <t>Woah, this really does make my head heavy.</t>
+  </si>
+  <si>
+    <t>Out of my way!</t>
+  </si>
+  <si>
+    <t>Also great for scaring people.</t>
+  </si>
+  <si>
+    <t>Everyone needs one of these.</t>
+  </si>
+  <si>
+    <t>A must have for the modern surivor.</t>
+  </si>
+  <si>
+    <t>Horseshoe</t>
+  </si>
+  <si>
+    <t>horseshoe</t>
+  </si>
+  <si>
+    <t>Gesundheit.</t>
+  </si>
+  <si>
+    <t>WARNING! Watch your thumbs.</t>
+  </si>
+  <si>
+    <t>Spray and pray.</t>
+  </si>
+  <si>
+    <t>May be purchased for 5 Steel or 6 Wood</t>
+  </si>
+  <si>
+    <t>Wait, when did this game get futuristic?!?!?</t>
+  </si>
+  <si>
+    <t>Make sure you use the pointy end.</t>
+  </si>
+  <si>
+    <t>You know, most people run from rockslides.</t>
+  </si>
+  <si>
+    <t>Obelisks and Turrets don't mix. Just sayin'.</t>
+  </si>
+  <si>
+    <t>Great for historical records until you drop them.</t>
+  </si>
+  <si>
+    <t>Sorry, no magical powers here.</t>
+  </si>
+  <si>
+    <t>Upon purchase, you may reorder cards on one row or column. May also be trashed to do the same.</t>
+  </si>
+  <si>
+    <t>Barn</t>
+  </si>
+  <si>
+    <t>barn</t>
+  </si>
+  <si>
+    <t>At game end, 1 VP if your deck has 10 or fewer cards.</t>
+  </si>
+  <si>
+    <t>Fun fact: not a good place to be born in.</t>
+  </si>
+  <si>
+    <t>May be purchased for 4 Steel or 2 Stone</t>
   </si>
 </sst>
 </file>
@@ -890,13 +977,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M51"/>
+  <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I1" sqref="I1"/>
+      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -943,7 +1030,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
@@ -973,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
@@ -1001,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -1010,11 +1097,13 @@
         <v>14</v>
       </c>
       <c r="L3"/>
-      <c r="M3"/>
+      <c r="M3" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
@@ -1027,7 +1116,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -1037,7 +1126,7 @@
       </c>
       <c r="L4"/>
       <c r="M4" t="s">
-        <v>128</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1055,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
@@ -1065,7 +1154,7 @@
       </c>
       <c r="L5"/>
       <c r="M5" s="6" t="s">
-        <v>15</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1082,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
@@ -1110,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
@@ -1119,10 +1208,10 @@
         <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>127</v>
+        <v>111</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1142,11 +1231,11 @@
         <v>1</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" ref="G8:G51" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
+        <f t="shared" ref="G8:G49" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
         <v>6</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>160</v>
+        <v>137</v>
       </c>
       <c r="J8" t="s">
         <v>27</v>
@@ -1156,6 +1245,9 @@
       </c>
       <c r="L8" t="s">
         <v>29</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1180,7 +1272,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="J9" t="s">
         <v>31</v>
@@ -1190,6 +1282,9 @@
       </c>
       <c r="L9" t="s">
         <v>29</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1213,7 +1308,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="J10" t="s">
         <v>33</v>
@@ -1223,6 +1318,9 @@
       </c>
       <c r="L10" t="s">
         <v>29</v>
+      </c>
+      <c r="M10" s="2" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1232,21 +1330,16 @@
       <c r="B11" s="9">
         <v>1</v>
       </c>
-      <c r="D11" s="9">
-        <v>1</v>
-      </c>
-      <c r="F11" s="9">
-        <v>1</v>
-      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="E11" s="10"/>
       <c r="G11" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H11" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="J11" t="s">
         <v>35</v>
@@ -1255,22 +1348,23 @@
         <v>36</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>37</v>
+        <v>144</v>
+      </c>
+      <c r="M11" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B12" s="9">
         <v>1</v>
       </c>
       <c r="D12" s="9">
-        <v>1</v>
-      </c>
-      <c r="F12" s="9">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E12" s="10"/>
       <c r="G12" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1279,56 +1373,69 @@
         <v>-1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="J12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K12" t="s">
         <v>36</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>40</v>
+        <v>143</v>
+      </c>
+      <c r="M12" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B13" s="9">
+        <v>1</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="G13" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H13" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="J13" t="s">
+        <v>40</v>
+      </c>
+      <c r="K13" t="s">
+        <v>36</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="9">
-        <v>1</v>
-      </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="E13" s="10"/>
-      <c r="G13" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="J13" t="s">
+      <c r="M13" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K13" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="M13"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B14" s="9">
         <v>1</v>
       </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
       <c r="D14" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E14" s="10"/>
       <c r="G14" s="9">
@@ -1339,27 +1446,29 @@
         <v>-1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="J14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K14" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="L14" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M14"/>
+        <v>41</v>
+      </c>
+      <c r="M14" s="6" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B15" s="9">
         <v>1</v>
       </c>
-      <c r="C15" s="9">
+      <c r="D15" s="9">
         <v>1</v>
       </c>
       <c r="E15" s="9">
@@ -1373,24 +1482,24 @@
         <v>-1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="J15" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K15" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="L15" s="6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>52</v>
+        <v>133</v>
       </c>
       <c r="B16" s="9">
         <v>1</v>
@@ -1398,343 +1507,361 @@
       <c r="C16" s="9">
         <v>1</v>
       </c>
-      <c r="D16" s="9">
-        <v>1</v>
-      </c>
-      <c r="E16" s="10"/>
       <c r="G16" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H16" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="J16" t="s">
-        <v>49</v>
+        <v>136</v>
       </c>
       <c r="K16" t="s">
-        <v>43</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>50</v>
+        <v>134</v>
+      </c>
+      <c r="L16" s="11" t="s">
+        <v>135</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>51</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="B17" s="9">
         <v>1</v>
       </c>
-      <c r="D17" s="9">
-        <v>1</v>
-      </c>
-      <c r="E17" s="9">
+      <c r="E17" s="10"/>
+      <c r="F17" s="9">
         <v>1</v>
       </c>
       <c r="G17" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H17" s="1">
-        <v>-1</v>
-      </c>
       <c r="I17" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="J17" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="M17" s="6" t="s">
         <v>49</v>
-      </c>
-      <c r="K17" t="s">
-        <v>43</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>156</v>
+        <v>123</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
       </c>
-      <c r="C18" s="9">
+      <c r="E18" s="10"/>
+      <c r="F18" s="9">
         <v>1</v>
       </c>
       <c r="G18" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="J18" t="s">
-        <v>159</v>
+        <v>124</v>
       </c>
       <c r="K18" t="s">
-        <v>157</v>
+        <v>47</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>158</v>
-      </c>
-      <c r="M18" s="6"/>
+        <v>125</v>
+      </c>
+      <c r="M18" s="6" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B19" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="H19" s="1">
+        <v>-2</v>
+      </c>
       <c r="I19" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="J19" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="K19" t="s">
-        <v>56</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>58</v>
+        <v>47</v>
+      </c>
+      <c r="L19" t="s">
+        <v>52</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>166</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>145</v>
+        <v>55</v>
       </c>
       <c r="B20" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G20" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="H20" s="1">
+        <v>-1</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="J20" t="s">
-        <v>146</v>
+        <v>116</v>
       </c>
       <c r="K20" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="L20" s="11" t="s">
-        <v>147</v>
-      </c>
-      <c r="M20" s="6"/>
+        <v>141</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B21" s="9">
         <v>1</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G21" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="H21" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="J21" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="K21" t="s">
-        <v>56</v>
-      </c>
-      <c r="L21" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="L21" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B22" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E22" s="10"/>
       <c r="F22" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H22" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="J22" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="K22" t="s">
-        <v>56</v>
-      </c>
-      <c r="L22" s="11" t="s">
-        <v>57</v>
+        <v>47</v>
+      </c>
+      <c r="L22"/>
+      <c r="M22" s="2" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G23" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="H23" s="1">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="J23" t="s">
-        <v>63</v>
+        <v>118</v>
       </c>
       <c r="K23" t="s">
-        <v>56</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
+      </c>
+      <c r="L23" s="6"/>
+      <c r="M23" s="2" t="s">
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
       </c>
+      <c r="C24" s="9">
+        <v>2</v>
+      </c>
       <c r="E24" s="10"/>
-      <c r="F24" s="9">
-        <v>5</v>
-      </c>
       <c r="G24" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>-2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="J24" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="K24" t="s">
-        <v>56</v>
-      </c>
-      <c r="L24"/>
+        <v>60</v>
+      </c>
+      <c r="L24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>171</v>
+      </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>137</v>
+        <v>62</v>
       </c>
       <c r="B25" s="9">
         <v>1</v>
       </c>
+      <c r="C25" s="9">
+        <v>2</v>
+      </c>
+      <c r="D25" s="9">
+        <v>2</v>
+      </c>
       <c r="E25" s="10"/>
-      <c r="F25" s="9">
-        <v>6</v>
-      </c>
       <c r="G25" s="9">
         <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="H25" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="J25" t="s">
-        <v>138</v>
+        <v>63</v>
       </c>
       <c r="K25" t="s">
-        <v>56</v>
-      </c>
-      <c r="L25" s="6"/>
+        <v>60</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="M25" s="2" t="s">
-        <v>139</v>
+        <v>172</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>67</v>
+        <v>188</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
       </c>
       <c r="C26" s="9">
-        <v>2</v>
-      </c>
-      <c r="E26" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1</v>
+      </c>
       <c r="G26" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H26" s="1">
-        <v>-1</v>
+        <f t="shared" ref="G26" si="1">ROUND(C26*WoodVP+D26*SteelVP+E26*StoneVP+F26*GoldVP,0) + H26</f>
+        <v>4</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="J26" t="s">
-        <v>68</v>
+        <v>189</v>
       </c>
       <c r="K26" t="s">
-        <v>69</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="M26"/>
+        <v>103</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>101</v>
       </c>
       <c r="B27" s="9">
         <v>1</v>
@@ -1745,27 +1872,35 @@
       <c r="D27" s="9">
         <v>2</v>
       </c>
-      <c r="E27" s="10"/>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
       <c r="G27" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>161</v>
+        <v>138</v>
       </c>
       <c r="J27" t="s">
-        <v>72</v>
+        <v>102</v>
       </c>
       <c r="K27" t="s">
-        <v>69</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>73</v>
+        <v>103</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>115</v>
+        <v>65</v>
       </c>
       <c r="B28" s="9">
         <v>1</v>
@@ -1773,440 +1908,479 @@
       <c r="C28" s="9">
         <v>2</v>
       </c>
-      <c r="D28" s="9">
-        <v>2</v>
-      </c>
-      <c r="E28" s="9">
-        <v>1</v>
-      </c>
-      <c r="F28" s="9">
-        <v>1</v>
-      </c>
+      <c r="E28" s="10"/>
       <c r="G28" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="J28" t="s">
-        <v>116</v>
+        <v>137</v>
+      </c>
+      <c r="J28" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="K28" t="s">
-        <v>117</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>118</v>
+        <v>67</v>
+      </c>
+      <c r="L28" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B29" s="9">
-        <v>2</v>
-      </c>
-      <c r="C29" s="9">
-        <v>2</v>
-      </c>
-      <c r="E29" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="E29" s="9">
+        <v>2</v>
+      </c>
       <c r="G29" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>75</v>
+        <v>138</v>
+      </c>
+      <c r="J29" t="s">
+        <v>70</v>
       </c>
       <c r="K29" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="M29"/>
+        <v>71</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>78</v>
+        <v>175</v>
       </c>
       <c r="B30" s="9">
-        <v>1</v>
-      </c>
-      <c r="E30" s="9">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D30" s="9">
+        <v>3</v>
+      </c>
+      <c r="E30" s="10"/>
       <c r="G30" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="J30" t="s">
-        <v>79</v>
+        <v>176</v>
       </c>
       <c r="K30" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="M30" s="6" t="s">
-        <v>81</v>
+        <v>153</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B31" s="9">
         <v>2</v>
       </c>
       <c r="D31" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="J31" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="K31" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>134</v>
+        <v>154</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>119</v>
       </c>
       <c r="B32" s="9">
         <v>1</v>
       </c>
       <c r="D32" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E32" s="10"/>
       <c r="G32" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="J32" t="s">
-        <v>85</v>
+        <v>120</v>
       </c>
       <c r="K32" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>135</v>
+        <v>155</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>140</v>
+        <v>121</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
       </c>
       <c r="D33" s="9">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="E33" s="10"/>
       <c r="G33" s="9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="J33" t="s">
-        <v>141</v>
+        <v>122</v>
       </c>
       <c r="K33" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>142</v>
+        <v>180</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>143</v>
+        <v>75</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
       </c>
       <c r="D34" s="9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E34" s="10"/>
       <c r="G34" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H34" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="J34" t="s">
-        <v>144</v>
+        <v>76</v>
       </c>
       <c r="K34" t="s">
-        <v>76</v>
-      </c>
-      <c r="L34" s="6"/>
+        <v>67</v>
+      </c>
+      <c r="L34" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B35" s="9">
         <v>1</v>
       </c>
-      <c r="D35" s="9">
-        <v>7</v>
-      </c>
-      <c r="E35" s="10"/>
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
       <c r="G35" s="9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="J35" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="K35" t="s">
-        <v>76</v>
-      </c>
-      <c r="L35" s="6" t="s">
-        <v>88</v>
+        <v>79</v>
+      </c>
+      <c r="L35" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
       </c>
-      <c r="C36" s="9">
-        <v>1</v>
-      </c>
-      <c r="E36" s="9">
-        <v>1</v>
+      <c r="D36" s="9">
+        <v>2</v>
       </c>
       <c r="G36" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="J36" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="K36" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="L36" s="11" t="s">
-        <v>123</v>
+        <v>108</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="B37" s="9">
         <v>1</v>
       </c>
-      <c r="D37" s="9">
+      <c r="C37" s="9">
+        <v>2</v>
+      </c>
+      <c r="E37" s="10"/>
+      <c r="G37" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G37" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
       <c r="I37" s="1" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="J37" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="K37" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="L37" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="M37"/>
+        <v>108</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="B38" s="9">
-        <v>1</v>
-      </c>
-      <c r="C38" s="9">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D38" s="9">
+        <v>2</v>
       </c>
       <c r="E38" s="10"/>
       <c r="G38" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="J38" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="K38" t="s">
-        <v>91</v>
-      </c>
-      <c r="L38" s="11" t="s">
-        <v>123</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="L38" s="11"/>
       <c r="M38" s="6" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>85</v>
       </c>
       <c r="B39" s="9">
         <v>2</v>
       </c>
-      <c r="D39" s="9">
-        <v>2</v>
-      </c>
-      <c r="E39" s="10"/>
+      <c r="E39" s="9">
+        <v>3</v>
+      </c>
       <c r="G39" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="H39" s="1">
+        <v>1</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="J39" t="s">
-        <v>149</v>
+        <v>86</v>
       </c>
       <c r="K39" t="s">
-        <v>91</v>
-      </c>
-      <c r="L39" s="11"/>
-      <c r="M39" s="6"/>
+        <v>79</v>
+      </c>
+      <c r="L39"/>
+      <c r="M39" s="2" t="s">
+        <v>185</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>97</v>
+        <v>129</v>
       </c>
       <c r="B40" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E40" s="9">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F40" s="9">
+        <v>2</v>
       </c>
       <c r="G40" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>8</v>
+      </c>
+      <c r="H40" s="1">
+        <v>1</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="J40" t="s">
-        <v>98</v>
+        <v>128</v>
       </c>
       <c r="K40" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="L40"/>
+      <c r="M40" s="2" t="s">
+        <v>186</v>
+      </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>151</v>
+        <v>87</v>
       </c>
       <c r="B41" s="9">
         <v>1</v>
       </c>
       <c r="E41" s="9">
-        <v>2</v>
-      </c>
-      <c r="F41" s="9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G41" s="9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="J41" t="s">
-        <v>150</v>
+        <v>88</v>
       </c>
       <c r="K41" t="s">
-        <v>91</v>
-      </c>
-      <c r="L41"/>
+        <v>79</v>
+      </c>
+      <c r="L41" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M41" s="2" t="s">
+        <v>184</v>
+      </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B42" s="9">
         <v>1</v>
       </c>
-      <c r="E42" s="9">
-        <v>6</v>
-      </c>
+      <c r="C42" s="9">
+        <v>2</v>
+      </c>
+      <c r="D42" s="9">
+        <v>1</v>
+      </c>
+      <c r="E42" s="10"/>
       <c r="G42" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="J42" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K42" t="s">
         <v>91</v>
       </c>
-      <c r="L42" s="6" t="s">
-        <v>101</v>
+      <c r="L42" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B43" s="9">
         <v>1</v>
       </c>
       <c r="C43" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D43" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" s="10"/>
       <c r="G43" s="9">
@@ -2214,105 +2388,106 @@
         <v>4</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>162</v>
+        <v>137</v>
       </c>
       <c r="J43" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="K43" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="L43" t="s">
-        <v>126</v>
+        <v>187</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>156</v>
       </c>
       <c r="B44" s="9">
         <v>1</v>
       </c>
-      <c r="C44" s="9">
-        <v>1</v>
-      </c>
-      <c r="D44" s="9">
-        <v>2</v>
-      </c>
-      <c r="E44" s="10"/>
+      <c r="E44" s="9">
+        <v>1</v>
+      </c>
       <c r="G44" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="J44" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="K44" t="s">
-        <v>104</v>
-      </c>
-      <c r="L44" t="s">
-        <v>126</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="M44" s="6"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
       <c r="B45" s="9">
         <v>2</v>
       </c>
-      <c r="D45" s="9">
-        <v>1</v>
+      <c r="C45" s="9">
+        <v>3</v>
       </c>
       <c r="E45" s="10"/>
       <c r="G45" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="H45" s="1">
+        <v>-1</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="J45" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K45" t="s">
-        <v>109</v>
-      </c>
-      <c r="L45" s="11" t="s">
-        <v>133</v>
+        <v>95</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B46" s="9">
-        <v>1</v>
-      </c>
-      <c r="E46" s="9">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="C46" s="9">
+        <v>4</v>
+      </c>
+      <c r="E46" s="10"/>
       <c r="G46" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="H46" s="1">
+        <v>-1</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="J46" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="K46" t="s">
-        <v>109</v>
-      </c>
-      <c r="L46" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M46" s="6" t="s">
-        <v>111</v>
+        <v>95</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
@@ -2323,142 +2498,86 @@
         <v>2</v>
       </c>
       <c r="C47" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E47" s="10"/>
       <c r="G47" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H47" s="1">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>160</v>
+        <v>139</v>
       </c>
       <c r="J47" t="s">
-        <v>112</v>
+        <v>131</v>
       </c>
       <c r="K47" t="s">
-        <v>109</v>
-      </c>
-      <c r="L47"/>
+        <v>95</v>
+      </c>
+      <c r="L47" s="2" t="s">
+        <v>150</v>
+      </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B48" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" s="9">
         <v>4</v>
       </c>
       <c r="E48" s="10"/>
+      <c r="F48" s="9">
+        <v>1</v>
+      </c>
       <c r="G48" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H48" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>161</v>
+        <v>137</v>
       </c>
       <c r="J48" t="s">
-        <v>112</v>
+        <v>148</v>
       </c>
       <c r="K48" t="s">
-        <v>109</v>
-      </c>
-      <c r="L48"/>
+        <v>95</v>
+      </c>
+      <c r="L48" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>152</v>
+        <v>99</v>
       </c>
       <c r="B49" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C49" s="9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E49" s="10"/>
       <c r="G49" s="9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="J49" t="s">
-        <v>153</v>
+        <v>100</v>
       </c>
       <c r="K49" t="s">
-        <v>109</v>
-      </c>
-      <c r="L49"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>154</v>
-      </c>
-      <c r="B50" s="9">
-        <v>1</v>
-      </c>
-      <c r="C50" s="9">
-        <v>4</v>
-      </c>
-      <c r="E50" s="10"/>
-      <c r="F50" s="9">
-        <v>1</v>
-      </c>
-      <c r="G50" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H50" s="1">
-        <v>1</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="J50" t="s">
-        <v>153</v>
-      </c>
-      <c r="K50" t="s">
-        <v>109</v>
-      </c>
-      <c r="L50" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>113</v>
-      </c>
-      <c r="B51" s="9">
-        <v>1</v>
-      </c>
-      <c r="C51" s="9">
-        <v>7</v>
-      </c>
-      <c r="E51" s="10"/>
-      <c r="G51" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="J51" t="s">
-        <v>114</v>
-      </c>
-      <c r="K51" t="s">
-        <v>109</v>
-      </c>
-      <c r="L51" s="6" t="s">
-        <v>125</v>
+        <v>95</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>
@@ -2487,10 +2606,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2549,13 +2668,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>119</v>
+        <v>104</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>121</v>
+        <v>106</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>122</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2563,11 +2682,11 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <f>COUNTA(Deck!C2:C111)</f>
-        <v>21</v>
+        <f>COUNTA(Deck!C2:C109)</f>
+        <v>22</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(Deck!C2:C110)</f>
+        <f>SUM(Deck!C2:C108)</f>
         <v>49</v>
       </c>
     </row>
@@ -2576,12 +2695,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <f>COUNTA(Deck!D2:D111)</f>
-        <v>21</v>
+        <f>COUNTA(Deck!D2:D109)</f>
+        <v>19</v>
       </c>
       <c r="C3" s="1">
-        <f>SUM(Deck!D2:D110)</f>
-        <v>50</v>
+        <f>SUM(Deck!D2:D108)</f>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2589,12 +2708,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <f>COUNTA(Deck!E2:E111)</f>
-        <v>12</v>
+        <f>COUNTA(Deck!E2:E109)</f>
+        <v>13</v>
       </c>
       <c r="C4" s="1">
-        <f>SUM(Deck!E2:E110)</f>
-        <v>21</v>
+        <f>SUM(Deck!E2:E108)</f>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2602,12 +2721,12 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <f>COUNTA(Deck!F2:F111)</f>
-        <v>16</v>
+        <f>COUNTA(Deck!F2:F109)</f>
+        <v>14</v>
       </c>
       <c r="C5" s="1">
-        <f>SUM(Deck!F2:F111)</f>
-        <v>32</v>
+        <f>SUM(Deck!F2:F109)</f>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Use +X VP for game end verbage
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -112,9 +112,6 @@
     <t>ancient</t>
   </si>
   <si>
-    <t>At game end, 2 VP for two Ancient artifacts, and 4 VP for three Ancient artifacts</t>
-  </si>
-  <si>
     <t>Ancient Armor</t>
   </si>
   <si>
@@ -355,9 +352,6 @@
     <t>Rusted Gears</t>
   </si>
   <si>
-    <t>At game end, 1 VP per Wood in any cards except this one.</t>
-  </si>
-  <si>
     <t>May also be used for any 1 Resource.</t>
   </si>
   <si>
@@ -460,21 +454,12 @@
     <t>Draw a card from your deck. If it contains Wood, draw one more card.</t>
   </si>
   <si>
-    <t>At game end, 3 VP if your deck has 10 or fewer cards.</t>
-  </si>
-  <si>
-    <t>At game end, 1 VP per card that contains Steel, including this one.</t>
-  </si>
-  <si>
     <t>At game end, 1 VP for every three cards in deck</t>
   </si>
   <si>
     <t>wizard-staff</t>
   </si>
   <si>
-    <t>At game end, 2 VP if deck contains 4 Wood besides this card.</t>
-  </si>
-  <si>
     <t>May be purchased for 4 Steel or 3 Stone</t>
   </si>
   <si>
@@ -595,13 +580,28 @@
     <t>barn</t>
   </si>
   <si>
-    <t>At game end, 1 VP if your deck has 10 or fewer cards.</t>
-  </si>
-  <si>
     <t>Fun fact: not a good place to be born in.</t>
   </si>
   <si>
     <t>May be purchased for 4 Steel or 2 Stone</t>
+  </si>
+  <si>
+    <t>At game end, +2 VP if deck contains 4 Wood besides this card.</t>
+  </si>
+  <si>
+    <t>At game end, +1 VP per Wood in any cards except this one.</t>
+  </si>
+  <si>
+    <t>At game end, +1 VP per card that contains Steel, including this one.</t>
+  </si>
+  <si>
+    <t>At game end, +3 VP if your deck has 10 or fewer cards.</t>
+  </si>
+  <si>
+    <t>At game end, +1 VP if your deck has 10 or fewer cards.</t>
+  </si>
+  <si>
+    <t>At game end, +2 VP for two Ancient artifacts, and +4 VP for three Ancient artifacts</t>
   </si>
 </sst>
 </file>
@@ -980,10 +980,10 @@
   <dimension ref="A1:M49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B15" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A49" sqref="A49"/>
+      <selection pane="bottomRight" activeCell="L46" sqref="L46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1030,7 +1030,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
@@ -1060,7 +1060,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
@@ -1088,7 +1088,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -1098,12 +1098,12 @@
       </c>
       <c r="L3"/>
       <c r="M3" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
@@ -1116,7 +1116,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="L4"/>
       <c r="M4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1144,7 +1144,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
@@ -1154,7 +1154,7 @@
       </c>
       <c r="L5"/>
       <c r="M5" s="6" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1171,7 +1171,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
@@ -1199,7 +1199,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
@@ -1208,10 +1208,10 @@
         <v>14</v>
       </c>
       <c r="L7" t="s">
+        <v>109</v>
+      </c>
+      <c r="M7" s="6" t="s">
         <v>111</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1235,7 +1235,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J8" t="s">
         <v>27</v>
@@ -1244,15 +1244,15 @@
         <v>28</v>
       </c>
       <c r="L8" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B9" s="9">
         <v>1</v>
@@ -1272,60 +1272,60 @@
         <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K9" t="s">
         <v>28</v>
       </c>
       <c r="L9" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J10" t="s">
         <v>32</v>
-      </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J10" t="s">
-        <v>33</v>
       </c>
       <c r="K10" t="s">
         <v>28</v>
       </c>
       <c r="L10" t="s">
-        <v>29</v>
+        <v>192</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B11" s="9">
         <v>1</v>
@@ -1339,24 +1339,24 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" t="s">
         <v>35</v>
       </c>
-      <c r="K11" t="s">
-        <v>36</v>
-      </c>
       <c r="L11" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="M11" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B12" s="9">
         <v>1</v>
@@ -1373,24 +1373,24 @@
         <v>-1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M12" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="9">
         <v>1</v>
@@ -1409,24 +1409,24 @@
         <v>-1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K13" t="s">
-        <v>36</v>
-      </c>
-      <c r="L13" s="6" t="s">
+      <c r="M13" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B14" s="9">
         <v>1</v>
@@ -1446,24 +1446,24 @@
         <v>-1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J14" t="s">
+        <v>39</v>
+      </c>
+      <c r="K14" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K14" t="s">
-        <v>36</v>
-      </c>
-      <c r="L14" s="6" t="s">
+      <c r="M14" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B15" s="9">
         <v>1</v>
@@ -1482,54 +1482,54 @@
         <v>-1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J15" t="s">
+        <v>39</v>
+      </c>
+      <c r="K15" t="s">
+        <v>35</v>
+      </c>
+      <c r="L15" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="K15" t="s">
-        <v>36</v>
-      </c>
-      <c r="L15" s="6" t="s">
+      <c r="M15" s="6" t="s">
         <v>41</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J16" t="s">
+        <v>134</v>
+      </c>
+      <c r="K16" t="s">
+        <v>132</v>
+      </c>
+      <c r="L16" s="11" t="s">
         <v>133</v>
       </c>
-      <c r="B16" s="9">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J16" t="s">
-        <v>136</v>
-      </c>
-      <c r="K16" t="s">
-        <v>134</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>135</v>
-      </c>
       <c r="M16" s="6" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="9">
         <v>1</v>
@@ -1543,24 +1543,24 @@
         <v>2</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J17" t="s">
+        <v>45</v>
+      </c>
+      <c r="K17" t="s">
         <v>46</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="L17" s="6" t="s">
+      <c r="M17" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="M17" s="6" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
@@ -1574,24 +1574,24 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J18" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B19" s="9">
         <v>2</v>
@@ -1608,24 +1608,24 @@
         <v>-2</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J19" t="s">
+        <v>50</v>
+      </c>
+      <c r="K19" t="s">
+        <v>46</v>
+      </c>
+      <c r="L19" t="s">
         <v>51</v>
       </c>
-      <c r="K19" t="s">
-        <v>47</v>
-      </c>
-      <c r="L19" t="s">
-        <v>52</v>
-      </c>
       <c r="M19" s="2" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20" s="9">
         <v>2</v>
@@ -1642,24 +1642,24 @@
         <v>-1</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J20" t="s">
+        <v>114</v>
+      </c>
+      <c r="K20" t="s">
+        <v>46</v>
+      </c>
+      <c r="L20" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="J20" t="s">
-        <v>116</v>
-      </c>
-      <c r="K20" t="s">
-        <v>47</v>
-      </c>
-      <c r="L20" s="11" t="s">
-        <v>141</v>
-      </c>
       <c r="M20" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B21" s="9">
         <v>1</v>
@@ -1676,24 +1676,24 @@
         <v>-1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J21" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="K21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L21" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="9">
         <v>1</v>
@@ -1710,22 +1710,22 @@
         <v>1</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L22"/>
       <c r="M22" s="2" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
@@ -1742,22 +1742,22 @@
         <v>2</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J23" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K23" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L23" s="6"/>
       <c r="M23" s="2" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
@@ -1774,24 +1774,24 @@
         <v>-2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J24" t="s">
+        <v>58</v>
+      </c>
+      <c r="K24" t="s">
         <v>59</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L24" s="6" t="s">
-        <v>61</v>
-      </c>
       <c r="M24" s="2" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B25" s="9">
         <v>1</v>
@@ -1808,24 +1808,24 @@
         <v>5</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J25" t="s">
+        <v>62</v>
+      </c>
+      <c r="K25" t="s">
+        <v>59</v>
+      </c>
+      <c r="L25" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="K25" t="s">
-        <v>60</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>64</v>
-      </c>
       <c r="M25" s="2" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
@@ -1844,63 +1844,63 @@
         <v>4</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J26" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="K26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="L26" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9">
+        <v>2</v>
+      </c>
+      <c r="D27" s="9">
+        <v>2</v>
+      </c>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J27" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="9">
-        <v>1</v>
-      </c>
-      <c r="C27" s="9">
-        <v>2</v>
-      </c>
-      <c r="D27" s="9">
-        <v>2</v>
-      </c>
-      <c r="E27" s="9">
-        <v>1</v>
-      </c>
-      <c r="F27" s="9">
-        <v>1</v>
-      </c>
-      <c r="G27" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J27" t="s">
+      <c r="K27" t="s">
         <v>102</v>
       </c>
-      <c r="K27" t="s">
-        <v>103</v>
-      </c>
       <c r="L27" s="2" t="s">
-        <v>145</v>
+        <v>190</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B28" s="9">
         <v>1</v>
@@ -1914,54 +1914,54 @@
         <v>3</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J28" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K28" t="s">
         <v>66</v>
       </c>
-      <c r="K28" t="s">
+      <c r="L28" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="L28" s="6" t="s">
-        <v>68</v>
-      </c>
       <c r="M28" s="2" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+      <c r="E29" s="9">
+        <v>2</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J29" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="9">
-        <v>1</v>
-      </c>
-      <c r="E29" s="9">
-        <v>2</v>
-      </c>
-      <c r="G29" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J29" t="s">
+      <c r="K29" t="s">
+        <v>66</v>
+      </c>
+      <c r="L29" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="K29" t="s">
-        <v>67</v>
-      </c>
-      <c r="L29" s="6" t="s">
+      <c r="M29" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B30" s="9">
         <v>2</v>
@@ -1975,24 +1975,24 @@
         <v>4</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J30" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="K30" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="9">
         <v>2</v>
@@ -2006,24 +2006,24 @@
         <v>6</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="K31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B32" s="9">
         <v>1</v>
@@ -2040,24 +2040,24 @@
         <v>1</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J32" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K32" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
@@ -2074,24 +2074,24 @@
         <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J33" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="K33" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
@@ -2105,87 +2105,87 @@
         <v>10</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J34" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K34" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>146</v>
+        <v>189</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>82</v>
+      </c>
+      <c r="B35" s="9">
+        <v>1</v>
+      </c>
+      <c r="C35" s="9">
+        <v>1</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J35" t="s">
         <v>83</v>
       </c>
-      <c r="B35" s="9">
-        <v>1</v>
-      </c>
-      <c r="C35" s="9">
-        <v>1</v>
-      </c>
-      <c r="E35" s="9">
-        <v>1</v>
-      </c>
-      <c r="G35" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="J35" t="s">
-        <v>84</v>
-      </c>
       <c r="K35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L35" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>76</v>
+      </c>
+      <c r="B36" s="9">
+        <v>1</v>
+      </c>
+      <c r="D36" s="9">
+        <v>2</v>
+      </c>
+      <c r="G36" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="J36" t="s">
         <v>77</v>
       </c>
-      <c r="B36" s="9">
-        <v>1</v>
-      </c>
-      <c r="D36" s="9">
-        <v>2</v>
-      </c>
-      <c r="G36" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="J36" t="s">
+      <c r="K36" t="s">
         <v>78</v>
       </c>
-      <c r="K36" t="s">
-        <v>79</v>
-      </c>
       <c r="L36" s="11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B37" s="9">
         <v>1</v>
@@ -2199,24 +2199,24 @@
         <v>3</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J37" t="s">
+        <v>80</v>
+      </c>
+      <c r="K37" t="s">
+        <v>78</v>
+      </c>
+      <c r="L37" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="M37" s="6" t="s">
         <v>81</v>
-      </c>
-      <c r="K37" t="s">
-        <v>79</v>
-      </c>
-      <c r="L37" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="M37" s="6" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B38" s="9">
         <v>2</v>
@@ -2230,22 +2230,22 @@
         <v>3</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J38" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="K38" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L38" s="11"/>
       <c r="M38" s="6" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B39" s="9">
         <v>2</v>
@@ -2261,22 +2261,22 @@
         <v>1</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J39" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="K39" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L39"/>
       <c r="M39" s="2" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B40" s="9">
         <v>1</v>
@@ -2295,22 +2295,22 @@
         <v>1</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J40" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="K40" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L40"/>
       <c r="M40" s="2" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B41" s="9">
         <v>1</v>
@@ -2323,24 +2323,24 @@
         <v>9</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J41" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K41" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="L41" s="6" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="M41" s="2" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B42" s="9">
         <v>1</v>
@@ -2357,21 +2357,21 @@
         <v>4</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J42" t="s">
+        <v>89</v>
+      </c>
+      <c r="K42" t="s">
         <v>90</v>
       </c>
-      <c r="K42" t="s">
-        <v>91</v>
-      </c>
       <c r="L42" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B43" s="9">
         <v>1</v>
@@ -2388,21 +2388,21 @@
         <v>4</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J43" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="L43" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B44" s="9">
         <v>1</v>
@@ -2415,22 +2415,22 @@
         <v>2</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J44" t="s">
+        <v>93</v>
+      </c>
+      <c r="K44" t="s">
         <v>94</v>
       </c>
-      <c r="K44" t="s">
+      <c r="L44" s="6" t="s">
         <v>95</v>
-      </c>
-      <c r="L44" s="6" t="s">
-        <v>96</v>
       </c>
       <c r="M44" s="6"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B45" s="9">
         <v>2</v>
@@ -2447,21 +2447,21 @@
         <v>-1</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J45" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L45" s="2" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B46" s="9">
         <v>2</v>
@@ -2478,21 +2478,21 @@
         <v>-1</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K46" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B47" s="9">
         <v>2</v>
@@ -2506,21 +2506,21 @@
         <v>7</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="J47" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="K47" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B48" s="9">
         <v>1</v>
@@ -2540,21 +2540,21 @@
         <v>1</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J48" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="K48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L48" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" s="9">
         <v>1</v>
@@ -2568,16 +2568,16 @@
         <v>9</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="J49" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K49" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="L49" s="6" t="s">
-        <v>110</v>
+        <v>188</v>
       </c>
     </row>
   </sheetData>
@@ -2606,10 +2606,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2668,13 +2668,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added Gold Mine, replacing one of the Pendants.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="197">
   <si>
     <t>Name</t>
   </si>
@@ -602,6 +602,18 @@
   </si>
   <si>
     <t>At game end, +2 VP for two Ancient artifacts, and +4 VP for three Ancient artifacts</t>
+  </si>
+  <si>
+    <t>Gold Mine</t>
+  </si>
+  <si>
+    <t>gold-mine</t>
+  </si>
+  <si>
+    <t>May also be purchased for 1 Wood, 1 Steel, and 1 Stone.</t>
+  </si>
+  <si>
+    <t>There's gold in them there hills!</t>
   </si>
 </sst>
 </file>
@@ -977,13 +989,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L46" sqref="L46"/>
+      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1231,7 +1243,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" ref="G8:G49" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
+        <f t="shared" ref="G8:G50" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
         <v>6</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -1594,7 +1606,7 @@
         <v>49</v>
       </c>
       <c r="B19" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E19" s="10"/>
       <c r="F19" s="9">
@@ -1625,75 +1637,72 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>193</v>
       </c>
       <c r="B20" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E20" s="10"/>
       <c r="F20" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G20" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H20" s="1">
-        <v>-1</v>
-      </c>
       <c r="I20" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J20" t="s">
-        <v>114</v>
+        <v>194</v>
       </c>
       <c r="K20" t="s">
         <v>46</v>
       </c>
-      <c r="L20" s="11" t="s">
-        <v>139</v>
+      <c r="L20" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>162</v>
+        <v>196</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B21" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E21" s="10"/>
       <c r="F21" s="9">
+        <v>3</v>
+      </c>
+      <c r="G21" s="9">
+        <f t="shared" si="0"/>
         <v>4</v>
-      </c>
-      <c r="G21" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
       <c r="H21" s="1">
         <v>-1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J21" t="s">
-        <v>53</v>
+        <v>114</v>
       </c>
       <c r="K21" t="s">
         <v>46</v>
       </c>
-      <c r="L21" s="6" t="s">
-        <v>140</v>
+      <c r="L21" s="11" t="s">
+        <v>139</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B22" s="9">
         <v>1</v>
@@ -1704,203 +1713,198 @@
       </c>
       <c r="G22" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H22" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J22" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="K22" t="s">
         <v>46</v>
       </c>
-      <c r="L22"/>
+      <c r="L22" s="6" t="s">
+        <v>140</v>
+      </c>
       <c r="M22" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>115</v>
+        <v>55</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
       </c>
       <c r="E23" s="10"/>
       <c r="F23" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G23" s="9">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H23" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J23" t="s">
-        <v>116</v>
+        <v>56</v>
       </c>
       <c r="K23" t="s">
         <v>46</v>
       </c>
-      <c r="L23" s="6"/>
+      <c r="L23"/>
       <c r="M23" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
       </c>
-      <c r="C24" s="9">
-        <v>2</v>
-      </c>
       <c r="E24" s="10"/>
+      <c r="F24" s="9">
+        <v>6</v>
+      </c>
       <c r="G24" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H24" s="1">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J24" t="s">
-        <v>58</v>
+        <v>116</v>
       </c>
       <c r="K24" t="s">
-        <v>59</v>
-      </c>
-      <c r="L24" s="6" t="s">
-        <v>60</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="L24" s="6"/>
       <c r="M24" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B25" s="9">
         <v>1</v>
       </c>
       <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="D25" s="9">
         <v>2</v>
       </c>
       <c r="E25" s="10"/>
       <c r="G25" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>-2</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="K25" t="s">
         <v>59</v>
       </c>
       <c r="L25" s="6" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>183</v>
+        <v>61</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
       </c>
       <c r="C26" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D26" s="9">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E26" s="10"/>
       <c r="G26" s="9">
-        <f t="shared" ref="G26" si="1">ROUND(C26*WoodVP+D26*SteelVP+E26*StoneVP+F26*GoldVP,0) + H26</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J26" t="s">
-        <v>184</v>
+        <v>62</v>
       </c>
       <c r="K26" t="s">
-        <v>102</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>191</v>
+        <v>59</v>
+      </c>
+      <c r="L26" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>100</v>
+        <v>183</v>
       </c>
       <c r="B27" s="9">
         <v>1</v>
       </c>
       <c r="C27" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D27" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E27" s="9">
         <v>1</v>
       </c>
-      <c r="F27" s="9">
-        <v>1</v>
-      </c>
       <c r="G27" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" ref="G27" si="1">ROUND(C27*WoodVP+D27*SteelVP+E27*StoneVP+F27*GoldVP,0) + H27</f>
+        <v>4</v>
       </c>
       <c r="I27" s="1" t="s">
         <v>136</v>
       </c>
       <c r="J27" t="s">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="K27" t="s">
         <v>102</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>169</v>
+        <v>185</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>64</v>
+        <v>100</v>
       </c>
       <c r="B28" s="9">
         <v>1</v>
@@ -1908,270 +1912,279 @@
       <c r="C28" s="9">
         <v>2</v>
       </c>
-      <c r="E28" s="10"/>
+      <c r="D28" s="9">
+        <v>2</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9">
+        <v>1</v>
+      </c>
       <c r="G28" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J28" s="7" t="s">
-        <v>65</v>
+        <v>136</v>
+      </c>
+      <c r="J28" t="s">
+        <v>101</v>
       </c>
       <c r="K28" t="s">
-        <v>66</v>
-      </c>
-      <c r="L28" s="6" t="s">
-        <v>67</v>
+        <v>102</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>190</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B29" s="9">
         <v>1</v>
       </c>
-      <c r="E29" s="9">
-        <v>2</v>
-      </c>
+      <c r="C29" s="9">
+        <v>2</v>
+      </c>
+      <c r="E29" s="10"/>
       <c r="G29" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J29" t="s">
-        <v>69</v>
+        <v>135</v>
+      </c>
+      <c r="J29" s="7" t="s">
+        <v>65</v>
       </c>
       <c r="K29" t="s">
         <v>66</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>170</v>
+        <v>68</v>
       </c>
       <c r="B30" s="9">
-        <v>2</v>
-      </c>
-      <c r="D30" s="9">
+        <v>1</v>
+      </c>
+      <c r="E30" s="9">
+        <v>2</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E30" s="10"/>
-      <c r="G30" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
       <c r="I30" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J30" t="s">
-        <v>171</v>
+        <v>69</v>
       </c>
       <c r="K30" t="s">
         <v>66</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>172</v>
+        <v>70</v>
+      </c>
+      <c r="M30" s="6" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>72</v>
+        <v>170</v>
       </c>
       <c r="B31" s="9">
         <v>2</v>
       </c>
       <c r="D31" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E31" s="10"/>
       <c r="G31" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J31" t="s">
-        <v>73</v>
+        <v>171</v>
       </c>
       <c r="K31" t="s">
         <v>66</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>117</v>
+        <v>72</v>
       </c>
       <c r="B32" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D32" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E32" s="10"/>
       <c r="G32" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H32" s="1">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J32" t="s">
-        <v>118</v>
+        <v>73</v>
       </c>
       <c r="K32" t="s">
         <v>66</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
       </c>
       <c r="D33" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E33" s="10"/>
       <c r="G33" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H33" s="1">
         <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J33" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="K33" t="s">
         <v>66</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>175</v>
+        <v>150</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>96</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>74</v>
+        <v>119</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
       </c>
       <c r="D34" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E34" s="10"/>
       <c r="G34" s="9">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="H34" s="1">
+        <v>1</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J34" t="s">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="K34" t="s">
         <v>66</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>176</v>
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="B35" s="9">
         <v>1</v>
       </c>
-      <c r="C35" s="9">
-        <v>1</v>
-      </c>
-      <c r="E35" s="9">
-        <v>1</v>
-      </c>
+      <c r="D35" s="9">
+        <v>7</v>
+      </c>
+      <c r="E35" s="10"/>
       <c r="G35" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J35" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="K35" t="s">
-        <v>78</v>
-      </c>
-      <c r="L35" s="11" t="s">
-        <v>107</v>
+        <v>66</v>
+      </c>
+      <c r="L35" s="6" t="s">
+        <v>189</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
       </c>
-      <c r="D36" s="9">
-        <v>2</v>
+      <c r="C36" s="9">
+        <v>1</v>
+      </c>
+      <c r="E36" s="9">
+        <v>1</v>
       </c>
       <c r="G36" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J36" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
       <c r="K36" t="s">
         <v>78</v>
@@ -2180,29 +2193,28 @@
         <v>107</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B37" s="9">
         <v>1</v>
       </c>
-      <c r="C37" s="9">
-        <v>2</v>
-      </c>
-      <c r="E37" s="10"/>
+      <c r="D37" s="9">
+        <v>2</v>
+      </c>
       <c r="G37" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J37" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K37" t="s">
         <v>78</v>
@@ -2210,18 +2222,18 @@
       <c r="L37" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="M37" s="6" t="s">
-        <v>81</v>
+      <c r="M37" s="2" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>124</v>
+        <v>79</v>
       </c>
       <c r="B38" s="9">
-        <v>2</v>
-      </c>
-      <c r="D38" s="9">
+        <v>1</v>
+      </c>
+      <c r="C38" s="9">
         <v>2</v>
       </c>
       <c r="E38" s="10"/>
@@ -2230,157 +2242,157 @@
         <v>3</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J38" t="s">
-        <v>125</v>
+        <v>80</v>
       </c>
       <c r="K38" t="s">
         <v>78</v>
       </c>
-      <c r="L38" s="11"/>
+      <c r="L38" s="11" t="s">
+        <v>107</v>
+      </c>
       <c r="M38" s="6" t="s">
-        <v>146</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="B39" s="9">
         <v>2</v>
       </c>
-      <c r="E39" s="9">
+      <c r="D39" s="9">
+        <v>2</v>
+      </c>
+      <c r="E39" s="10"/>
+      <c r="G39" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G39" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H39" s="1">
-        <v>1</v>
-      </c>
       <c r="I39" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J39" t="s">
-        <v>85</v>
+        <v>125</v>
       </c>
       <c r="K39" t="s">
         <v>78</v>
       </c>
-      <c r="L39"/>
-      <c r="M39" s="2" t="s">
-        <v>180</v>
+      <c r="L39" s="11"/>
+      <c r="M39" s="6" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="B40" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E40" s="9">
-        <v>2</v>
-      </c>
-      <c r="F40" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G40" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H40" s="1">
         <v>1</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J40" t="s">
-        <v>126</v>
+        <v>85</v>
       </c>
       <c r="K40" t="s">
         <v>78</v>
       </c>
       <c r="L40"/>
       <c r="M40" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="B41" s="9">
         <v>1</v>
       </c>
       <c r="E41" s="9">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="F41" s="9">
+        <v>2</v>
       </c>
       <c r="G41" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="H41" s="1">
+        <v>1</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J41" t="s">
-        <v>87</v>
+        <v>126</v>
       </c>
       <c r="K41" t="s">
         <v>78</v>
       </c>
-      <c r="L41" s="6" t="s">
-        <v>143</v>
-      </c>
+      <c r="L41"/>
       <c r="M41" s="2" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B42" s="9">
         <v>1</v>
       </c>
-      <c r="C42" s="9">
-        <v>2</v>
-      </c>
-      <c r="D42" s="9">
-        <v>1</v>
-      </c>
-      <c r="E42" s="10"/>
+      <c r="E42" s="9">
+        <v>6</v>
+      </c>
       <c r="G42" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J42" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K42" t="s">
-        <v>90</v>
-      </c>
-      <c r="L42" t="s">
-        <v>182</v>
+        <v>78</v>
+      </c>
+      <c r="L42" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="M42" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B43" s="9">
         <v>1</v>
       </c>
       <c r="C43" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D43" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" s="10"/>
       <c r="G43" s="9">
@@ -2388,10 +2400,10 @@
         <v>4</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J43" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="K43" t="s">
         <v>90</v>
@@ -2402,83 +2414,83 @@
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>151</v>
+        <v>91</v>
       </c>
       <c r="B44" s="9">
         <v>1</v>
       </c>
-      <c r="E44" s="9">
-        <v>1</v>
-      </c>
+      <c r="C44" s="9">
+        <v>1</v>
+      </c>
+      <c r="D44" s="9">
+        <v>2</v>
+      </c>
+      <c r="E44" s="10"/>
       <c r="G44" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="J44" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="K44" t="s">
-        <v>94</v>
-      </c>
-      <c r="L44" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="M44" s="6"/>
+        <v>90</v>
+      </c>
+      <c r="L44" t="s">
+        <v>182</v>
+      </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="B45" s="9">
-        <v>2</v>
-      </c>
-      <c r="C45" s="9">
-        <v>3</v>
-      </c>
-      <c r="E45" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1</v>
+      </c>
       <c r="G45" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H45" s="1">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J45" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="K45" t="s">
         <v>94</v>
       </c>
-      <c r="L45" s="2" t="s">
-        <v>147</v>
-      </c>
+      <c r="L45" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="M45" s="6"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B46" s="9">
         <v>2</v>
       </c>
       <c r="C46" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E46" s="10"/>
       <c r="G46" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H46" s="1">
         <v>-1</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J46" t="s">
         <v>97</v>
@@ -2487,96 +2499,127 @@
         <v>94</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>186</v>
+        <v>147</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B47" s="9">
         <v>2</v>
       </c>
       <c r="C47" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E47" s="10"/>
       <c r="G47" s="9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="H47" s="1">
+        <v>-1</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J47" t="s">
-        <v>129</v>
+        <v>97</v>
       </c>
       <c r="K47" t="s">
         <v>94</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>145</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B48" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" s="9">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E48" s="10"/>
-      <c r="F48" s="9">
-        <v>1</v>
-      </c>
       <c r="G48" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H48" s="1">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="J48" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="K48" t="s">
         <v>94</v>
       </c>
-      <c r="L48" t="s">
-        <v>187</v>
+      <c r="L48" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>130</v>
       </c>
       <c r="B49" s="9">
         <v>1</v>
       </c>
       <c r="C49" s="9">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E49" s="10"/>
+      <c r="F49" s="9">
+        <v>1</v>
+      </c>
       <c r="G49" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
+      </c>
+      <c r="H49" s="1">
+        <v>1</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J49" t="s">
-        <v>99</v>
+        <v>144</v>
       </c>
       <c r="K49" t="s">
         <v>94</v>
       </c>
-      <c r="L49" s="6" t="s">
+      <c r="L49" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>98</v>
+      </c>
+      <c r="B50" s="9">
+        <v>1</v>
+      </c>
+      <c r="C50" s="9">
+        <v>7</v>
+      </c>
+      <c r="E50" s="10"/>
+      <c r="G50" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J50" t="s">
+        <v>99</v>
+      </c>
+      <c r="K50" t="s">
+        <v>94</v>
+      </c>
+      <c r="L50" s="6" t="s">
         <v>188</v>
       </c>
     </row>
@@ -2682,11 +2725,11 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <f>COUNTA(Deck!C2:C109)</f>
+        <f>COUNTA(Deck!C2:C110)</f>
         <v>22</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(Deck!C2:C108)</f>
+        <f>SUM(Deck!C2:C109)</f>
         <v>49</v>
       </c>
     </row>
@@ -2695,11 +2738,11 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <f>COUNTA(Deck!D2:D109)</f>
+        <f>COUNTA(Deck!D2:D110)</f>
         <v>19</v>
       </c>
       <c r="C3" s="1">
-        <f>SUM(Deck!D2:D108)</f>
+        <f>SUM(Deck!D2:D109)</f>
         <v>48</v>
       </c>
     </row>
@@ -2708,11 +2751,11 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <f>COUNTA(Deck!E2:E109)</f>
+        <f>COUNTA(Deck!E2:E110)</f>
         <v>13</v>
       </c>
       <c r="C4" s="1">
-        <f>SUM(Deck!E2:E108)</f>
+        <f>SUM(Deck!E2:E109)</f>
         <v>22</v>
       </c>
     </row>
@@ -2721,12 +2764,12 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <f>COUNTA(Deck!F2:F109)</f>
-        <v>14</v>
+        <f>COUNTA(Deck!F2:F110)</f>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
-        <f>SUM(Deck!F2:F109)</f>
-        <v>29</v>
+        <f>SUM(Deck!F2:F110)</f>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Windmill and Crossbow become Colony Ships
The re-ordering takes too long for players, and leads to analysis paralysis.

Instead, let's make these guys about building more cards. What you spend is the time and gamble to get the right card.

Adjust the VP downward so these are more likely to go away since the bonus is pretty powerful.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -295,9 +295,6 @@
     <t>windmill</t>
   </si>
   <si>
-    <t>swap</t>
-  </si>
-  <si>
     <t>Crossbow</t>
   </si>
   <si>
@@ -571,9 +568,6 @@
     <t>Sorry, no magical powers here.</t>
   </si>
   <si>
-    <t>Upon purchase, you may reorder cards on one row or column. May also be trashed to do the same.</t>
-  </si>
-  <si>
     <t>Barn</t>
   </si>
   <si>
@@ -614,6 +608,12 @@
   </si>
   <si>
     <t>There's gold in them there hills!</t>
+  </si>
+  <si>
+    <t>build</t>
+  </si>
+  <si>
+    <t>When played, trash this card to build any available blueprint for free.</t>
   </si>
 </sst>
 </file>
@@ -992,10 +992,10 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M20" sqref="M20"/>
+      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J1" s="3" t="s">
         <v>8</v>
@@ -1072,7 +1072,7 @@
         <v>0</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J2" t="s">
         <v>13</v>
@@ -1100,7 +1100,7 @@
         <v>0</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J3" t="s">
         <v>17</v>
@@ -1110,12 +1110,12 @@
       </c>
       <c r="L3"/>
       <c r="M3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
@@ -1128,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
@@ -1138,7 +1138,7 @@
       </c>
       <c r="L4"/>
       <c r="M4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1156,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J5" t="s">
         <v>20</v>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="L5"/>
       <c r="M5" s="6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1183,7 +1183,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J6" t="s">
         <v>22</v>
@@ -1211,7 +1211,7 @@
         <v>0</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J7" t="s">
         <v>25</v>
@@ -1220,10 +1220,10 @@
         <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1247,7 +1247,7 @@
         <v>6</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J8" t="s">
         <v>27</v>
@@ -1256,10 +1256,10 @@
         <v>28</v>
       </c>
       <c r="L8" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1284,7 +1284,7 @@
         <v>6</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J9" t="s">
         <v>30</v>
@@ -1293,10 +1293,10 @@
         <v>28</v>
       </c>
       <c r="L9" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1320,7 +1320,7 @@
         <v>6</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J10" t="s">
         <v>32</v>
@@ -1329,10 +1329,10 @@
         <v>28</v>
       </c>
       <c r="L10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1351,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J11" t="s">
         <v>34</v>
@@ -1360,10 +1360,10 @@
         <v>35</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1385,7 +1385,7 @@
         <v>-1</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J12" t="s">
         <v>37</v>
@@ -1394,10 +1394,10 @@
         <v>35</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="M12" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -1421,7 +1421,7 @@
         <v>-1</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J13" t="s">
         <v>39</v>
@@ -1458,7 +1458,7 @@
         <v>-1</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J14" t="s">
         <v>39</v>
@@ -1494,7 +1494,7 @@
         <v>-1</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J15" t="s">
         <v>39</v>
@@ -1511,32 +1511,32 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>130</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J16" t="s">
+        <v>133</v>
+      </c>
+      <c r="K16" t="s">
         <v>131</v>
       </c>
-      <c r="B16" s="9">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J16" t="s">
-        <v>134</v>
-      </c>
-      <c r="K16" t="s">
+      <c r="L16" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="L16" s="11" t="s">
-        <v>133</v>
-      </c>
       <c r="M16" s="6" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
@@ -1555,7 +1555,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J17" t="s">
         <v>45</v>
@@ -1572,7 +1572,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
@@ -1586,19 +1586,19 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="K18" t="s">
         <v>46</v>
       </c>
       <c r="L18" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
@@ -1620,7 +1620,7 @@
         <v>-2</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J19" t="s">
         <v>50</v>
@@ -1632,12 +1632,12 @@
         <v>51</v>
       </c>
       <c r="M19" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B20" s="9">
         <v>1</v>
@@ -1651,19 +1651,19 @@
         <v>4</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J20" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="K20" t="s">
         <v>46</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
@@ -1685,19 +1685,19 @@
         <v>-1</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J21" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="K21" t="s">
         <v>46</v>
       </c>
       <c r="L21" s="11" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1719,7 +1719,7 @@
         <v>-1</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J22" t="s">
         <v>53</v>
@@ -1728,10 +1728,10 @@
         <v>46</v>
       </c>
       <c r="L22" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
@@ -1753,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J23" t="s">
         <v>56</v>
@@ -1763,12 +1763,12 @@
       </c>
       <c r="L23"/>
       <c r="M23" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
@@ -1785,17 +1785,17 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J24" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="K24" t="s">
         <v>46</v>
       </c>
       <c r="L24" s="6"/>
       <c r="M24" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
@@ -1817,7 +1817,7 @@
         <v>-2</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J25" t="s">
         <v>58</v>
@@ -1829,7 +1829,7 @@
         <v>60</v>
       </c>
       <c r="M25" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
@@ -1851,7 +1851,7 @@
         <v>5</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J26" t="s">
         <v>62</v>
@@ -1863,12 +1863,12 @@
         <v>63</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B27" s="9">
         <v>1</v>
@@ -1887,58 +1887,58 @@
         <v>4</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J27" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="K27" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B28" s="9">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9">
+        <v>2</v>
+      </c>
+      <c r="D28" s="9">
+        <v>2</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9">
+        <v>1</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="J28" t="s">
         <v>100</v>
       </c>
-      <c r="B28" s="9">
-        <v>1</v>
-      </c>
-      <c r="C28" s="9">
-        <v>2</v>
-      </c>
-      <c r="D28" s="9">
-        <v>2</v>
-      </c>
-      <c r="E28" s="9">
-        <v>1</v>
-      </c>
-      <c r="F28" s="9">
-        <v>1</v>
-      </c>
-      <c r="G28" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J28" t="s">
+      <c r="K28" t="s">
         <v>101</v>
       </c>
-      <c r="K28" t="s">
-        <v>102</v>
-      </c>
       <c r="L28" s="2" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
@@ -1957,7 +1957,7 @@
         <v>3</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J29" s="7" t="s">
         <v>65</v>
@@ -1969,7 +1969,7 @@
         <v>67</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
@@ -1987,7 +1987,7 @@
         <v>3</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J30" t="s">
         <v>69</v>
@@ -2004,7 +2004,7 @@
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B31" s="9">
         <v>2</v>
@@ -2018,19 +2018,19 @@
         <v>4</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J31" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="K31" t="s">
         <v>66</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="M31" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
@@ -2049,7 +2049,7 @@
         <v>6</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J32" t="s">
         <v>73</v>
@@ -2058,15 +2058,15 @@
         <v>66</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
@@ -2083,24 +2083,24 @@
         <v>1</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J33" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="K33" t="s">
         <v>66</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
@@ -2117,19 +2117,19 @@
         <v>1</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J34" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="K34" t="s">
         <v>66</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
@@ -2148,7 +2148,7 @@
         <v>10</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J35" t="s">
         <v>75</v>
@@ -2157,10 +2157,10 @@
         <v>66</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
@@ -2181,7 +2181,7 @@
         <v>3</v>
       </c>
       <c r="I36" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J36" t="s">
         <v>83</v>
@@ -2190,10 +2190,10 @@
         <v>78</v>
       </c>
       <c r="L36" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
@@ -2211,7 +2211,7 @@
         <v>3</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J37" t="s">
         <v>77</v>
@@ -2220,10 +2220,10 @@
         <v>78</v>
       </c>
       <c r="L37" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
@@ -2242,7 +2242,7 @@
         <v>3</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J38" t="s">
         <v>80</v>
@@ -2251,7 +2251,7 @@
         <v>78</v>
       </c>
       <c r="L38" s="11" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="M38" s="6" t="s">
         <v>81</v>
@@ -2259,7 +2259,7 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B39" s="9">
         <v>2</v>
@@ -2273,17 +2273,17 @@
         <v>3</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="K39" t="s">
         <v>78</v>
       </c>
       <c r="L39" s="11"/>
       <c r="M39" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
@@ -2304,7 +2304,7 @@
         <v>1</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J40" t="s">
         <v>85</v>
@@ -2314,12 +2314,12 @@
       </c>
       <c r="L40"/>
       <c r="M40" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B41" s="9">
         <v>1</v>
@@ -2338,17 +2338,17 @@
         <v>1</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J41" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="K41" t="s">
         <v>78</v>
       </c>
       <c r="L41"/>
       <c r="M41" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -2366,7 +2366,7 @@
         <v>9</v>
       </c>
       <c r="I42" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J42" t="s">
         <v>87</v>
@@ -2375,10 +2375,10 @@
         <v>78</v>
       </c>
       <c r="L42" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="M42" s="2" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
@@ -2397,24 +2397,27 @@
       <c r="E43" s="10"/>
       <c r="G43" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="H43" s="1">
+        <v>-1</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J43" t="s">
         <v>89</v>
       </c>
       <c r="K43" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
       <c r="L43" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B44" s="9">
         <v>1</v>
@@ -2428,24 +2431,27 @@
       <c r="E44" s="10"/>
       <c r="G44" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
+      </c>
+      <c r="H44" s="1">
+        <v>-1</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J44" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K44" t="s">
-        <v>90</v>
+        <v>195</v>
       </c>
       <c r="L44" t="s">
-        <v>182</v>
+        <v>196</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B45" s="9">
         <v>1</v>
@@ -2458,22 +2464,22 @@
         <v>2</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J45" t="s">
+        <v>92</v>
+      </c>
+      <c r="K45" t="s">
         <v>93</v>
       </c>
-      <c r="K45" t="s">
+      <c r="L45" s="6" t="s">
         <v>94</v>
-      </c>
-      <c r="L45" s="6" t="s">
-        <v>95</v>
       </c>
       <c r="M45" s="6"/>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B46" s="9">
         <v>2</v>
@@ -2490,21 +2496,21 @@
         <v>-1</v>
       </c>
       <c r="I46" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K46" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L46" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B47" s="9">
         <v>2</v>
@@ -2521,21 +2527,21 @@
         <v>-1</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J47" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="K47" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L47" s="2" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B48" s="9">
         <v>2</v>
@@ -2549,21 +2555,21 @@
         <v>7</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J48" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K48" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L48" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B49" s="9">
         <v>1</v>
@@ -2583,21 +2589,21 @@
         <v>1</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J49" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K49" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L49" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B50" s="9">
         <v>1</v>
@@ -2611,16 +2617,16 @@
         <v>9</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J50" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K50" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L50" s="6" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -2649,10 +2655,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2711,13 +2717,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Nerfing the Windmill+Crossbow to 6vp or less
Reasoning: really, this card is worth 4VP in resources before the adjustment.

So this card essentially buys you up to 2VP. Or lets you convert Wood+Steel to other things.

By making it >=5VP, this makes this useful for the entire game too.
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -613,7 +613,7 @@
     <t>build</t>
   </si>
   <si>
-    <t>When played, trash this card to build any available blueprint for free.</t>
+    <t>Trash this card to build any available blueprint worth 6 VP or less for free.</t>
   </si>
 </sst>
 </file>
@@ -992,10 +992,10 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H43" sqref="H43"/>
+      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
better instructions! and other stuff
* Better Guardfile
* New cards and icons
* Game-end stuff
* New fonts
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\project-spider-monkey\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
   </bookViews>
@@ -18,12 +23,12 @@
     <definedName name="WoodValue">VPs!$B$2</definedName>
     <definedName name="WoodVP">VPs!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="218">
   <si>
     <t>Name</t>
   </si>
@@ -166,9 +171,6 @@
     <t>gold path</t>
   </si>
   <si>
-    <t>-1 Gold per turn</t>
-  </si>
-  <si>
     <t>Shiny things! I like shiny things.</t>
   </si>
   <si>
@@ -178,9 +180,6 @@
     <t>gem-pendant</t>
   </si>
   <si>
-    <t>-2 Gold per turn</t>
-  </si>
-  <si>
     <t>War Chest</t>
   </si>
   <si>
@@ -226,18 +225,12 @@
     <t>steel path</t>
   </si>
   <si>
-    <t>-2 Steel per turn</t>
-  </si>
-  <si>
     <t>Smelter</t>
   </si>
   <si>
     <t>thrown-charcoal</t>
   </si>
   <si>
-    <t>-3 Steel per turn</t>
-  </si>
-  <si>
     <t>How does smelting actually CREATE things?</t>
   </si>
   <si>
@@ -307,9 +300,6 @@
     <t>wood path</t>
   </si>
   <si>
-    <t>-2 Wood per turn</t>
-  </si>
-  <si>
     <t>And my axe.</t>
   </si>
   <si>
@@ -343,9 +333,6 @@
     <t>Total Economy</t>
   </si>
   <si>
-    <t>-1 Stone per turn</t>
-  </si>
-  <si>
     <t>Rusted Gears</t>
   </si>
   <si>
@@ -391,9 +378,6 @@
     <t>key</t>
   </si>
   <si>
-    <t>-1 Gold to build items consisting only of Gold</t>
-  </si>
-  <si>
     <t>Stone Pile</t>
   </si>
   <si>
@@ -421,39 +405,15 @@
     <t>pass</t>
   </si>
   <si>
-    <t>-1 Wood for the current turn. At end of turn, pass to left and place in opponent's hand.</t>
-  </si>
-  <si>
     <t>boomerang</t>
   </si>
   <si>
-    <t>food</t>
-  </si>
-  <si>
-    <t>shelter</t>
-  </si>
-  <si>
-    <t>clothing</t>
-  </si>
-  <si>
-    <t>VPtype</t>
-  </si>
-  <si>
-    <t>Can be purchased for 2 Gold</t>
-  </si>
-  <si>
-    <t>Can be purchased for 3 Gold</t>
-  </si>
-  <si>
     <t>Draw a card from your deck. If it contains Steel, draw one more card.</t>
   </si>
   <si>
     <t>Draw a card from your deck. If it contains Wood, draw one more card.</t>
   </si>
   <si>
-    <t>At game end, 1 VP for every three cards in deck</t>
-  </si>
-  <si>
     <t>wizard-staff</t>
   </si>
   <si>
@@ -529,9 +489,6 @@
     <t>Everyone needs one of these.</t>
   </si>
   <si>
-    <t>A must have for the modern surivor.</t>
-  </si>
-  <si>
     <t>Horseshoe</t>
   </si>
   <si>
@@ -541,9 +498,6 @@
     <t>Gesundheit.</t>
   </si>
   <si>
-    <t>WARNING! Watch your thumbs.</t>
-  </si>
-  <si>
     <t>Spray and pray.</t>
   </si>
   <si>
@@ -580,24 +534,6 @@
     <t>May be purchased for 4 Steel or 2 Stone</t>
   </si>
   <si>
-    <t>At game end, +2 VP if deck contains 4 Wood besides this card.</t>
-  </si>
-  <si>
-    <t>At game end, +1 VP per Wood in any cards except this one.</t>
-  </si>
-  <si>
-    <t>At game end, +1 VP per card that contains Steel, including this one.</t>
-  </si>
-  <si>
-    <t>At game end, +3 VP if your deck has 10 or fewer cards.</t>
-  </si>
-  <si>
-    <t>At game end, +1 VP if your deck has 10 or fewer cards.</t>
-  </si>
-  <si>
-    <t>At game end, +2 VP for two Ancient artifacts, and +4 VP for three Ancient artifacts</t>
-  </si>
-  <si>
     <t>Gold Mine</t>
   </si>
   <si>
@@ -614,6 +550,138 @@
   </si>
   <si>
     <t>Trash this card to build any available blueprint worth 6 VP or less for free.</t>
+  </si>
+  <si>
+    <t>Save 1 Wood this turn. At end of this turn, pass to left and place in opponent's hand.</t>
+  </si>
+  <si>
+    <t>Save 1 Gold this turn</t>
+  </si>
+  <si>
+    <t>Save 1 Gold on items made only of Gold</t>
+  </si>
+  <si>
+    <t>Save 2 Gold this turn</t>
+  </si>
+  <si>
+    <t>May be be purchased for 2 Gold</t>
+  </si>
+  <si>
+    <t>May be purchased for 3 Gold</t>
+  </si>
+  <si>
+    <t>Save 2 Steel this turn</t>
+  </si>
+  <si>
+    <t>Save 3 Steel this turn</t>
+  </si>
+  <si>
+    <t>Save 1 Stone this turn</t>
+  </si>
+  <si>
+    <t>Save 2 Wood this turn</t>
+  </si>
+  <si>
+    <t>Draw a card from your deck. If it contains Wood or Steel, discard it.</t>
+  </si>
+  <si>
+    <t>Just the heavy stuff, please.</t>
+  </si>
+  <si>
+    <t>open-chest</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Stone Wheel</t>
+  </si>
+  <si>
+    <t>You can rebuild it, just don't reinvent it.</t>
+  </si>
+  <si>
+    <t>stone-wheel</t>
+  </si>
+  <si>
+    <t>pulley-hook</t>
+  </si>
+  <si>
+    <t>Watch your thumbs.</t>
+  </si>
+  <si>
+    <t>Pulley System</t>
+  </si>
+  <si>
+    <t>Simple machines always come in handy.</t>
+  </si>
+  <si>
+    <t>Windmill, or windfall??</t>
+  </si>
+  <si>
+    <t>We don't illustrate how a crossbow was used to accomplish this.</t>
+  </si>
+  <si>
+    <t>It's made of stone, but for wood.</t>
+  </si>
+  <si>
+    <t>Good for carrying stuff. If you can carry it.</t>
+  </si>
+  <si>
+    <t>Even better for carrying stuff.</t>
+  </si>
+  <si>
+    <t>This way!</t>
+  </si>
+  <si>
+    <t>Wizards have expensive taste.</t>
+  </si>
+  <si>
+    <t>The wood cost is just an estimate.</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>AtEnd</t>
+  </si>
+  <si>
+    <t>*At game end, +2 VP for two Ancient artifacts, and +4 VP for three Ancient artifacts</t>
+  </si>
+  <si>
+    <t>*At game end, +1 VP per card that contains Steel, including this one.</t>
+  </si>
+  <si>
+    <t>*At game end, +3 VP if you have two Stone Wheels (count this bonus once)</t>
+  </si>
+  <si>
+    <t>*At game end, 1 VP for every three cards in deck</t>
+  </si>
+  <si>
+    <t>*At game end, +2 VP if deck contains 4 Wood besides this card.</t>
+  </si>
+  <si>
+    <t>*At game end, +1 VP per Wood in any cards except this one.</t>
+  </si>
+  <si>
+    <t>You may build any card in any row this turn.</t>
+  </si>
+  <si>
+    <t>mechanical-arm</t>
+  </si>
+  <si>
+    <t>Robot Arm</t>
+  </si>
+  <si>
+    <t>The coding should be the easiest part.</t>
+  </si>
+  <si>
+    <t>*At game end, +3 VP if your deck and discard has 8 or fewer cards total.</t>
+  </si>
+  <si>
+    <t>*At game end, +1 VP if your deck and discard has 10 or fewer cards total.</t>
+  </si>
+  <si>
+    <t>A must-have for the modern surivor.</t>
   </si>
 </sst>
 </file>
@@ -657,7 +725,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -684,7 +752,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -697,6 +764,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -745,7 +815,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -780,7 +850,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -989,13 +1059,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M50"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L43" sqref="L43"/>
+      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,9 +1078,9 @@
     <col min="6" max="6" width="5.28515625" style="9"/>
     <col min="7" max="7" width="9.140625" style="9"/>
     <col min="8" max="8" width="6.140625" style="1"/>
-    <col min="9" max="9" width="9.140625" style="1"/>
-    <col min="10" max="10" width="14.85546875"/>
-    <col min="11" max="11" width="10.28515625"/>
+    <col min="9" max="9" width="14.85546875"/>
+    <col min="10" max="10" width="10.28515625"/>
+    <col min="11" max="11" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="73.5703125" style="2"/>
     <col min="13" max="13" width="40" style="2"/>
     <col min="14" max="1026" width="8.5703125"/>
@@ -1041,14 +1111,14 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
-        <v>137</v>
+      <c r="I1" s="3" t="s">
+        <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="3" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>204</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>10</v>
@@ -1062,22 +1132,18 @@
         <v>12</v>
       </c>
       <c r="B2" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C2" s="9">
         <v>1</v>
       </c>
-      <c r="E2" s="10"/>
       <c r="G2" s="9">
         <v>0</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>134</v>
+      <c r="I2" t="s">
+        <v>13</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K2" t="s">
         <v>14</v>
       </c>
       <c r="L2"/>
@@ -1090,55 +1156,47 @@
         <v>16</v>
       </c>
       <c r="B3" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C3" s="9">
         <v>2</v>
       </c>
-      <c r="E3" s="10"/>
       <c r="G3" s="9">
         <v>0</v>
       </c>
-      <c r="I3" s="1" t="s">
-        <v>134</v>
+      <c r="I3" t="s">
+        <v>17</v>
       </c>
       <c r="J3" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" t="s">
         <v>14</v>
       </c>
       <c r="L3"/>
       <c r="M3" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="B4" s="9">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D4" s="9">
         <v>3</v>
       </c>
-      <c r="E4" s="10"/>
       <c r="G4" s="9">
         <v>0</v>
       </c>
-      <c r="I4" s="1" t="s">
-        <v>135</v>
+      <c r="I4" t="s">
+        <v>18</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
-      </c>
-      <c r="K4" t="s">
         <v>14</v>
       </c>
       <c r="L4"/>
       <c r="M4" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1146,27 +1204,23 @@
         <v>19</v>
       </c>
       <c r="B5" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D5" s="9">
         <v>1</v>
       </c>
-      <c r="E5" s="10"/>
       <c r="G5" s="9">
         <v>0</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>135</v>
+      <c r="I5" t="s">
+        <v>20</v>
       </c>
       <c r="J5" t="s">
-        <v>20</v>
-      </c>
-      <c r="K5" t="s">
         <v>14</v>
       </c>
       <c r="L5"/>
       <c r="M5" s="6" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1174,7 +1228,7 @@
         <v>21</v>
       </c>
       <c r="B6" s="9">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="E6" s="9">
         <v>1</v>
@@ -1182,13 +1236,10 @@
       <c r="G6" s="9">
         <v>0</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>135</v>
+      <c r="I6" t="s">
+        <v>22</v>
       </c>
       <c r="J6" t="s">
-        <v>22</v>
-      </c>
-      <c r="K6" t="s">
         <v>14</v>
       </c>
       <c r="L6"/>
@@ -1201,29 +1252,25 @@
         <v>24</v>
       </c>
       <c r="B7" s="9">
-        <v>6</v>
-      </c>
-      <c r="E7" s="10"/>
+        <v>12</v>
+      </c>
       <c r="F7" s="9">
         <v>1</v>
       </c>
       <c r="G7" s="9">
         <v>0</v>
       </c>
-      <c r="I7" s="1" t="s">
-        <v>136</v>
+      <c r="I7" t="s">
+        <v>25</v>
       </c>
       <c r="J7" t="s">
-        <v>25</v>
-      </c>
-      <c r="K7" t="s">
         <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1243,23 +1290,23 @@
         <v>1</v>
       </c>
       <c r="G8" s="9">
-        <f t="shared" ref="G8:G50" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
+        <f t="shared" ref="G8:G54" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
         <v>6</v>
       </c>
-      <c r="I8" s="1" t="s">
-        <v>134</v>
+      <c r="I8" t="s">
+        <v>27</v>
       </c>
       <c r="J8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" t="s">
         <v>28</v>
       </c>
+      <c r="K8" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="L8" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1275,7 +1322,6 @@
       <c r="D9" s="9">
         <v>1</v>
       </c>
-      <c r="E9" s="10"/>
       <c r="F9" s="9">
         <v>1</v>
       </c>
@@ -1283,20 +1329,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>136</v>
+      <c r="I9" t="s">
+        <v>30</v>
       </c>
       <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" t="s">
         <v>28</v>
       </c>
+      <c r="K9" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="L9" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1319,20 +1365,20 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>135</v>
+      <c r="I10" t="s">
+        <v>32</v>
       </c>
       <c r="J10" t="s">
-        <v>32</v>
-      </c>
-      <c r="K10" t="s">
         <v>28</v>
       </c>
+      <c r="K10" s="1" t="s">
+        <v>203</v>
+      </c>
       <c r="L10" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1345,25 +1391,21 @@
       <c r="C11" s="9">
         <v>1</v>
       </c>
-      <c r="E11" s="10"/>
       <c r="G11" s="9">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>136</v>
+      <c r="I11" t="s">
+        <v>34</v>
       </c>
       <c r="J11" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" t="s">
         <v>35</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
       <c r="M11" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1376,7 +1418,6 @@
       <c r="D12" s="9">
         <v>2</v>
       </c>
-      <c r="E12" s="10"/>
       <c r="G12" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1384,32 +1425,26 @@
       <c r="H12" s="1">
         <v>-1</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>134</v>
+      <c r="I12" t="s">
+        <v>37</v>
       </c>
       <c r="J12" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" t="s">
         <v>35</v>
       </c>
       <c r="L12" s="6" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
       <c r="M12" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>187</v>
       </c>
       <c r="B13" s="9">
         <v>1</v>
       </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
       <c r="E13" s="9">
         <v>1</v>
       </c>
@@ -1417,28 +1452,22 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H13" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>135</v>
+      <c r="I13" t="s">
+        <v>186</v>
       </c>
       <c r="J13" t="s">
-        <v>39</v>
-      </c>
-      <c r="K13" t="s">
         <v>35</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M13" s="6" t="s">
-        <v>41</v>
+        <v>184</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B14" s="9">
         <v>1</v>
@@ -1446,10 +1475,9 @@
       <c r="C14" s="9">
         <v>1</v>
       </c>
-      <c r="D14" s="9">
-        <v>1</v>
-      </c>
-      <c r="E14" s="10"/>
+      <c r="E14" s="9">
+        <v>1</v>
+      </c>
       <c r="G14" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -1457,13 +1485,10 @@
       <c r="H14" s="1">
         <v>-1</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>136</v>
+      <c r="I14" t="s">
+        <v>39</v>
       </c>
       <c r="J14" t="s">
-        <v>39</v>
-      </c>
-      <c r="K14" t="s">
         <v>35</v>
       </c>
       <c r="L14" s="6" t="s">
@@ -1475,15 +1500,15 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="9">
         <v>1</v>
       </c>
+      <c r="C15" s="9">
+        <v>1</v>
+      </c>
       <c r="D15" s="9">
-        <v>1</v>
-      </c>
-      <c r="E15" s="9">
         <v>1</v>
       </c>
       <c r="G15" s="9">
@@ -1493,13 +1518,10 @@
       <c r="H15" s="1">
         <v>-1</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>134</v>
+      <c r="I15" t="s">
+        <v>39</v>
       </c>
       <c r="J15" t="s">
-        <v>39</v>
-      </c>
-      <c r="K15" t="s">
         <v>35</v>
       </c>
       <c r="L15" s="6" t="s">
@@ -1511,73 +1533,71 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>130</v>
+        <v>43</v>
       </c>
       <c r="B16" s="9">
         <v>1</v>
       </c>
-      <c r="C16" s="9">
+      <c r="D16" s="9">
+        <v>1</v>
+      </c>
+      <c r="E16" s="9">
         <v>1</v>
       </c>
       <c r="G16" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>135</v>
+        <v>2</v>
+      </c>
+      <c r="H16" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I16" t="s">
+        <v>39</v>
       </c>
       <c r="J16" t="s">
-        <v>133</v>
-      </c>
-      <c r="K16" t="s">
-        <v>131</v>
-      </c>
-      <c r="L16" s="11" t="s">
-        <v>132</v>
+        <v>35</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="M16" s="6" t="s">
-        <v>154</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>44</v>
+        <v>123</v>
       </c>
       <c r="B17" s="9">
         <v>1</v>
       </c>
-      <c r="E17" s="10"/>
-      <c r="F17" s="9">
+      <c r="C17" s="9">
         <v>1</v>
       </c>
       <c r="G17" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>136</v>
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>125</v>
       </c>
       <c r="J17" t="s">
-        <v>45</v>
-      </c>
-      <c r="K17" t="s">
-        <v>46</v>
-      </c>
-      <c r="L17" s="6" t="s">
-        <v>47</v>
+        <v>124</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>174</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>48</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>120</v>
+        <v>44</v>
       </c>
       <c r="B18" s="9">
         <v>1</v>
       </c>
-      <c r="E18" s="10"/>
       <c r="F18" s="9">
         <v>1</v>
       </c>
@@ -1585,119 +1605,101 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>134</v>
+      <c r="I18" t="s">
+        <v>45</v>
       </c>
       <c r="J18" t="s">
-        <v>121</v>
-      </c>
-      <c r="K18" t="s">
         <v>46</v>
       </c>
-      <c r="L18" s="11" t="s">
-        <v>122</v>
+      <c r="L18" s="10" t="s">
+        <v>175</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>159</v>
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>49</v>
+        <v>114</v>
       </c>
       <c r="B19" s="9">
         <v>1</v>
       </c>
-      <c r="E19" s="10"/>
       <c r="F19" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="H19" s="1">
-        <v>-2</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>135</v>
+      <c r="I19" t="s">
+        <v>115</v>
       </c>
       <c r="J19" t="s">
-        <v>50</v>
-      </c>
-      <c r="K19" t="s">
         <v>46</v>
       </c>
-      <c r="L19" t="s">
-        <v>51</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>160</v>
+      <c r="L19" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="M19" s="6" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>191</v>
+        <v>48</v>
       </c>
       <c r="B20" s="9">
         <v>1</v>
       </c>
-      <c r="E20" s="10"/>
       <c r="F20" s="9">
         <v>2</v>
       </c>
       <c r="G20" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>135</v>
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
+        <v>-2</v>
+      </c>
+      <c r="I20" t="s">
+        <v>49</v>
       </c>
       <c r="J20" t="s">
-        <v>192</v>
-      </c>
-      <c r="K20" t="s">
         <v>46</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>193</v>
+      <c r="L20" t="s">
+        <v>177</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>194</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>168</v>
       </c>
       <c r="B21" s="9">
-        <v>2</v>
-      </c>
-      <c r="E21" s="10"/>
+        <v>1</v>
+      </c>
       <c r="F21" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="H21" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>136</v>
+      <c r="I21" t="s">
+        <v>169</v>
       </c>
       <c r="J21" t="s">
-        <v>113</v>
-      </c>
-      <c r="K21" t="s">
         <v>46</v>
       </c>
-      <c r="L21" s="11" t="s">
-        <v>138</v>
+      <c r="L21" s="2" t="s">
+        <v>170</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
@@ -1705,136 +1707,120 @@
         <v>52</v>
       </c>
       <c r="B22" s="9">
-        <v>1</v>
-      </c>
-      <c r="E22" s="10"/>
+        <v>2</v>
+      </c>
       <c r="F22" s="9">
+        <v>3</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="0"/>
         <v>4</v>
-      </c>
-      <c r="G22" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
       <c r="H22" s="1">
         <v>-1</v>
       </c>
-      <c r="I22" s="1" t="s">
-        <v>135</v>
+      <c r="I22" t="s">
+        <v>107</v>
       </c>
       <c r="J22" t="s">
-        <v>53</v>
-      </c>
-      <c r="K22" t="s">
         <v>46</v>
       </c>
-      <c r="L22" s="6" t="s">
-        <v>139</v>
+      <c r="L22" s="10" t="s">
+        <v>178</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
       </c>
-      <c r="E23" s="10"/>
       <c r="F23" s="9">
         <v>4</v>
       </c>
       <c r="G23" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H23" s="1">
-        <v>1</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>134</v>
+        <v>-1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>51</v>
       </c>
       <c r="J23" t="s">
-        <v>56</v>
-      </c>
-      <c r="K23" t="s">
         <v>46</v>
       </c>
-      <c r="L23"/>
+      <c r="L23" s="6" t="s">
+        <v>179</v>
+      </c>
       <c r="M23" s="2" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>114</v>
+        <v>53</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
       </c>
-      <c r="E24" s="10"/>
       <c r="F24" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G24" s="9">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="H24" s="1">
-        <v>2</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>136</v>
+        <v>1</v>
+      </c>
+      <c r="I24" t="s">
+        <v>54</v>
       </c>
       <c r="J24" t="s">
-        <v>115</v>
-      </c>
-      <c r="K24" t="s">
         <v>46</v>
       </c>
-      <c r="L24" s="6"/>
+      <c r="L24"/>
       <c r="M24" s="2" t="s">
-        <v>164</v>
+        <v>148</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="B25" s="9">
         <v>1</v>
       </c>
-      <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="E25" s="10"/>
+      <c r="F25" s="9">
+        <v>6</v>
+      </c>
       <c r="G25" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="H25" s="1">
-        <v>-2</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>134</v>
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>109</v>
       </c>
       <c r="J25" t="s">
-        <v>58</v>
-      </c>
-      <c r="K25" t="s">
-        <v>59</v>
-      </c>
-      <c r="L25" s="6" t="s">
-        <v>60</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="L25" s="6"/>
       <c r="M25" s="2" t="s">
-        <v>165</v>
+        <v>149</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
@@ -1842,108 +1828,95 @@
       <c r="C26" s="9">
         <v>2</v>
       </c>
-      <c r="D26" s="9">
-        <v>2</v>
-      </c>
-      <c r="E26" s="10"/>
       <c r="G26" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>135</v>
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>-2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>56</v>
       </c>
       <c r="J26" t="s">
-        <v>62</v>
-      </c>
-      <c r="K26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L26" s="6" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>181</v>
+        <v>59</v>
       </c>
       <c r="B27" s="9">
         <v>1</v>
       </c>
       <c r="C27" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D27" s="9">
-        <v>1</v>
-      </c>
-      <c r="E27" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27" s="9">
-        <f t="shared" ref="G27" si="1">ROUND(C27*WoodVP+D27*SteelVP+E27*StoneVP+F27*GoldVP,0) + H27</f>
-        <v>4</v>
-      </c>
-      <c r="I27" s="1" t="s">
-        <v>135</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I27" t="s">
+        <v>60</v>
       </c>
       <c r="J27" t="s">
-        <v>182</v>
-      </c>
-      <c r="K27" t="s">
-        <v>101</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>189</v>
+        <v>57</v>
+      </c>
+      <c r="L27" s="6" t="s">
+        <v>61</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>183</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="B28" s="9">
         <v>1</v>
       </c>
       <c r="C28" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D28" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E28" s="9">
         <v>1</v>
       </c>
-      <c r="F28" s="9">
-        <v>1</v>
-      </c>
       <c r="G28" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I28" s="1" t="s">
-        <v>135</v>
+        <f t="shared" ref="G28" si="1">ROUND(C28*WoodVP+D28*SteelVP+E28*StoneVP+F28*GoldVP,0) + H28</f>
+        <v>4</v>
+      </c>
+      <c r="I28" t="s">
+        <v>165</v>
       </c>
       <c r="J28" t="s">
-        <v>100</v>
-      </c>
-      <c r="K28" t="s">
-        <v>101</v>
+        <v>96</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>188</v>
+        <v>216</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>94</v>
       </c>
       <c r="B29" s="9">
         <v>1</v>
@@ -1951,543 +1924,507 @@
       <c r="C29" s="9">
         <v>2</v>
       </c>
-      <c r="E29" s="10"/>
+      <c r="D29" s="9">
+        <v>2</v>
+      </c>
+      <c r="E29" s="9">
+        <v>1</v>
+      </c>
+      <c r="F29" s="9">
+        <v>1</v>
+      </c>
       <c r="G29" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J29" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="K29" t="s">
-        <v>66</v>
-      </c>
-      <c r="L29" s="6" t="s">
-        <v>67</v>
+        <v>9</v>
+      </c>
+      <c r="I29" t="s">
+        <v>95</v>
+      </c>
+      <c r="J29" t="s">
+        <v>96</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>167</v>
+        <v>217</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B30" s="9">
         <v>1</v>
       </c>
-      <c r="E30" s="9">
+      <c r="C30" s="9">
         <v>2</v>
       </c>
       <c r="G30" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I30" s="1" t="s">
-        <v>135</v>
+      <c r="I30" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="J30" t="s">
-        <v>69</v>
-      </c>
-      <c r="K30" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L30" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="M30" s="6" t="s">
-        <v>71</v>
+        <v>180</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>169</v>
+        <v>65</v>
       </c>
       <c r="B31" s="9">
-        <v>2</v>
-      </c>
-      <c r="D31" s="9">
+        <v>1</v>
+      </c>
+      <c r="E31" s="9">
+        <v>2</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="E31" s="10"/>
-      <c r="G31" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="I31" s="1" t="s">
-        <v>136</v>
+      <c r="I31" t="s">
+        <v>66</v>
       </c>
       <c r="J31" t="s">
-        <v>170</v>
-      </c>
-      <c r="K31" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>171</v>
+        <v>181</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>153</v>
       </c>
       <c r="B32" s="9">
         <v>2</v>
       </c>
       <c r="D32" s="9">
+        <v>3</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E32" s="10"/>
-      <c r="G32" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I32" s="1" t="s">
-        <v>134</v>
+      <c r="I32" t="s">
+        <v>154</v>
       </c>
       <c r="J32" t="s">
-        <v>73</v>
-      </c>
-      <c r="K32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="M32" s="2" t="s">
-        <v>172</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>116</v>
+        <v>68</v>
       </c>
       <c r="B33" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D33" s="9">
-        <v>5</v>
-      </c>
-      <c r="E33" s="10"/>
+        <v>4</v>
+      </c>
       <c r="G33" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H33" s="1">
-        <v>1</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>135</v>
+        <v>6</v>
+      </c>
+      <c r="I33" t="s">
+        <v>69</v>
       </c>
       <c r="J33" t="s">
-        <v>117</v>
-      </c>
-      <c r="K33" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>173</v>
+        <v>192</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
       </c>
       <c r="D34" s="9">
-        <v>6</v>
-      </c>
-      <c r="E34" s="10"/>
+        <v>5</v>
+      </c>
       <c r="G34" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H34" s="1">
         <v>1</v>
       </c>
-      <c r="I34" s="1" t="s">
-        <v>136</v>
+      <c r="I34" t="s">
+        <v>111</v>
       </c>
       <c r="J34" t="s">
-        <v>119</v>
-      </c>
-      <c r="K34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>174</v>
+        <v>134</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>95</v>
+        <v>156</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>74</v>
+        <v>112</v>
       </c>
       <c r="B35" s="9">
         <v>1</v>
       </c>
       <c r="D35" s="9">
-        <v>7</v>
-      </c>
-      <c r="E35" s="10"/>
+        <v>6</v>
+      </c>
       <c r="G35" s="9">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="I35" s="1" t="s">
-        <v>134</v>
+        <v>9</v>
+      </c>
+      <c r="H35" s="1">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>113</v>
       </c>
       <c r="J35" t="s">
-        <v>75</v>
-      </c>
-      <c r="K35" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>187</v>
+        <v>157</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>175</v>
+        <v>90</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
       </c>
-      <c r="C36" s="9">
-        <v>1</v>
-      </c>
-      <c r="E36" s="9">
-        <v>1</v>
+      <c r="D36" s="9">
+        <v>7</v>
       </c>
       <c r="G36" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>135</v>
+        <v>10</v>
+      </c>
+      <c r="I36" t="s">
+        <v>71</v>
       </c>
       <c r="J36" t="s">
-        <v>83</v>
-      </c>
-      <c r="K36" t="s">
-        <v>78</v>
-      </c>
-      <c r="L36" s="11" t="s">
-        <v>106</v>
+        <v>64</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L36" s="6" t="s">
+        <v>206</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B37" s="9">
         <v>1</v>
       </c>
-      <c r="D37" s="9">
-        <v>2</v>
+      <c r="C37" s="9">
+        <v>1</v>
+      </c>
+      <c r="E37" s="9">
+        <v>1</v>
       </c>
       <c r="G37" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I37" s="1" t="s">
-        <v>136</v>
+      <c r="I37" t="s">
+        <v>79</v>
       </c>
       <c r="J37" t="s">
-        <v>77</v>
-      </c>
-      <c r="K37" t="s">
-        <v>78</v>
-      </c>
-      <c r="L37" s="11" t="s">
-        <v>106</v>
+        <v>74</v>
+      </c>
+      <c r="L37" s="10" t="s">
+        <v>182</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>177</v>
+        <v>159</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="B38" s="9">
         <v>1</v>
       </c>
-      <c r="C38" s="9">
-        <v>2</v>
-      </c>
-      <c r="E38" s="10"/>
+      <c r="D38" s="9">
+        <v>2</v>
+      </c>
       <c r="G38" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I38" s="1" t="s">
-        <v>134</v>
+      <c r="I38" t="s">
+        <v>73</v>
       </c>
       <c r="J38" t="s">
-        <v>80</v>
-      </c>
-      <c r="K38" t="s">
-        <v>78</v>
-      </c>
-      <c r="L38" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="M38" s="6" t="s">
-        <v>81</v>
+        <v>74</v>
+      </c>
+      <c r="L38" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="B39" s="9">
-        <v>2</v>
-      </c>
-      <c r="D39" s="9">
-        <v>2</v>
-      </c>
-      <c r="E39" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="C39" s="9">
+        <v>2</v>
+      </c>
       <c r="G39" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="I39" s="1" t="s">
-        <v>135</v>
+      <c r="I39" t="s">
+        <v>76</v>
       </c>
       <c r="J39" t="s">
-        <v>124</v>
-      </c>
-      <c r="K39" t="s">
-        <v>78</v>
-      </c>
-      <c r="L39" s="11"/>
+        <v>74</v>
+      </c>
+      <c r="L39" s="10" t="s">
+        <v>182</v>
+      </c>
       <c r="M39" s="6" t="s">
-        <v>145</v>
+        <v>77</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
       <c r="B40" s="9">
         <v>2</v>
       </c>
       <c r="E40" s="9">
+        <v>2</v>
+      </c>
+      <c r="G40" s="9">
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G40" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H40" s="1">
-        <v>1</v>
-      </c>
-      <c r="I40" s="1" t="s">
-        <v>136</v>
+      <c r="I40" t="s">
+        <v>190</v>
       </c>
       <c r="J40" t="s">
-        <v>85</v>
-      </c>
-      <c r="K40" t="s">
-        <v>78</v>
-      </c>
-      <c r="L40"/>
-      <c r="M40" s="2" t="s">
-        <v>179</v>
+        <v>74</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L40" s="10" t="s">
+        <v>207</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B41" s="9">
-        <v>1</v>
-      </c>
-      <c r="E41" s="9">
-        <v>2</v>
-      </c>
-      <c r="F41" s="9">
+        <v>2</v>
+      </c>
+      <c r="D41" s="9">
         <v>2</v>
       </c>
       <c r="G41" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H41" s="1">
-        <v>1</v>
-      </c>
-      <c r="I41" s="1" t="s">
-        <v>134</v>
+        <v>3</v>
+      </c>
+      <c r="I41" t="s">
+        <v>117</v>
       </c>
       <c r="J41" t="s">
-        <v>125</v>
-      </c>
-      <c r="K41" t="s">
-        <v>78</v>
-      </c>
-      <c r="L41"/>
-      <c r="M41" s="2" t="s">
-        <v>180</v>
+        <v>74</v>
+      </c>
+      <c r="L41" s="10"/>
+      <c r="M41" s="6" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>193</v>
       </c>
       <c r="B42" s="9">
         <v>1</v>
       </c>
+      <c r="C42" s="9">
+        <v>2</v>
+      </c>
       <c r="E42" s="9">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G42" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I42" s="1" t="s">
-        <v>135</v>
+        <v>5</v>
+      </c>
+      <c r="H42" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I42" t="s">
+        <v>191</v>
       </c>
       <c r="J42" t="s">
-        <v>87</v>
-      </c>
-      <c r="K42" t="s">
-        <v>78</v>
-      </c>
-      <c r="L42" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="M42" s="2" t="s">
-        <v>178</v>
+        <v>74</v>
+      </c>
+      <c r="L42" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="M42" s="6" t="s">
+        <v>194</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B43" s="9">
-        <v>1</v>
-      </c>
-      <c r="C43" s="9">
-        <v>2</v>
-      </c>
-      <c r="D43" s="9">
-        <v>1</v>
-      </c>
-      <c r="E43" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="E43" s="9">
+        <v>3</v>
+      </c>
       <c r="G43" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="H43" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I43" s="1" t="s">
-        <v>136</v>
+        <v>1</v>
+      </c>
+      <c r="I43" t="s">
+        <v>81</v>
       </c>
       <c r="J43" t="s">
-        <v>89</v>
-      </c>
-      <c r="K43" t="s">
-        <v>195</v>
-      </c>
-      <c r="L43" t="s">
-        <v>196</v>
+        <v>74</v>
+      </c>
+      <c r="L43"/>
+      <c r="M43" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>119</v>
       </c>
       <c r="B44" s="9">
         <v>1</v>
       </c>
-      <c r="C44" s="9">
-        <v>1</v>
-      </c>
-      <c r="D44" s="9">
-        <v>2</v>
-      </c>
-      <c r="E44" s="10"/>
+      <c r="E44" s="9">
+        <v>2</v>
+      </c>
+      <c r="F44" s="9">
+        <v>2</v>
+      </c>
       <c r="G44" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="H44" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I44" s="1" t="s">
-        <v>134</v>
+        <v>1</v>
+      </c>
+      <c r="I44" t="s">
+        <v>118</v>
       </c>
       <c r="J44" t="s">
-        <v>91</v>
-      </c>
-      <c r="K44" t="s">
-        <v>195</v>
-      </c>
-      <c r="L44" t="s">
-        <v>196</v>
+        <v>74</v>
+      </c>
+      <c r="L44"/>
+      <c r="M44" s="2" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>150</v>
+        <v>82</v>
       </c>
       <c r="B45" s="9">
         <v>1</v>
       </c>
       <c r="E45" s="9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G45" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>136</v>
+        <v>9</v>
+      </c>
+      <c r="I45" t="s">
+        <v>83</v>
       </c>
       <c r="J45" t="s">
-        <v>92</v>
-      </c>
-      <c r="K45" t="s">
-        <v>93</v>
+        <v>74</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>203</v>
       </c>
       <c r="L45" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="M45" s="6"/>
+        <v>208</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="B46" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C46" s="9">
-        <v>3</v>
-      </c>
-      <c r="E46" s="10"/>
+        <v>2</v>
+      </c>
+      <c r="D46" s="9">
+        <v>1</v>
+      </c>
       <c r="G46" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -2495,143 +2432,271 @@
       <c r="H46" s="1">
         <v>-1</v>
       </c>
-      <c r="I46" s="1" t="s">
-        <v>134</v>
+      <c r="I46" t="s">
+        <v>85</v>
       </c>
       <c r="J46" t="s">
-        <v>96</v>
-      </c>
-      <c r="K46" t="s">
-        <v>93</v>
-      </c>
-      <c r="L46" s="2" t="s">
-        <v>146</v>
+        <v>172</v>
+      </c>
+      <c r="L46" t="s">
+        <v>173</v>
+      </c>
+      <c r="M46" s="2" t="s">
+        <v>195</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>112</v>
+        <v>86</v>
       </c>
       <c r="B47" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C47" s="9">
-        <v>4</v>
-      </c>
-      <c r="E47" s="10"/>
+        <v>1</v>
+      </c>
+      <c r="D47" s="9">
+        <v>2</v>
+      </c>
       <c r="G47" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H47" s="1">
         <v>-1</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>135</v>
+      <c r="I47" t="s">
+        <v>87</v>
       </c>
       <c r="J47" t="s">
-        <v>96</v>
-      </c>
-      <c r="K47" t="s">
-        <v>93</v>
-      </c>
-      <c r="L47" s="2" t="s">
-        <v>184</v>
+        <v>172</v>
+      </c>
+      <c r="L47" t="s">
+        <v>173</v>
+      </c>
+      <c r="M47" s="2" t="s">
+        <v>196</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>127</v>
+        <v>213</v>
       </c>
       <c r="B48" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" s="9">
+        <v>2</v>
+      </c>
+      <c r="D48" s="9">
+        <v>2</v>
+      </c>
+      <c r="E48" s="9">
+        <v>1</v>
+      </c>
+      <c r="G48" s="9">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="E48" s="10"/>
-      <c r="G48" s="9">
+      <c r="H48" s="1">
+        <v>-2</v>
+      </c>
+      <c r="I48" t="s">
+        <v>212</v>
+      </c>
+      <c r="J48" t="s">
+        <v>172</v>
+      </c>
+      <c r="L48" t="s">
+        <v>211</v>
+      </c>
+      <c r="M48" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>135</v>
+      </c>
+      <c r="B49" s="9">
+        <v>1</v>
+      </c>
+      <c r="E49" s="9">
+        <v>1</v>
+      </c>
+      <c r="G49" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I49" t="s">
+        <v>88</v>
+      </c>
+      <c r="J49" t="s">
+        <v>89</v>
+      </c>
+      <c r="L49" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="M49" s="6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>105</v>
+      </c>
+      <c r="B50" s="9">
+        <v>2</v>
+      </c>
+      <c r="C50" s="9">
+        <v>3</v>
+      </c>
+      <c r="G50" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H50" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I50" t="s">
+        <v>91</v>
+      </c>
+      <c r="J50" t="s">
+        <v>89</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="M50" s="2" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>106</v>
+      </c>
+      <c r="B51" s="9">
+        <v>2</v>
+      </c>
+      <c r="C51" s="9">
+        <v>4</v>
+      </c>
+      <c r="G51" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H51" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I51" t="s">
+        <v>91</v>
+      </c>
+      <c r="J51" t="s">
+        <v>89</v>
+      </c>
+      <c r="L51" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="M51" s="2" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="B52" s="9">
+        <v>2</v>
+      </c>
+      <c r="C52" s="9">
+        <v>5</v>
+      </c>
+      <c r="G52" s="9">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="J48" t="s">
+      <c r="I52" t="s">
+        <v>121</v>
+      </c>
+      <c r="J52" t="s">
+        <v>89</v>
+      </c>
+      <c r="L52" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="M52" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>122</v>
+      </c>
+      <c r="B53" s="9">
+        <v>1</v>
+      </c>
+      <c r="C53" s="9">
+        <v>4</v>
+      </c>
+      <c r="F53" s="9">
+        <v>1</v>
+      </c>
+      <c r="G53" s="9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H53" s="1">
+        <v>1</v>
+      </c>
+      <c r="I53" t="s">
         <v>128</v>
       </c>
-      <c r="K48" t="s">
+      <c r="J53" t="s">
+        <v>89</v>
+      </c>
+      <c r="K53" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L53" t="s">
+        <v>209</v>
+      </c>
+      <c r="M53" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>92</v>
+      </c>
+      <c r="B54" s="9">
+        <v>1</v>
+      </c>
+      <c r="C54" s="9">
+        <v>7</v>
+      </c>
+      <c r="G54" s="9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I54" t="s">
         <v>93</v>
       </c>
-      <c r="L48" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>129</v>
-      </c>
-      <c r="B49" s="9">
-        <v>1</v>
-      </c>
-      <c r="C49" s="9">
-        <v>4</v>
-      </c>
-      <c r="E49" s="10"/>
-      <c r="F49" s="9">
-        <v>1</v>
-      </c>
-      <c r="G49" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H49" s="1">
-        <v>1</v>
-      </c>
-      <c r="I49" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J49" t="s">
-        <v>143</v>
-      </c>
-      <c r="K49" t="s">
-        <v>93</v>
-      </c>
-      <c r="L49" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>97</v>
-      </c>
-      <c r="B50" s="9">
-        <v>1</v>
-      </c>
-      <c r="C50" s="9">
-        <v>7</v>
-      </c>
-      <c r="E50" s="10"/>
-      <c r="G50" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I50" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="J50" t="s">
-        <v>98</v>
-      </c>
-      <c r="K50" t="s">
-        <v>93</v>
-      </c>
-      <c r="L50" s="6" t="s">
-        <v>186</v>
+      <c r="J54" t="s">
+        <v>89</v>
+      </c>
+      <c r="K54" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L54" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="M54" s="2" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>
   <sortState ref="A2:M41">
-    <sortCondition ref="K2:K41"/>
+    <sortCondition ref="J2:J41"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2655,10 +2720,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2717,13 +2782,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2731,12 +2796,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <f>COUNTA(Deck!C2:C110)</f>
-        <v>22</v>
+        <f>COUNTA(Deck!C2:C114)</f>
+        <v>24</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(Deck!C2:C109)</f>
-        <v>49</v>
+        <f>SUM(Deck!C2:C113)</f>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2744,12 +2809,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <f>COUNTA(Deck!D2:D110)</f>
-        <v>19</v>
+        <f>COUNTA(Deck!D2:D114)</f>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
-        <f>SUM(Deck!D2:D109)</f>
-        <v>48</v>
+        <f>SUM(Deck!D2:D113)</f>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2757,12 +2822,12 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <f>COUNTA(Deck!E2:E110)</f>
-        <v>13</v>
+        <f>COUNTA(Deck!E2:E114)</f>
+        <v>17</v>
       </c>
       <c r="C4" s="1">
-        <f>SUM(Deck!E2:E109)</f>
-        <v>22</v>
+        <f>SUM(Deck!E2:E113)</f>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -2770,11 +2835,11 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <f>COUNTA(Deck!F2:F110)</f>
+        <f>COUNTA(Deck!F2:F114)</f>
         <v>15</v>
       </c>
       <c r="C5" s="1">
-        <f>SUM(Deck!F2:F110)</f>
+        <f>SUM(Deck!F2:F114)</f>
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Tons of game changes
Aiming for 108 cards in total for 4 players.

Renames:
* Gold Bar --> Gold Ingot

Clarifications
* Ancient artifacts don't stack bonus

Removals
* Chest - not as good, and confusing
* Normal Spade - too many Draw powers
* Necklace - switch to Gold Mine
* Only one Horseshoe, also tweaked points
* Only one Anvil now
* Stone piles are gone... what was I thinking??
* Windmill is gone - we don't need two crossbows really

Additions
* Fireball - another fun interactive card
* A second Gold Mine instead of a second
* Cave - rewards having a big deck

Revised
* Pulley System is better now, but comes out later
* Robot arm got cheaper
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\project-spider-monkey\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="218">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="216">
   <si>
     <t>Name</t>
   </si>
@@ -102,9 +102,6 @@
     <t>Build it strong, build it right.</t>
   </si>
   <si>
-    <t>A Gold Bar</t>
-  </si>
-  <si>
     <t>gold-bar</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>Most people just call this a shovel.</t>
   </si>
   <si>
-    <t>Normal Spade</t>
-  </si>
-  <si>
     <t>Heavy Spade</t>
   </si>
   <si>
@@ -207,15 +201,6 @@
     <t>You may keep 2 Resources until the next turn</t>
   </si>
   <si>
-    <t>Barrel</t>
-  </si>
-  <si>
-    <t>barrel</t>
-  </si>
-  <si>
-    <t>You may keep 3 Resources until the next turn</t>
-  </si>
-  <si>
     <t>Screwdriver</t>
   </si>
   <si>
@@ -282,12 +267,6 @@
     <t>stone-tower</t>
   </si>
   <si>
-    <t>Windmill</t>
-  </si>
-  <si>
-    <t>windmill</t>
-  </si>
-  <si>
     <t>Crossbow</t>
   </si>
   <si>
@@ -378,12 +357,6 @@
     <t>key</t>
   </si>
   <si>
-    <t>Stone Pile</t>
-  </si>
-  <si>
-    <t>stone-pile</t>
-  </si>
-  <si>
     <t>rune-stone</t>
   </si>
   <si>
@@ -402,9 +375,6 @@
     <t>Boomerang</t>
   </si>
   <si>
-    <t>pass</t>
-  </si>
-  <si>
     <t>boomerang</t>
   </si>
   <si>
@@ -420,15 +390,9 @@
     <t>May be purchased for 4 Steel or 3 Stone</t>
   </si>
   <si>
-    <t>We used the steel to collect the stones, duh!</t>
-  </si>
-  <si>
     <t>May be purchased for 3 Steel</t>
   </si>
   <si>
-    <t>May be purchased for 2 Steel or 3 Wood</t>
-  </si>
-  <si>
     <t>May be purchased for 3 Steel or 4 Wood</t>
   </si>
   <si>
@@ -450,9 +414,6 @@
     <t>This one messes up your small deck strategy.</t>
   </si>
   <si>
-    <t>To war!</t>
-  </si>
-  <si>
     <t>Great for making decrees.</t>
   </si>
   <si>
@@ -483,9 +444,6 @@
     <t>Out of my way!</t>
   </si>
   <si>
-    <t>Also great for scaring people.</t>
-  </si>
-  <si>
     <t>Everyone needs one of these.</t>
   </si>
   <si>
@@ -552,9 +510,6 @@
     <t>Trash this card to build any available blueprint worth 6 VP or less for free.</t>
   </si>
   <si>
-    <t>Save 1 Wood this turn. At end of this turn, pass to left and place in opponent's hand.</t>
-  </si>
-  <si>
     <t>Save 1 Gold this turn</t>
   </si>
   <si>
@@ -582,18 +537,6 @@
     <t>Save 2 Wood this turn</t>
   </si>
   <si>
-    <t>Draw a card from your deck. If it contains Wood or Steel, discard it.</t>
-  </si>
-  <si>
-    <t>Just the heavy stuff, please.</t>
-  </si>
-  <si>
-    <t>open-chest</t>
-  </si>
-  <si>
-    <t>Chest</t>
-  </si>
-  <si>
     <t>Stone Wheel</t>
   </si>
   <si>
@@ -615,9 +558,6 @@
     <t>Simple machines always come in handy.</t>
   </si>
   <si>
-    <t>Windmill, or windfall??</t>
-  </si>
-  <si>
     <t>We don't illustrate how a crossbow was used to accomplish this.</t>
   </si>
   <si>
@@ -645,18 +585,12 @@
     <t>AtEnd</t>
   </si>
   <si>
-    <t>*At game end, +2 VP for two Ancient artifacts, and +4 VP for three Ancient artifacts</t>
-  </si>
-  <si>
     <t>*At game end, +1 VP per card that contains Steel, including this one.</t>
   </si>
   <si>
     <t>*At game end, +3 VP if you have two Stone Wheels (count this bonus once)</t>
   </si>
   <si>
-    <t>*At game end, 1 VP for every three cards in deck</t>
-  </si>
-  <si>
     <t>*At game end, +2 VP if deck contains 4 Wood besides this card.</t>
   </si>
   <si>
@@ -682,6 +616,66 @@
   </si>
   <si>
     <t>A must-have for the modern surivor.</t>
+  </si>
+  <si>
+    <t>Nobody tell him that gold is too soft for armor.</t>
+  </si>
+  <si>
+    <t>*At game end, gain 2/5 VP if you have 2/3 Ancient artifacts (count this bonus only once)</t>
+  </si>
+  <si>
+    <t>Save 2 Wood this turn. Pass to another player of your choice at the end of your turn.</t>
+  </si>
+  <si>
+    <t>May be purchased for 3 Wood</t>
+  </si>
+  <si>
+    <t>interactive</t>
+  </si>
+  <si>
+    <t>Will you pull the trigger?</t>
+  </si>
+  <si>
+    <t>Trash this card to trash any two cards in any row.</t>
+  </si>
+  <si>
+    <t>Gold Ingot</t>
+  </si>
+  <si>
+    <t>big deck</t>
+  </si>
+  <si>
+    <t>*At game end,  +3 VP if your deck has 10 or more cards total</t>
+  </si>
+  <si>
+    <t>Good year.</t>
+  </si>
+  <si>
+    <t>Cave</t>
+  </si>
+  <si>
+    <t>cave-entrance</t>
+  </si>
+  <si>
+    <t>Save 2 Stone this turn</t>
+  </si>
+  <si>
+    <t>Fireball</t>
+  </si>
+  <si>
+    <t>burning-meteor</t>
+  </si>
+  <si>
+    <t>Steeltoe Boots</t>
+  </si>
+  <si>
+    <t>steeltoe-boots</t>
+  </si>
+  <si>
+    <t>*At game end, +1 VP for every three cards in your deck</t>
+  </si>
+  <si>
+    <t>May be purchased for 2 Stone</t>
   </si>
 </sst>
 </file>
@@ -1059,13 +1053,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M54"/>
+  <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1118,7 +1112,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>204</v>
+        <v>184</v>
       </c>
       <c r="L1" s="5" t="s">
         <v>10</v>
@@ -1172,12 +1166,12 @@
       </c>
       <c r="L3"/>
       <c r="M3" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="B4" s="9">
         <v>4</v>
@@ -1196,7 +1190,7 @@
       </c>
       <c r="L4"/>
       <c r="M4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1220,7 +1214,7 @@
       </c>
       <c r="L5"/>
       <c r="M5" s="6" t="s">
-        <v>142</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1249,7 +1243,7 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>203</v>
       </c>
       <c r="B7" s="9">
         <v>12</v>
@@ -1261,156 +1255,156 @@
         <v>0</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J7" t="s">
         <v>14</v>
       </c>
       <c r="L7" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="M7" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="9">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>2</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1</v>
+      </c>
+      <c r="G8" s="9">
+        <f t="shared" ref="G8:G52" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="E8" s="9">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9">
-        <f t="shared" ref="G8:G54" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
-        <v>6</v>
-      </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>27</v>
       </c>
-      <c r="J8" t="s">
-        <v>28</v>
-      </c>
       <c r="K8" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="L8" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>141</v>
+        <v>128</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2</v>
+      </c>
+      <c r="D9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I9" t="s">
-        <v>30</v>
-      </c>
       <c r="J9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="L9" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>140</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9">
+        <v>1</v>
+      </c>
+      <c r="F10" s="9">
+        <v>1</v>
+      </c>
+      <c r="G10" s="9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="9">
-        <v>1</v>
-      </c>
-      <c r="F10" s="9">
-        <v>1</v>
-      </c>
-      <c r="G10" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I10" t="s">
-        <v>32</v>
-      </c>
       <c r="J10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="L10" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>143</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>34</v>
       </c>
-      <c r="J11" t="s">
-        <v>35</v>
-      </c>
       <c r="L11" s="6" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="M11" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="9">
         <v>1</v>
@@ -1426,25 +1420,28 @@
         <v>-1</v>
       </c>
       <c r="I12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="J12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L12" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="M12" t="s">
         <v>126</v>
-      </c>
-      <c r="M12" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>187</v>
+        <v>37</v>
       </c>
       <c r="B13" s="9">
         <v>1</v>
       </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
       <c r="E13" s="9">
         <v>1</v>
       </c>
@@ -1452,27 +1449,30 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="H13" s="1">
+        <v>-1</v>
+      </c>
       <c r="I13" t="s">
-        <v>186</v>
+        <v>38</v>
       </c>
       <c r="J13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="L13" s="6" t="s">
-        <v>184</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>185</v>
+        <v>39</v>
+      </c>
+      <c r="M13" s="6" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B14" s="9">
         <v>1</v>
       </c>
-      <c r="C14" s="9">
+      <c r="D14" s="9">
         <v>1</v>
       </c>
       <c r="E14" s="9">
@@ -1486,21 +1486,21 @@
         <v>-1</v>
       </c>
       <c r="I14" t="s">
+        <v>38</v>
+      </c>
+      <c r="J14" t="s">
+        <v>34</v>
+      </c>
+      <c r="L14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="J14" t="s">
-        <v>35</v>
-      </c>
-      <c r="L14" s="6" t="s">
+      <c r="M14" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="M14" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>114</v>
       </c>
       <c r="B15" s="9">
         <v>1</v>
@@ -1508,233 +1508,230 @@
       <c r="C15" s="9">
         <v>1</v>
       </c>
-      <c r="D15" s="9">
-        <v>1</v>
-      </c>
       <c r="G15" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H15" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I15" t="s">
-        <v>39</v>
+        <v>115</v>
       </c>
       <c r="J15" t="s">
-        <v>35</v>
-      </c>
-      <c r="L15" s="6" t="s">
-        <v>40</v>
+        <v>200</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>198</v>
       </c>
       <c r="M15" s="6" t="s">
-        <v>41</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>43</v>
+        <v>210</v>
       </c>
       <c r="B16" s="9">
         <v>1</v>
       </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
       <c r="D16" s="9">
         <v>1</v>
       </c>
-      <c r="E16" s="9">
-        <v>1</v>
-      </c>
       <c r="G16" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
+        <f t="shared" ref="G16" si="1">ROUND(C16*WoodVP+D16*SteelVP+E16*StoneVP+F16*GoldVP,0) + H16</f>
+        <v>4</v>
       </c>
       <c r="H16" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>39</v>
+        <v>211</v>
       </c>
       <c r="J16" t="s">
-        <v>35</v>
+        <v>200</v>
       </c>
       <c r="L16" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="M16" s="6" t="s">
-        <v>41</v>
+        <v>202</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>123</v>
+        <v>42</v>
       </c>
       <c r="B17" s="9">
         <v>1</v>
       </c>
-      <c r="C17" s="9">
+      <c r="F17" s="9">
         <v>1</v>
       </c>
       <c r="G17" s="9">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>125</v>
+        <v>43</v>
       </c>
       <c r="J17" t="s">
-        <v>124</v>
+        <v>44</v>
       </c>
       <c r="L17" s="10" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="M17" s="6" t="s">
-        <v>139</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
+        <v>108</v>
+      </c>
+      <c r="J18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" s="9">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9">
-        <v>1</v>
-      </c>
-      <c r="G18" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>45</v>
-      </c>
-      <c r="J18" t="s">
-        <v>46</v>
-      </c>
       <c r="L18" s="10" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
       <c r="M18" s="6" t="s">
-        <v>47</v>
+        <v>131</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>114</v>
+        <v>46</v>
       </c>
       <c r="B19" s="9">
         <v>1</v>
       </c>
       <c r="F19" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="9">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
+      <c r="H19" s="1">
+        <v>-2</v>
+      </c>
       <c r="I19" t="s">
-        <v>115</v>
+        <v>47</v>
       </c>
       <c r="J19" t="s">
-        <v>46</v>
-      </c>
-      <c r="L19" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>144</v>
+        <v>44</v>
+      </c>
+      <c r="L19" t="s">
+        <v>162</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>48</v>
+        <v>154</v>
       </c>
       <c r="B20" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="9">
         <v>2</v>
       </c>
       <c r="G20" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H20" s="1">
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="I20" t="s">
-        <v>49</v>
+        <v>155</v>
       </c>
       <c r="J20" t="s">
-        <v>46</v>
-      </c>
-      <c r="L20" t="s">
-        <v>177</v>
+        <v>44</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>156</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>50</v>
       </c>
       <c r="B21" s="9">
         <v>1</v>
       </c>
       <c r="F21" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G21" s="9">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="H21" s="1">
+        <v>-1</v>
+      </c>
       <c r="I21" t="s">
-        <v>169</v>
+        <v>100</v>
       </c>
       <c r="J21" t="s">
-        <v>46</v>
-      </c>
-      <c r="L21" s="2" t="s">
-        <v>170</v>
+        <v>44</v>
+      </c>
+      <c r="L21" s="10" t="s">
+        <v>163</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>171</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B22" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F22" s="9">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G22" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H22" s="1">
         <v>-1</v>
       </c>
       <c r="I22" t="s">
-        <v>107</v>
+        <v>49</v>
       </c>
       <c r="J22" t="s">
-        <v>46</v>
-      </c>
-      <c r="L22" s="10" t="s">
-        <v>178</v>
+        <v>44</v>
+      </c>
+      <c r="L22" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="M22" s="2" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
@@ -1744,113 +1741,119 @@
       </c>
       <c r="G23" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H23" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="J23" t="s">
-        <v>46</v>
-      </c>
-      <c r="L23" s="6" t="s">
-        <v>179</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="L23"/>
       <c r="M23" s="2" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
       </c>
       <c r="F24" s="9">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G24" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="H24" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I24" t="s">
-        <v>54</v>
+        <v>102</v>
       </c>
       <c r="J24" t="s">
-        <v>46</v>
-      </c>
-      <c r="L24"/>
+        <v>44</v>
+      </c>
+      <c r="L24" s="6"/>
       <c r="M24" s="2" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>108</v>
+        <v>53</v>
       </c>
       <c r="B25" s="9">
         <v>1</v>
       </c>
-      <c r="F25" s="9">
-        <v>6</v>
+      <c r="C25" s="9">
+        <v>2</v>
       </c>
       <c r="G25" s="9">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="H25" s="1">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="I25" t="s">
-        <v>109</v>
+        <v>54</v>
       </c>
       <c r="J25" t="s">
-        <v>46</v>
-      </c>
-      <c r="L25" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="L25" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="M25" s="2" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>55</v>
+        <v>150</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
       </c>
       <c r="C26" s="9">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D26" s="9">
+        <v>1</v>
+      </c>
+      <c r="E26" s="9">
+        <v>1</v>
       </c>
       <c r="G26" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H26" s="1">
-        <v>-2</v>
+        <f t="shared" ref="G26" si="2">ROUND(C26*WoodVP+D26*SteelVP+E26*StoneVP+F26*GoldVP,0) + H26</f>
+        <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>56</v>
+        <v>151</v>
       </c>
       <c r="J26" t="s">
-        <v>57</v>
-      </c>
-      <c r="L26" s="6" t="s">
-        <v>58</v>
+        <v>89</v>
+      </c>
+      <c r="K26" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>59</v>
+        <v>87</v>
       </c>
       <c r="B27" s="9">
         <v>1</v>
@@ -1861,62 +1864,68 @@
       <c r="D27" s="9">
         <v>2</v>
       </c>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="F27" s="9">
+        <v>1</v>
+      </c>
       <c r="G27" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="I27" t="s">
-        <v>60</v>
+        <v>88</v>
       </c>
       <c r="J27" t="s">
-        <v>57</v>
-      </c>
-      <c r="L27" s="6" t="s">
-        <v>61</v>
+        <v>89</v>
+      </c>
+      <c r="K27" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="M27" s="2" t="s">
-        <v>151</v>
+        <v>195</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>164</v>
+        <v>207</v>
       </c>
       <c r="B28" s="9">
         <v>1</v>
       </c>
-      <c r="C28" s="9">
-        <v>1</v>
-      </c>
-      <c r="D28" s="9">
-        <v>1</v>
-      </c>
       <c r="E28" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28" s="9">
-        <f t="shared" ref="G28" si="1">ROUND(C28*WoodVP+D28*SteelVP+E28*StoneVP+F28*GoldVP,0) + H28</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
       <c r="I28" t="s">
-        <v>165</v>
+        <v>208</v>
       </c>
       <c r="J28" t="s">
-        <v>96</v>
+        <v>204</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="M28" s="2" t="s">
-        <v>166</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>94</v>
+        <v>57</v>
       </c>
       <c r="B29" s="9">
         <v>1</v>
@@ -1924,122 +1933,116 @@
       <c r="C29" s="9">
         <v>2</v>
       </c>
-      <c r="D29" s="9">
-        <v>2</v>
-      </c>
-      <c r="E29" s="9">
-        <v>1</v>
-      </c>
-      <c r="F29" s="9">
-        <v>1</v>
-      </c>
       <c r="G29" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I29" t="s">
-        <v>95</v>
+        <v>3</v>
+      </c>
+      <c r="I29" s="7" t="s">
+        <v>58</v>
       </c>
       <c r="J29" t="s">
-        <v>96</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L29" s="2" t="s">
-        <v>215</v>
+        <v>59</v>
+      </c>
+      <c r="L29" s="6" t="s">
+        <v>165</v>
       </c>
       <c r="M29" s="2" t="s">
-        <v>217</v>
+        <v>138</v>
       </c>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B30" s="9">
+        <v>1</v>
+      </c>
+      <c r="E30" s="9">
+        <v>2</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I30" t="s">
+        <v>61</v>
+      </c>
+      <c r="J30" t="s">
+        <v>59</v>
+      </c>
+      <c r="L30" s="6" t="s">
+        <v>166</v>
+      </c>
+      <c r="M30" s="6" t="s">
         <v>62</v>
-      </c>
-      <c r="B30" s="9">
-        <v>1</v>
-      </c>
-      <c r="C30" s="9">
-        <v>2</v>
-      </c>
-      <c r="G30" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="J30" t="s">
-        <v>64</v>
-      </c>
-      <c r="L30" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="M30" s="2" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>65</v>
+        <v>139</v>
       </c>
       <c r="B31" s="9">
         <v>1</v>
       </c>
-      <c r="E31" s="9">
-        <v>2</v>
+      <c r="D31" s="9">
+        <v>3</v>
       </c>
       <c r="G31" s="9">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
+      <c r="H31" s="1">
+        <v>-1</v>
+      </c>
       <c r="I31" t="s">
-        <v>66</v>
+        <v>140</v>
       </c>
       <c r="J31" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L31" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>67</v>
+        <v>199</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>153</v>
+        <v>212</v>
       </c>
       <c r="B32" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="9">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="E32" s="9">
+        <v>1</v>
       </c>
       <c r="G32" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="H32" s="1">
+        <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>154</v>
+        <v>213</v>
       </c>
       <c r="J32" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L32" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="M32" s="2" t="s">
-        <v>155</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="B33" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="9">
         <v>4</v>
@@ -2049,21 +2052,21 @@
         <v>6</v>
       </c>
       <c r="I33" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="J33" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L33" s="6" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="M33" s="2" t="s">
-        <v>192</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
@@ -2079,21 +2082,21 @@
         <v>1</v>
       </c>
       <c r="I34" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="J34" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L34" s="6" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="M34" s="2" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B35" s="9">
         <v>1</v>
@@ -2109,21 +2112,21 @@
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="J35" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="L35" s="6" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="M35" s="2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
@@ -2136,24 +2139,24 @@
         <v>10</v>
       </c>
       <c r="I36" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J36" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="L36" s="6" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="M36" s="2" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B37" s="9">
         <v>1</v>
@@ -2169,21 +2172,21 @@
         <v>3</v>
       </c>
       <c r="I37" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J37" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L37" s="10" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="M37" s="2" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B38" s="9">
         <v>1</v>
@@ -2196,21 +2199,21 @@
         <v>3</v>
       </c>
       <c r="I38" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="J38" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L38" s="10" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="M38" s="2" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B39" s="9">
         <v>1</v>
@@ -2223,21 +2226,21 @@
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="J39" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L39" s="10" t="s">
-        <v>182</v>
+        <v>167</v>
       </c>
       <c r="M39" s="6" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>188</v>
+        <v>169</v>
       </c>
       <c r="B40" s="9">
         <v>2</v>
@@ -2250,171 +2253,179 @@
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>190</v>
+        <v>171</v>
       </c>
       <c r="J40" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>203</v>
+        <v>183</v>
       </c>
       <c r="L40" s="10" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>189</v>
+        <v>170</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>116</v>
+        <v>174</v>
       </c>
       <c r="B41" s="9">
+        <v>1</v>
+      </c>
+      <c r="C41" s="9">
         <v>2</v>
       </c>
       <c r="D41" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G41" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="H41" s="1">
+        <v>-1</v>
       </c>
       <c r="I41" t="s">
-        <v>117</v>
+        <v>172</v>
       </c>
       <c r="J41" t="s">
-        <v>74</v>
-      </c>
-      <c r="L41" s="10"/>
+        <v>69</v>
+      </c>
+      <c r="L41" s="10" t="s">
+        <v>209</v>
+      </c>
       <c r="M41" s="6" t="s">
-        <v>130</v>
+        <v>175</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>193</v>
+        <v>75</v>
       </c>
       <c r="B42" s="9">
-        <v>1</v>
-      </c>
-      <c r="C42" s="9">
         <v>2</v>
       </c>
       <c r="E42" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G42" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H42" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I42" t="s">
-        <v>191</v>
+        <v>76</v>
       </c>
       <c r="J42" t="s">
-        <v>74</v>
-      </c>
-      <c r="L42" s="10" t="s">
-        <v>182</v>
-      </c>
-      <c r="M42" s="6" t="s">
-        <v>194</v>
+        <v>69</v>
+      </c>
+      <c r="L42"/>
+      <c r="M42" s="2" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="B43" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E43" s="9">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="F43" s="9">
+        <v>2</v>
       </c>
       <c r="G43" s="9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="H43" s="1">
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>81</v>
+        <v>109</v>
       </c>
       <c r="J43" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="L43"/>
       <c r="M43" s="2" t="s">
-        <v>162</v>
+        <v>149</v>
       </c>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
       <c r="B44" s="9">
         <v>1</v>
       </c>
       <c r="E44" s="9">
-        <v>2</v>
-      </c>
-      <c r="F44" s="9">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G44" s="9">
         <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H44" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="I44" t="s">
-        <v>118</v>
+        <v>78</v>
       </c>
       <c r="J44" t="s">
-        <v>74</v>
-      </c>
-      <c r="L44"/>
+        <v>69</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L44" s="6" t="s">
+        <v>214</v>
+      </c>
       <c r="M44" s="2" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B45" s="9">
         <v>1</v>
       </c>
-      <c r="E45" s="9">
-        <v>6</v>
+      <c r="C45" s="9">
+        <v>1</v>
+      </c>
+      <c r="D45" s="9">
+        <v>2</v>
       </c>
       <c r="G45" s="9">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>3</v>
+      </c>
+      <c r="H45" s="1">
+        <v>-1</v>
       </c>
       <c r="I45" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="J45" t="s">
-        <v>74</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L45" s="6" t="s">
-        <v>208</v>
+        <v>158</v>
+      </c>
+      <c r="L45" t="s">
+        <v>159</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>191</v>
       </c>
       <c r="B46" s="9">
         <v>1</v>
@@ -2425,273 +2436,207 @@
       <c r="D46" s="9">
         <v>1</v>
       </c>
+      <c r="E46" s="9">
+        <v>1</v>
+      </c>
       <c r="G46" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H46" s="1">
         <v>-1</v>
       </c>
       <c r="I46" t="s">
-        <v>85</v>
+        <v>190</v>
       </c>
       <c r="J46" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
       <c r="L46" t="s">
-        <v>173</v>
+        <v>189</v>
       </c>
       <c r="M46" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>86</v>
+        <v>123</v>
       </c>
       <c r="B47" s="9">
         <v>1</v>
       </c>
-      <c r="C47" s="9">
-        <v>1</v>
-      </c>
-      <c r="D47" s="9">
-        <v>2</v>
+      <c r="E47" s="9">
+        <v>1</v>
       </c>
       <c r="G47" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H47" s="1">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I47" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="J47" t="s">
-        <v>172</v>
-      </c>
-      <c r="L47" t="s">
-        <v>173</v>
-      </c>
-      <c r="M47" s="2" t="s">
-        <v>196</v>
+        <v>82</v>
+      </c>
+      <c r="L47" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="M47" s="6" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>213</v>
+        <v>98</v>
       </c>
       <c r="B48" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C48" s="9">
-        <v>2</v>
-      </c>
-      <c r="D48" s="9">
-        <v>2</v>
-      </c>
-      <c r="E48" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G48" s="9">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H48" s="1">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="I48" t="s">
-        <v>212</v>
+        <v>84</v>
       </c>
       <c r="J48" t="s">
-        <v>172</v>
-      </c>
-      <c r="L48" t="s">
-        <v>211</v>
+        <v>82</v>
+      </c>
+      <c r="L48" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>214</v>
+        <v>178</v>
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>135</v>
+        <v>99</v>
       </c>
       <c r="B49" s="9">
-        <v>1</v>
-      </c>
-      <c r="E49" s="9">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C49" s="9">
+        <v>4</v>
       </c>
       <c r="G49" s="9">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="H49" s="1">
+        <v>-1</v>
       </c>
       <c r="I49" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="J49" t="s">
-        <v>89</v>
-      </c>
-      <c r="L49" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="M49" s="6" t="s">
-        <v>197</v>
+        <v>82</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="M49" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B50" s="9">
         <v>2</v>
       </c>
       <c r="C50" s="9">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G50" s="9">
         <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H50" s="1">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="I50" t="s">
-        <v>91</v>
+        <v>112</v>
       </c>
       <c r="J50" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>198</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B51" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C51" s="9">
         <v>4</v>
       </c>
+      <c r="F51" s="9">
+        <v>1</v>
+      </c>
       <c r="G51" s="9">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H51" s="1">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I51" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="J51" t="s">
-        <v>89</v>
-      </c>
-      <c r="L51" s="2" t="s">
-        <v>167</v>
+        <v>82</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L51" t="s">
+        <v>187</v>
       </c>
       <c r="M51" s="2" t="s">
-        <v>199</v>
+        <v>181</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>120</v>
+        <v>85</v>
       </c>
       <c r="B52" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C52" s="9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="G52" s="9">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I52" t="s">
-        <v>121</v>
+        <v>86</v>
       </c>
       <c r="J52" t="s">
-        <v>89</v>
-      </c>
-      <c r="L52" s="2" t="s">
-        <v>129</v>
+        <v>82</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>188</v>
       </c>
       <c r="M52" s="2" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>122</v>
-      </c>
-      <c r="B53" s="9">
-        <v>1</v>
-      </c>
-      <c r="C53" s="9">
-        <v>4</v>
-      </c>
-      <c r="F53" s="9">
-        <v>1</v>
-      </c>
-      <c r="G53" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H53" s="1">
-        <v>1</v>
-      </c>
-      <c r="I53" t="s">
-        <v>128</v>
-      </c>
-      <c r="J53" t="s">
-        <v>89</v>
-      </c>
-      <c r="K53" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L53" t="s">
-        <v>209</v>
-      </c>
-      <c r="M53" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>92</v>
-      </c>
-      <c r="B54" s="9">
-        <v>1</v>
-      </c>
-      <c r="C54" s="9">
-        <v>7</v>
-      </c>
-      <c r="G54" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I54" t="s">
-        <v>93</v>
-      </c>
-      <c r="J54" t="s">
-        <v>89</v>
-      </c>
-      <c r="K54" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="L54" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="M54" s="2" t="s">
-        <v>202</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
@@ -2720,10 +2665,10 @@
   <sheetData>
     <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2769,7 +2714,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2782,13 +2727,13 @@
   <sheetData>
     <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2796,12 +2741,12 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <f>COUNTA(Deck!C2:C114)</f>
-        <v>24</v>
+        <f>COUNTA(Deck!C2:C112)</f>
+        <v>22</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(Deck!C2:C113)</f>
-        <v>53</v>
+        <f>SUM(Deck!C2:C111)</f>
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -2809,12 +2754,12 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <f>COUNTA(Deck!D2:D114)</f>
-        <v>20</v>
+        <f>COUNTA(Deck!D2:D112)</f>
+        <v>19</v>
       </c>
       <c r="C3" s="1">
-        <f>SUM(Deck!D2:D113)</f>
-        <v>50</v>
+        <f>SUM(Deck!D2:D111)</f>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -2822,11 +2767,11 @@
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <f>COUNTA(Deck!E2:E114)</f>
+        <f>COUNTA(Deck!E2:E112)</f>
         <v>17</v>
       </c>
       <c r="C4" s="1">
-        <f>SUM(Deck!E2:E113)</f>
+        <f>SUM(Deck!E2:E111)</f>
         <v>28</v>
       </c>
     </row>
@@ -2835,11 +2780,11 @@
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <f>COUNTA(Deck!F2:F114)</f>
+        <f>COUNTA(Deck!F2:F112)</f>
         <v>15</v>
       </c>
       <c r="C5" s="1">
-        <f>SUM(Deck!F2:F114)</f>
+        <f>SUM(Deck!F2:F112)</f>
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add some grit to the svg effects
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\project spider monkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1059,13 +1059,13 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
+      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.28515625"/>
-    <col min="2" max="2" width="9.140625" style="9"/>
+    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6.42578125" style="9"/>
     <col min="4" max="4" width="5.5703125" style="9"/>
     <col min="5" max="5" width="6.140625" style="9"/>

</xml_diff>

<commit_message>
add in icons for type desc
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="219">
   <si>
     <t>Name</t>
   </si>
@@ -387,18 +387,6 @@
     <t>wizard-staff</t>
   </si>
   <si>
-    <t>May be purchased for 4 Steel or 3 Stone</t>
-  </si>
-  <si>
-    <t>May be purchased for 3 Steel</t>
-  </si>
-  <si>
-    <t>May be purchased for 3 Steel or 4 Wood</t>
-  </si>
-  <si>
-    <t>May be purchased for 4 Steel or 5 Wood</t>
-  </si>
-  <si>
     <t>Stone Axe</t>
   </si>
   <si>
@@ -459,9 +447,6 @@
     <t>Spray and pray.</t>
   </si>
   <si>
-    <t>May be purchased for 5 Steel or 6 Wood</t>
-  </si>
-  <si>
     <t>Wait, when did this game get futuristic?!?!?</t>
   </si>
   <si>
@@ -489,18 +474,12 @@
     <t>Fun fact: not a good place to be born in.</t>
   </si>
   <si>
-    <t>May be purchased for 4 Steel or 2 Stone</t>
-  </si>
-  <si>
     <t>Gold Mine</t>
   </si>
   <si>
     <t>gold-mine</t>
   </si>
   <si>
-    <t>May also be purchased for 1 Wood, 1 Steel, and 1 Stone.</t>
-  </si>
-  <si>
     <t>There's gold in them there hills!</t>
   </si>
   <si>
@@ -519,12 +498,6 @@
     <t>Save 2 Gold this turn</t>
   </si>
   <si>
-    <t>May be be purchased for 2 Gold</t>
-  </si>
-  <si>
-    <t>May be purchased for 3 Gold</t>
-  </si>
-  <si>
     <t>Save 2 Steel this turn</t>
   </si>
   <si>
@@ -627,9 +600,6 @@
     <t>Save 2 Wood this turn. Pass to another player of your choice at the end of your turn.</t>
   </si>
   <si>
-    <t>May be purchased for 3 Wood</t>
-  </si>
-  <si>
     <t>interactive</t>
   </si>
   <si>
@@ -675,7 +645,46 @@
     <t>*At game end, +1 VP for every three cards in your deck</t>
   </si>
   <si>
-    <t>May be purchased for 2 Stone</t>
+    <t>May be built for 3 Wood</t>
+  </si>
+  <si>
+    <t>May be built for 2 Stone</t>
+  </si>
+  <si>
+    <t>May be built for 3 Steel or 4 Wood</t>
+  </si>
+  <si>
+    <t>May be built for 4 Steel or 5 Wood</t>
+  </si>
+  <si>
+    <t>May be built for 5 Steel or 6 Wood</t>
+  </si>
+  <si>
+    <t>May also be built for 1 Wood, 1 Steel, and 1 Stone.</t>
+  </si>
+  <si>
+    <t>May be be built for 2 Gold</t>
+  </si>
+  <si>
+    <t>May be built for 3 Gold</t>
+  </si>
+  <si>
+    <t>play</t>
+  </si>
+  <si>
+    <t>score</t>
+  </si>
+  <si>
+    <t>May be built for 3 Steel</t>
+  </si>
+  <si>
+    <t>May be built for 4 Steel or 2 Stone</t>
+  </si>
+  <si>
+    <t>May be built for 4 Steel or 3 Stone</t>
+  </si>
+  <si>
+    <t>TypeDesc</t>
   </si>
 </sst>
 </file>
@@ -1053,13 +1062,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:N52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1074,13 +1083,14 @@
     <col min="8" max="8" width="6.140625" style="1"/>
     <col min="9" max="9" width="14.85546875"/>
     <col min="10" max="10" width="10.28515625"/>
-    <col min="11" max="11" width="5.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="73.5703125" style="2"/>
-    <col min="13" max="13" width="40" style="2"/>
-    <col min="14" max="1026" width="8.5703125"/>
+    <col min="11" max="11" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="73.5703125" style="2"/>
+    <col min="14" max="14" width="40" style="2"/>
+    <col min="15" max="1027" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1112,16 +1122,19 @@
         <v>9</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="L1" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="M1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1140,12 +1153,12 @@
       <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="L2"/>
-      <c r="M2" s="6" t="s">
+      <c r="M2"/>
+      <c r="N2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1164,12 +1177,12 @@
       <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="L3"/>
-      <c r="M3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M3"/>
+      <c r="N3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1188,12 +1201,12 @@
       <c r="J4" t="s">
         <v>14</v>
       </c>
-      <c r="L4"/>
-      <c r="M4" t="s">
+      <c r="M4"/>
+      <c r="N4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1212,12 +1225,12 @@
       <c r="J5" t="s">
         <v>14</v>
       </c>
-      <c r="L5"/>
-      <c r="M5" s="6" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M5"/>
+      <c r="N5" s="6" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1236,14 +1249,14 @@
       <c r="J6" t="s">
         <v>14</v>
       </c>
-      <c r="L6"/>
-      <c r="M6" s="6" t="s">
+      <c r="M6"/>
+      <c r="N6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B7" s="9">
         <v>12</v>
@@ -1260,14 +1273,14 @@
       <c r="J7" t="s">
         <v>14</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>95</v>
       </c>
-      <c r="M7" s="6" t="s">
+      <c r="N7" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -1294,16 +1307,19 @@
         <v>27</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L8" t="s">
-        <v>197</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M8" t="s">
+        <v>188</v>
+      </c>
+      <c r="N8" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1330,16 +1346,19 @@
         <v>27</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L9" t="s">
-        <v>197</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M9" t="s">
+        <v>188</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1366,16 +1385,19 @@
         <v>27</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L10" t="s">
-        <v>197</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M10" t="s">
+        <v>188</v>
+      </c>
+      <c r="N10" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>32</v>
       </c>
@@ -1395,14 +1417,17 @@
       <c r="J11" t="s">
         <v>34</v>
       </c>
-      <c r="L11" s="6" t="s">
+      <c r="L11" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M11" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="M11" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
@@ -1425,14 +1450,17 @@
       <c r="J12" t="s">
         <v>34</v>
       </c>
-      <c r="L12" s="6" t="s">
+      <c r="L12" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M12" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="M12" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1458,14 +1486,17 @@
       <c r="J13" t="s">
         <v>34</v>
       </c>
-      <c r="L13" s="6" t="s">
+      <c r="L13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M13" s="6" t="s">
+      <c r="N13" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>41</v>
       </c>
@@ -1491,14 +1522,17 @@
       <c r="J14" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="6" t="s">
+      <c r="L14" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="N14" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>114</v>
       </c>
@@ -1516,18 +1550,21 @@
         <v>115</v>
       </c>
       <c r="J15" t="s">
+        <v>190</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>200</v>
-      </c>
-      <c r="L15" s="10" t="s">
-        <v>198</v>
-      </c>
-      <c r="M15" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>210</v>
       </c>
       <c r="B16" s="9">
         <v>1</v>
@@ -1546,19 +1583,22 @@
         <v>1</v>
       </c>
       <c r="I16" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="J16" t="s">
-        <v>200</v>
-      </c>
-      <c r="L16" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="N16" s="2" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>42</v>
       </c>
@@ -1578,14 +1618,17 @@
       <c r="J17" t="s">
         <v>44</v>
       </c>
-      <c r="L17" s="10" t="s">
-        <v>160</v>
-      </c>
-      <c r="M17" s="6" t="s">
+      <c r="L17" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="N17" s="6" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -1605,14 +1648,17 @@
       <c r="J18" t="s">
         <v>44</v>
       </c>
-      <c r="L18" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="M18" s="6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M18" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>46</v>
       </c>
@@ -1635,16 +1681,19 @@
       <c r="J19" t="s">
         <v>44</v>
       </c>
-      <c r="L19" t="s">
-        <v>162</v>
-      </c>
-      <c r="M19" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L19" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M19" t="s">
+        <v>155</v>
+      </c>
+      <c r="N19" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="B20" s="9">
         <v>2</v>
@@ -1657,19 +1706,22 @@
         <v>4</v>
       </c>
       <c r="I20" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="J20" t="s">
         <v>44</v>
       </c>
-      <c r="L20" s="2" t="s">
-        <v>156</v>
+      <c r="L20" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="N20" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>50</v>
       </c>
@@ -1692,14 +1744,17 @@
       <c r="J21" t="s">
         <v>44</v>
       </c>
-      <c r="L21" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="M21" s="2" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L21" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M21" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="N21" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>48</v>
       </c>
@@ -1722,14 +1777,17 @@
       <c r="J22" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="M22" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L22" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M22" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="N22" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>51</v>
       </c>
@@ -1752,12 +1810,12 @@
       <c r="J23" t="s">
         <v>44</v>
       </c>
-      <c r="L23"/>
-      <c r="M23" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M23"/>
+      <c r="N23" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>101</v>
       </c>
@@ -1780,12 +1838,12 @@
       <c r="J24" t="s">
         <v>44</v>
       </c>
-      <c r="L24" s="6"/>
-      <c r="M24" s="2" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M24" s="6"/>
+      <c r="N24" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1808,16 +1866,19 @@
       <c r="J25" t="s">
         <v>55</v>
       </c>
-      <c r="L25" s="6" t="s">
+      <c r="L25" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M25" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="M25" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N25" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B26" s="9">
         <v>1</v>
@@ -1836,22 +1897,25 @@
         <v>4</v>
       </c>
       <c r="I26" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="J26" t="s">
         <v>89</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>194</v>
+        <v>174</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="M26" s="2" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+      <c r="N26" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>87</v>
       </c>
@@ -1881,49 +1945,55 @@
         <v>89</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>193</v>
+        <v>174</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="M27" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="N27" s="2" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>197</v>
+      </c>
+      <c r="B28" s="9">
+        <v>1</v>
+      </c>
+      <c r="E28" s="9">
+        <v>2</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>198</v>
+      </c>
+      <c r="J28" t="s">
+        <v>194</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M28" s="2" t="s">
         <v>195</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>207</v>
-      </c>
-      <c r="B28" s="9">
-        <v>1</v>
-      </c>
-      <c r="E28" s="9">
-        <v>2</v>
-      </c>
-      <c r="G28" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="H28" s="1">
-        <v>1</v>
-      </c>
-      <c r="I28" t="s">
-        <v>208</v>
-      </c>
-      <c r="J28" t="s">
-        <v>204</v>
-      </c>
-      <c r="K28" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L28" s="2" t="s">
-        <v>205</v>
-      </c>
-      <c r="M28" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N28" s="2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>57</v>
       </c>
@@ -1943,14 +2013,17 @@
       <c r="J29" t="s">
         <v>59</v>
       </c>
-      <c r="L29" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="M29" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M29" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="N29" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>60</v>
       </c>
@@ -1970,16 +2043,19 @@
       <c r="J30" t="s">
         <v>59</v>
       </c>
-      <c r="L30" s="6" t="s">
-        <v>166</v>
+      <c r="L30" s="1" t="s">
+        <v>213</v>
       </c>
       <c r="M30" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="N30" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B31" s="9">
         <v>1</v>
@@ -1995,21 +2071,24 @@
         <v>-1</v>
       </c>
       <c r="I31" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="J31" t="s">
         <v>59</v>
       </c>
-      <c r="L31" s="6" t="s">
-        <v>199</v>
-      </c>
-      <c r="M31" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L31" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M31" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="N31" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="B32" s="9">
         <v>1</v>
@@ -2028,16 +2107,19 @@
         <v>1</v>
       </c>
       <c r="I32" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="J32" t="s">
         <v>59</v>
       </c>
-      <c r="L32" s="6" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M32" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>63</v>
       </c>
@@ -2057,14 +2139,17 @@
       <c r="J33" t="s">
         <v>59</v>
       </c>
-      <c r="L33" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="M33" s="2" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L33" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M33" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="N33" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>103</v>
       </c>
@@ -2087,14 +2172,17 @@
       <c r="J34" t="s">
         <v>59</v>
       </c>
-      <c r="L34" s="6" t="s">
-        <v>122</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L34" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M34" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="N34" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>105</v>
       </c>
@@ -2117,14 +2205,17 @@
       <c r="J35" t="s">
         <v>59</v>
       </c>
-      <c r="L35" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="M35" s="2" t="s">
+      <c r="L35" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M35" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="N35" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>65</v>
       </c>
@@ -2145,16 +2236,19 @@
         <v>59</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L36" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="M36" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="N36" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>73</v>
       </c>
@@ -2177,14 +2271,17 @@
       <c r="J37" t="s">
         <v>69</v>
       </c>
-      <c r="L37" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L37" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M37" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="N37" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>67</v>
       </c>
@@ -2204,14 +2301,17 @@
       <c r="J38" t="s">
         <v>69</v>
       </c>
-      <c r="L38" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="M38" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L38" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M38" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="N38" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>70</v>
       </c>
@@ -2231,16 +2331,19 @@
       <c r="J39" t="s">
         <v>69</v>
       </c>
-      <c r="L39" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="M39" s="6" t="s">
+      <c r="L39" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M39" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="N39" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="B40" s="9">
         <v>2</v>
@@ -2253,24 +2356,27 @@
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="J40" t="s">
         <v>69</v>
       </c>
       <c r="K40" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L40" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="M40" s="6" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="L40" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M40" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="N40" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B41" s="9">
         <v>1</v>
@@ -2289,19 +2395,22 @@
         <v>-1</v>
       </c>
       <c r="I41" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="J41" t="s">
         <v>69</v>
       </c>
-      <c r="L41" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="M41" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L41" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M41" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="N41" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>75</v>
       </c>
@@ -2324,12 +2433,12 @@
       <c r="J42" t="s">
         <v>69</v>
       </c>
-      <c r="L42"/>
-      <c r="M42" s="2" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M42"/>
+      <c r="N42" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>110</v>
       </c>
@@ -2355,12 +2464,12 @@
       <c r="J43" t="s">
         <v>69</v>
       </c>
-      <c r="L43"/>
-      <c r="M43" s="2" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M43"/>
+      <c r="N43" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>77</v>
       </c>
@@ -2381,16 +2490,19 @@
         <v>69</v>
       </c>
       <c r="K44" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L44" s="6" t="s">
+        <v>174</v>
+      </c>
+      <c r="L44" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="M44" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="N44" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -2414,18 +2526,21 @@
         <v>80</v>
       </c>
       <c r="J45" t="s">
-        <v>158</v>
-      </c>
-      <c r="L45" t="s">
-        <v>159</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M45" t="s">
+        <v>152</v>
+      </c>
+      <c r="N45" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B46" s="9">
         <v>1</v>
@@ -2447,21 +2562,24 @@
         <v>-1</v>
       </c>
       <c r="I46" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="J46" t="s">
-        <v>158</v>
-      </c>
-      <c r="L46" t="s">
-        <v>189</v>
-      </c>
-      <c r="M46" s="2" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M46" t="s">
+        <v>180</v>
+      </c>
+      <c r="N46" s="2" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B47" s="9">
         <v>1</v>
@@ -2479,14 +2597,17 @@
       <c r="J47" t="s">
         <v>82</v>
       </c>
-      <c r="L47" s="6" t="s">
+      <c r="L47" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="M47" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="N47" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="M47" s="6" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>98</v>
       </c>
@@ -2509,14 +2630,17 @@
       <c r="J48" t="s">
         <v>82</v>
       </c>
-      <c r="L48" s="2" t="s">
-        <v>120</v>
+      <c r="L48" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="M48" s="2" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="N48" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -2539,14 +2663,17 @@
       <c r="J49" t="s">
         <v>82</v>
       </c>
-      <c r="L49" s="2" t="s">
-        <v>153</v>
+      <c r="L49" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="M49" s="2" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="N49" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>111</v>
       </c>
@@ -2566,14 +2693,17 @@
       <c r="J50" t="s">
         <v>82</v>
       </c>
-      <c r="L50" s="2" t="s">
-        <v>119</v>
+      <c r="L50" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="M50" s="2" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="N50" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>113</v>
       </c>
@@ -2600,16 +2730,19 @@
         <v>82</v>
       </c>
       <c r="K51" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L51" t="s">
-        <v>187</v>
-      </c>
-      <c r="M51" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M51" t="s">
+        <v>178</v>
+      </c>
+      <c r="N51" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>85</v>
       </c>
@@ -2630,13 +2763,16 @@
         <v>82</v>
       </c>
       <c r="K52" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="L52" s="6" t="s">
-        <v>188</v>
-      </c>
-      <c r="M52" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
+      </c>
+      <c r="L52" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="N52" s="2" t="s">
+        <v>173</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new backs, stage icons, a json, many more
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\project spider monkey\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\project spider monkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A9948-4751-40AC-8BCA-314A686E9798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="989"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Deck" sheetId="1" r:id="rId1"/>
@@ -23,12 +24,12 @@
     <definedName name="WoodValue">VPs!$B$2</definedName>
     <definedName name="WoodVP">VPs!$B$2</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="224">
   <si>
     <t>Name</t>
   </si>
@@ -685,12 +686,27 @@
   </si>
   <si>
     <t>TypeDesc</t>
+  </si>
+  <si>
+    <t>Gold Stack</t>
+  </si>
+  <si>
+    <t>gold-stack</t>
+  </si>
+  <si>
+    <t>Maybe also be used for any 2 Resources.</t>
+  </si>
+  <si>
+    <t>You're welcome.</t>
+  </si>
+  <si>
+    <t>Stage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -851,6 +867,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -886,6 +919,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1061,36 +1111,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N52"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" style="9"/>
-    <col min="4" max="4" width="5.5703125" style="9"/>
-    <col min="5" max="5" width="6.140625" style="9"/>
-    <col min="6" max="6" width="5.28515625" style="9"/>
-    <col min="7" max="7" width="9.140625" style="9"/>
-    <col min="8" max="8" width="6.140625" style="1"/>
-    <col min="9" max="9" width="14.85546875"/>
-    <col min="10" max="10" width="10.28515625"/>
-    <col min="11" max="11" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="73.5703125" style="2"/>
-    <col min="14" max="14" width="40" style="2"/>
-    <col min="15" max="1027" width="8.5703125"/>
+    <col min="1" max="1" width="15.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" style="9"/>
+    <col min="4" max="4" width="5.54296875" style="9"/>
+    <col min="5" max="5" width="6.1796875" style="9"/>
+    <col min="6" max="6" width="5.26953125" style="9"/>
+    <col min="7" max="7" width="9.1796875" style="9"/>
+    <col min="8" max="8" width="6.1796875" style="1"/>
+    <col min="9" max="9" width="14.81640625"/>
+    <col min="10" max="10" width="10.26953125"/>
+    <col min="11" max="11" width="5.36328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="6.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="73.54296875" style="2"/>
+    <col min="15" max="15" width="40" style="2"/>
+    <col min="16" max="1028" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1121,20 +1172,23 @@
       <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>218</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="O1" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1153,12 +1207,16 @@
       <c r="J2" t="s">
         <v>14</v>
       </c>
-      <c r="M2"/>
-      <c r="N2" s="6" t="s">
+      <c r="K2" s="1" t="str">
+        <f>IF(G2=0,"start", IF(G2&lt;5,"early","late"))</f>
+        <v>start</v>
+      </c>
+      <c r="N2"/>
+      <c r="O2" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -1177,12 +1235,16 @@
       <c r="J3" t="s">
         <v>14</v>
       </c>
-      <c r="M3"/>
-      <c r="N3" t="s">
+      <c r="K3" s="1" t="str">
+        <f>IF(G3=0,"start", IF(G3&lt;5,"early","late"))</f>
+        <v>start</v>
+      </c>
+      <c r="N3"/>
+      <c r="O3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>94</v>
       </c>
@@ -1201,12 +1263,16 @@
       <c r="J4" t="s">
         <v>14</v>
       </c>
-      <c r="M4"/>
-      <c r="N4" t="s">
+      <c r="K4" s="1" t="str">
+        <f t="shared" ref="K4:K53" si="0">IF(G4=0,"start", IF(G4&lt;5,"early","late"))</f>
+        <v>start</v>
+      </c>
+      <c r="N4"/>
+      <c r="O4" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -1225,12 +1291,16 @@
       <c r="J5" t="s">
         <v>14</v>
       </c>
-      <c r="M5"/>
-      <c r="N5" s="6" t="s">
+      <c r="K5" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>start</v>
+      </c>
+      <c r="N5"/>
+      <c r="O5" s="6" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -1249,12 +1319,16 @@
       <c r="J6" t="s">
         <v>14</v>
       </c>
-      <c r="M6"/>
-      <c r="N6" s="6" t="s">
+      <c r="K6" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>start</v>
+      </c>
+      <c r="N6"/>
+      <c r="O6" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>193</v>
       </c>
@@ -1273,244 +1347,262 @@
       <c r="J7" t="s">
         <v>14</v>
       </c>
-      <c r="M7" t="s">
+      <c r="K7" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>start</v>
+      </c>
+      <c r="N7" t="s">
         <v>95</v>
       </c>
-      <c r="N7" s="6" t="s">
+      <c r="O7" s="6" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="9">
+        <v>4</v>
+      </c>
+      <c r="F8" s="9">
+        <v>2</v>
+      </c>
+      <c r="G8" s="9">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>220</v>
+      </c>
+      <c r="J8" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>start</v>
+      </c>
+      <c r="N8" t="s">
+        <v>221</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="9">
-        <v>1</v>
-      </c>
-      <c r="C8" s="9">
-        <v>2</v>
-      </c>
-      <c r="E8" s="9">
-        <v>1</v>
-      </c>
-      <c r="F8" s="9">
-        <v>1</v>
-      </c>
-      <c r="G8" s="9">
-        <f t="shared" ref="G8:G52" si="0">ROUND(C8*WoodVP+D8*SteelVP+E8*StoneVP+F8*GoldVP,0) + H8</f>
+      <c r="B9" s="9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="9">
+        <v>1</v>
+      </c>
+      <c r="G9" s="9">
+        <f t="shared" ref="G9:G53" si="1">ROUND(C9*WoodVP+D9*SteelVP+E9*StoneVP+F9*GoldVP,0) + H9</f>
         <v>6</v>
       </c>
-      <c r="I8" t="s">
+      <c r="I9" t="s">
         <v>26</v>
-      </c>
-      <c r="J8" t="s">
-        <v>27</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="M8" t="s">
-        <v>188</v>
-      </c>
-      <c r="N8" s="2" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2</v>
-      </c>
-      <c r="D9" s="9">
-        <v>1</v>
-      </c>
-      <c r="F9" s="9">
-        <v>1</v>
-      </c>
-      <c r="G9" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="I9" t="s">
-        <v>29</v>
       </c>
       <c r="J9" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="K9" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="M9" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>188</v>
       </c>
-      <c r="N9" s="2" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O9" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B10" s="9">
         <v>1</v>
       </c>
+      <c r="C10" s="9">
+        <v>2</v>
+      </c>
       <c r="D10" s="9">
-        <v>2</v>
-      </c>
-      <c r="E10" s="9">
         <v>1</v>
       </c>
       <c r="F10" s="9">
         <v>1</v>
       </c>
       <c r="G10" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="J10" t="s">
         <v>27</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="K10" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="M10" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>188</v>
       </c>
-      <c r="N10" s="2" t="s">
+      <c r="O10" s="2" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1</v>
+      </c>
+      <c r="G11" s="9">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N11" t="s">
+        <v>188</v>
+      </c>
+      <c r="O11" s="2" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="9">
-        <v>1</v>
-      </c>
-      <c r="C11" s="9">
-        <v>1</v>
-      </c>
-      <c r="G11" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I11" t="s">
+      <c r="B12" s="9">
+        <v>1</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="G12" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I12" t="s">
         <v>33</v>
-      </c>
-      <c r="J11" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M11" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="N11" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>35</v>
-      </c>
-      <c r="B12" s="9">
-        <v>1</v>
-      </c>
-      <c r="D12" s="9">
-        <v>2</v>
-      </c>
-      <c r="G12" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H12" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I12" t="s">
-        <v>36</v>
       </c>
       <c r="J12" t="s">
         <v>34</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="K12" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M12" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M12" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="N12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N12" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="O12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B13" s="9">
         <v>1</v>
       </c>
-      <c r="C13" s="9">
-        <v>1</v>
-      </c>
-      <c r="E13" s="9">
-        <v>1</v>
+      <c r="D13" s="9">
+        <v>2</v>
       </c>
       <c r="G13" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H13" s="1">
         <v>-1</v>
       </c>
       <c r="I13" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="J13" t="s">
         <v>34</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="K13" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M13" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M13" s="6" t="s">
-        <v>39</v>
-      </c>
       <c r="N13" s="6" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="O13" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B14" s="9">
         <v>1</v>
       </c>
-      <c r="D14" s="9">
+      <c r="C14" s="9">
         <v>1</v>
       </c>
       <c r="E14" s="9">
         <v>1</v>
       </c>
       <c r="G14" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="H14" s="1">
@@ -1522,274 +1614,313 @@
       <c r="J14" t="s">
         <v>34</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="K14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M14" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M14" s="6" t="s">
+      <c r="N14" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="N14" s="6" t="s">
+      <c r="O14" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="D15" s="9">
+        <v>1</v>
+      </c>
+      <c r="E15" s="9">
+        <v>1</v>
+      </c>
+      <c r="G15" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H15" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I15" t="s">
+        <v>38</v>
+      </c>
+      <c r="J15" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N15" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O15" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>114</v>
       </c>
-      <c r="B15" s="9">
-        <v>1</v>
-      </c>
-      <c r="C15" s="9">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="I15" t="s">
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9">
+        <v>1</v>
+      </c>
+      <c r="G16" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I16" t="s">
         <v>115</v>
-      </c>
-      <c r="J15" t="s">
-        <v>190</v>
-      </c>
-      <c r="L15" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M15" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="N15" s="6" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>200</v>
-      </c>
-      <c r="B16" s="9">
-        <v>1</v>
-      </c>
-      <c r="C16" s="9">
-        <v>1</v>
-      </c>
-      <c r="D16" s="9">
-        <v>1</v>
-      </c>
-      <c r="G16" s="9">
-        <f t="shared" ref="G16" si="1">ROUND(C16*WoodVP+D16*SteelVP+E16*StoneVP+F16*GoldVP,0) + H16</f>
-        <v>4</v>
-      </c>
-      <c r="H16" s="1">
-        <v>1</v>
-      </c>
-      <c r="I16" t="s">
-        <v>201</v>
       </c>
       <c r="J16" t="s">
         <v>190</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="K16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M16" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="N16" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="O16" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>200</v>
+      </c>
+      <c r="B17" s="9">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9">
+        <v>1</v>
+      </c>
+      <c r="D17" s="9">
+        <v>1</v>
+      </c>
+      <c r="G17" s="9">
+        <f t="shared" ref="G17" si="2">ROUND(C17*WoodVP+D17*SteelVP+E17*StoneVP+F17*GoldVP,0) + H17</f>
+        <v>4</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+      <c r="I17" t="s">
+        <v>201</v>
+      </c>
+      <c r="J17" t="s">
+        <v>190</v>
+      </c>
+      <c r="K17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N17" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="N16" s="2" t="s">
+      <c r="O17" s="2" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="9">
-        <v>1</v>
-      </c>
-      <c r="F17" s="9">
-        <v>1</v>
-      </c>
-      <c r="G17" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+      <c r="F18" s="9">
+        <v>1</v>
+      </c>
+      <c r="G18" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I18" t="s">
         <v>43</v>
-      </c>
-      <c r="J17" t="s">
-        <v>44</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M17" s="10" t="s">
-        <v>153</v>
-      </c>
-      <c r="N17" s="6" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" s="9">
-        <v>1</v>
-      </c>
-      <c r="F18" s="9">
-        <v>1</v>
-      </c>
-      <c r="G18" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I18" t="s">
-        <v>108</v>
       </c>
       <c r="J18" t="s">
         <v>44</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="K18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M18" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M18" s="10" t="s">
-        <v>154</v>
-      </c>
-      <c r="N18" s="6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N18" s="10" t="s">
+        <v>153</v>
+      </c>
+      <c r="O18" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>46</v>
+        <v>107</v>
       </c>
       <c r="B19" s="9">
         <v>1</v>
       </c>
       <c r="F19" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G19" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="H19" s="1">
-        <v>-2</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="I19" t="s">
-        <v>47</v>
+        <v>108</v>
       </c>
       <c r="J19" t="s">
         <v>44</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="K19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M19" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M19" t="s">
-        <v>155</v>
-      </c>
-      <c r="N19" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N19" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="O19" s="6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>148</v>
+        <v>46</v>
       </c>
       <c r="B20" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F20" s="9">
         <v>2</v>
       </c>
       <c r="G20" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="H20" s="1">
+        <v>-2</v>
       </c>
       <c r="I20" t="s">
-        <v>149</v>
+        <v>47</v>
       </c>
       <c r="J20" t="s">
         <v>44</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="N20" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N20" t="s">
+        <v>155</v>
+      </c>
+      <c r="O20" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="B21" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F21" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G21" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H21" s="1">
-        <v>-1</v>
-      </c>
       <c r="I21" t="s">
-        <v>100</v>
+        <v>149</v>
       </c>
       <c r="J21" t="s">
         <v>44</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="K21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M21" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M21" s="10" t="s">
-        <v>211</v>
-      </c>
       <c r="N21" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+        <v>210</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B22" s="9">
         <v>1</v>
       </c>
       <c r="F22" s="9">
+        <v>3</v>
+      </c>
+      <c r="G22" s="9">
+        <f t="shared" si="1"/>
         <v>4</v>
-      </c>
-      <c r="G22" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
       </c>
       <c r="H22" s="1">
         <v>-1</v>
       </c>
       <c r="I22" t="s">
-        <v>49</v>
+        <v>100</v>
       </c>
       <c r="J22" t="s">
         <v>44</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="K22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M22" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M22" s="6" t="s">
-        <v>212</v>
-      </c>
-      <c r="N22" s="2" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N22" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="O22" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B23" s="9">
         <v>1</v>
@@ -1798,861 +1929,965 @@
         <v>4</v>
       </c>
       <c r="G23" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="H23" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I23" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="J23" t="s">
         <v>44</v>
       </c>
-      <c r="M23"/>
-      <c r="N23" s="2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="M23" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="N23" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>101</v>
+        <v>51</v>
       </c>
       <c r="B24" s="9">
         <v>1</v>
       </c>
       <c r="F24" s="9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G24" s="9">
-        <f t="shared" si="0"/>
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="H24" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I24" t="s">
-        <v>102</v>
+        <v>52</v>
       </c>
       <c r="J24" t="s">
         <v>44</v>
       </c>
-      <c r="M24" s="6"/>
-      <c r="N24" s="2" t="s">
+      <c r="K24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="N24"/>
+      <c r="O24" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>101</v>
+      </c>
+      <c r="B25" s="9">
+        <v>1</v>
+      </c>
+      <c r="F25" s="9">
+        <v>6</v>
+      </c>
+      <c r="G25" s="9">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H25" s="1">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>102</v>
+      </c>
+      <c r="J25" t="s">
+        <v>44</v>
+      </c>
+      <c r="K25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="N25" s="6"/>
+      <c r="O25" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="9">
-        <v>1</v>
-      </c>
-      <c r="C25" s="9">
-        <v>2</v>
-      </c>
-      <c r="G25" s="9">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="H25" s="1">
+      <c r="B26" s="9">
+        <v>1</v>
+      </c>
+      <c r="C26" s="9">
+        <v>2</v>
+      </c>
+      <c r="G26" s="9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="H26" s="1">
         <v>-2</v>
       </c>
-      <c r="I25" t="s">
+      <c r="I26" t="s">
         <v>54</v>
       </c>
-      <c r="J25" t="s">
+      <c r="J26" t="s">
         <v>55</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="K26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M26" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M25" s="6" t="s">
+      <c r="N26" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="O26" s="2" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="9">
-        <v>1</v>
-      </c>
-      <c r="C26" s="9">
-        <v>1</v>
-      </c>
-      <c r="D26" s="9">
-        <v>1</v>
-      </c>
-      <c r="E26" s="9">
-        <v>1</v>
-      </c>
-      <c r="G26" s="9">
-        <f t="shared" ref="G26" si="2">ROUND(C26*WoodVP+D26*SteelVP+E26*StoneVP+F26*GoldVP,0) + H26</f>
+      <c r="B27" s="9">
+        <v>1</v>
+      </c>
+      <c r="C27" s="9">
+        <v>1</v>
+      </c>
+      <c r="D27" s="9">
+        <v>1</v>
+      </c>
+      <c r="E27" s="9">
+        <v>1</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" ref="G27" si="3">ROUND(C27*WoodVP+D27*SteelVP+E27*StoneVP+F27*GoldVP,0) + H27</f>
         <v>4</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I27" t="s">
         <v>146</v>
-      </c>
-      <c r="J26" t="s">
-        <v>89</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L26" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>185</v>
-      </c>
-      <c r="N26" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>87</v>
-      </c>
-      <c r="B27" s="9">
-        <v>1</v>
-      </c>
-      <c r="C27" s="9">
-        <v>2</v>
-      </c>
-      <c r="D27" s="9">
-        <v>2</v>
-      </c>
-      <c r="E27" s="9">
-        <v>1</v>
-      </c>
-      <c r="F27" s="9">
-        <v>1</v>
-      </c>
-      <c r="G27" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="I27" t="s">
-        <v>88</v>
       </c>
       <c r="J27" t="s">
         <v>89</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="K27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="L27" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L27" s="1" t="s">
+      <c r="M27" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="M27" s="2" t="s">
+      <c r="N27" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="9">
+        <v>1</v>
+      </c>
+      <c r="C28" s="9">
+        <v>2</v>
+      </c>
+      <c r="D28" s="9">
+        <v>2</v>
+      </c>
+      <c r="E28" s="9">
+        <v>1</v>
+      </c>
+      <c r="F28" s="9">
+        <v>1</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I28" t="s">
+        <v>88</v>
+      </c>
+      <c r="J28" t="s">
+        <v>89</v>
+      </c>
+      <c r="K28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N28" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="N27" s="2" t="s">
+      <c r="O28" s="2" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
         <v>197</v>
       </c>
-      <c r="B28" s="9">
-        <v>1</v>
-      </c>
-      <c r="E28" s="9">
-        <v>2</v>
-      </c>
-      <c r="G28" s="9">
-        <f t="shared" si="0"/>
+      <c r="B29" s="9">
+        <v>1</v>
+      </c>
+      <c r="E29" s="9">
+        <v>2</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="H28" s="1">
-        <v>1</v>
-      </c>
-      <c r="I28" t="s">
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
         <v>198</v>
       </c>
-      <c r="J28" t="s">
+      <c r="J29" t="s">
         <v>194</v>
       </c>
-      <c r="K28" s="1" t="s">
+      <c r="K29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L28" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="M28" s="2" t="s">
+      <c r="N29" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="N28" s="2" t="s">
+      <c r="O29" s="2" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
         <v>57</v>
       </c>
-      <c r="B29" s="9">
-        <v>1</v>
-      </c>
-      <c r="C29" s="9">
-        <v>2</v>
-      </c>
-      <c r="G29" s="9">
-        <f t="shared" si="0"/>
+      <c r="B30" s="9">
+        <v>1</v>
+      </c>
+      <c r="C30" s="9">
+        <v>2</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I30" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="J29" t="s">
-        <v>59</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M29" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="N29" s="2" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B30" s="9">
-        <v>1</v>
-      </c>
-      <c r="E30" s="9">
-        <v>2</v>
-      </c>
-      <c r="G30" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I30" t="s">
-        <v>61</v>
       </c>
       <c r="J30" t="s">
         <v>59</v>
       </c>
-      <c r="L30" s="1" t="s">
+      <c r="K30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M30" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M30" s="6" t="s">
-        <v>157</v>
-      </c>
       <c r="N30" s="6" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>135</v>
+        <v>60</v>
       </c>
       <c r="B31" s="9">
         <v>1</v>
       </c>
-      <c r="D31" s="9">
+      <c r="E31" s="9">
+        <v>2</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G31" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H31" s="1">
-        <v>-1</v>
-      </c>
       <c r="I31" t="s">
-        <v>136</v>
+        <v>61</v>
       </c>
       <c r="J31" t="s">
         <v>59</v>
       </c>
-      <c r="L31" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="M31" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="N31" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N31" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="O31" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>202</v>
+        <v>135</v>
       </c>
       <c r="B32" s="9">
         <v>1</v>
       </c>
       <c r="D32" s="9">
-        <v>2</v>
-      </c>
-      <c r="E32" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G32" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="H32" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I32" t="s">
-        <v>203</v>
+        <v>136</v>
       </c>
       <c r="J32" t="s">
         <v>59</v>
       </c>
-      <c r="L32" s="1" t="s">
+      <c r="K32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M32" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M32" s="6" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N32" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="O32" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>63</v>
+        <v>202</v>
       </c>
       <c r="B33" s="9">
         <v>1</v>
       </c>
       <c r="D33" s="9">
-        <v>4</v>
+        <v>2</v>
+      </c>
+      <c r="E33" s="9">
+        <v>1</v>
       </c>
       <c r="G33" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H33" s="1">
+        <v>1</v>
       </c>
       <c r="I33" t="s">
-        <v>64</v>
+        <v>203</v>
       </c>
       <c r="J33" t="s">
         <v>59</v>
       </c>
-      <c r="L33" s="1" t="s">
+      <c r="K33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="M33" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M33" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="N33" s="2" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N33" s="6" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>63</v>
       </c>
       <c r="B34" s="9">
         <v>1</v>
       </c>
       <c r="D34" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G34" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H34" s="1">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="I34" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="J34" t="s">
         <v>59</v>
       </c>
-      <c r="L34" s="1" t="s">
+      <c r="K34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="M34" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M34" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="N34" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N34" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="O34" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B35" s="9">
         <v>1</v>
       </c>
       <c r="D35" s="9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G35" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
       </c>
       <c r="H35" s="1">
         <v>1</v>
       </c>
       <c r="I35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J35" t="s">
         <v>59</v>
       </c>
-      <c r="L35" s="1" t="s">
+      <c r="K35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="M35" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M35" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="N35" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="N35" s="6" t="s">
+        <v>208</v>
+      </c>
+      <c r="O35" s="2" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>65</v>
+        <v>105</v>
       </c>
       <c r="B36" s="9">
         <v>1</v>
       </c>
       <c r="D36" s="9">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G36" s="9">
-        <f t="shared" si="0"/>
-        <v>10</v>
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H36" s="1">
+        <v>1</v>
       </c>
       <c r="I36" t="s">
-        <v>66</v>
+        <v>106</v>
       </c>
       <c r="J36" t="s">
         <v>59</v>
       </c>
-      <c r="K36" s="1" t="s">
+      <c r="K36" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="M36" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="N36" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="O36" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>65</v>
+      </c>
+      <c r="B37" s="9">
+        <v>1</v>
+      </c>
+      <c r="D37" s="9">
+        <v>7</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I37" t="s">
+        <v>66</v>
+      </c>
+      <c r="J37" t="s">
+        <v>59</v>
+      </c>
+      <c r="K37" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="L37" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L36" s="1" t="s">
+      <c r="M37" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="M36" s="6" t="s">
+      <c r="N37" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="N36" s="2" t="s">
+      <c r="O37" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
         <v>73</v>
       </c>
-      <c r="B37" s="9">
-        <v>1</v>
-      </c>
-      <c r="C37" s="9">
-        <v>1</v>
-      </c>
-      <c r="E37" s="9">
-        <v>1</v>
-      </c>
-      <c r="G37" s="9">
-        <f t="shared" si="0"/>
+      <c r="B38" s="9">
+        <v>1</v>
+      </c>
+      <c r="C38" s="9">
+        <v>1</v>
+      </c>
+      <c r="E38" s="9">
+        <v>1</v>
+      </c>
+      <c r="G38" s="9">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="I37" t="s">
+      <c r="I38" t="s">
         <v>74</v>
-      </c>
-      <c r="J37" t="s">
-        <v>69</v>
-      </c>
-      <c r="L37" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M37" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="N37" s="2" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>67</v>
-      </c>
-      <c r="B38" s="9">
-        <v>1</v>
-      </c>
-      <c r="D38" s="9">
-        <v>2</v>
-      </c>
-      <c r="G38" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="I38" t="s">
-        <v>68</v>
       </c>
       <c r="J38" t="s">
         <v>69</v>
       </c>
-      <c r="L38" s="1" t="s">
+      <c r="K38" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M38" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M38" s="10" t="s">
+      <c r="N38" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="N38" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O38" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B39" s="9">
         <v>1</v>
       </c>
-      <c r="C39" s="9">
+      <c r="D39" s="9">
         <v>2</v>
       </c>
       <c r="G39" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I39" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J39" t="s">
         <v>69</v>
       </c>
-      <c r="L39" s="1" t="s">
+      <c r="K39" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M39" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M39" s="10" t="s">
+      <c r="N39" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="N39" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O39" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>160</v>
+        <v>70</v>
       </c>
       <c r="B40" s="9">
-        <v>2</v>
-      </c>
-      <c r="E40" s="9">
+        <v>1</v>
+      </c>
+      <c r="C40" s="9">
         <v>2</v>
       </c>
       <c r="G40" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="I40" t="s">
-        <v>162</v>
+        <v>71</v>
       </c>
       <c r="J40" t="s">
         <v>69</v>
       </c>
-      <c r="K40" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L40" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="M40" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="N40" s="6" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K40" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M40" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N40" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="O40" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B41" s="9">
-        <v>1</v>
-      </c>
-      <c r="C41" s="9">
-        <v>2</v>
-      </c>
-      <c r="D41" s="9">
+        <v>2</v>
+      </c>
+      <c r="E41" s="9">
+        <v>2</v>
+      </c>
+      <c r="G41" s="9">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G41" s="9">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="H41" s="1">
-        <v>-1</v>
-      </c>
       <c r="I41" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="J41" t="s">
         <v>69</v>
       </c>
+      <c r="K41" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
       <c r="L41" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M41" s="10" t="s">
-        <v>199</v>
-      </c>
-      <c r="N41" s="6" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+      <c r="M41" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N41" s="10" t="s">
+        <v>177</v>
+      </c>
+      <c r="O41" s="6" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>75</v>
+        <v>165</v>
       </c>
       <c r="B42" s="9">
-        <v>2</v>
-      </c>
-      <c r="E42" s="9">
+        <v>1</v>
+      </c>
+      <c r="C42" s="9">
+        <v>2</v>
+      </c>
+      <c r="D42" s="9">
         <v>3</v>
       </c>
       <c r="G42" s="9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="H42" s="1">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="I42" t="s">
-        <v>76</v>
+        <v>163</v>
       </c>
       <c r="J42" t="s">
         <v>69</v>
       </c>
-      <c r="M42"/>
-      <c r="N42" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K42" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="M42" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N42" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="O42" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>110</v>
+        <v>75</v>
       </c>
       <c r="B43" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" s="9">
-        <v>2</v>
-      </c>
-      <c r="F43" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G43" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
+        <f t="shared" si="1"/>
+        <v>6</v>
       </c>
       <c r="H43" s="1">
         <v>1</v>
       </c>
       <c r="I43" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="J43" t="s">
         <v>69</v>
       </c>
-      <c r="M43"/>
-      <c r="N43" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K43" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="N43"/>
+      <c r="O43" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="B44" s="9">
         <v>1</v>
       </c>
       <c r="E44" s="9">
-        <v>6</v>
+        <v>2</v>
+      </c>
+      <c r="F44" s="9">
+        <v>2</v>
       </c>
       <c r="G44" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H44" s="1">
+        <v>1</v>
       </c>
       <c r="I44" t="s">
-        <v>78</v>
+        <v>109</v>
       </c>
       <c r="J44" t="s">
         <v>69</v>
       </c>
-      <c r="K44" s="1" t="s">
+      <c r="K44" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="N44"/>
+      <c r="O44" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" s="9">
+        <v>1</v>
+      </c>
+      <c r="E45" s="9">
+        <v>6</v>
+      </c>
+      <c r="G45" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I45" t="s">
+        <v>78</v>
+      </c>
+      <c r="J45" t="s">
+        <v>69</v>
+      </c>
+      <c r="K45" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="L45" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="M45" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="M44" s="6" t="s">
+      <c r="N45" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="O45" s="2" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="9">
-        <v>1</v>
-      </c>
-      <c r="C45" s="9">
-        <v>1</v>
-      </c>
-      <c r="D45" s="9">
-        <v>2</v>
-      </c>
-      <c r="G45" s="9">
-        <f t="shared" si="0"/>
+      <c r="B46" s="9">
+        <v>1</v>
+      </c>
+      <c r="C46" s="9">
+        <v>1</v>
+      </c>
+      <c r="D46" s="9">
+        <v>2</v>
+      </c>
+      <c r="G46" s="9">
+        <f t="shared" si="1"/>
         <v>3</v>
-      </c>
-      <c r="H45" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I45" t="s">
-        <v>80</v>
-      </c>
-      <c r="J45" t="s">
-        <v>151</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M45" t="s">
-        <v>152</v>
-      </c>
-      <c r="N45" s="2" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>182</v>
-      </c>
-      <c r="B46" s="9">
-        <v>1</v>
-      </c>
-      <c r="C46" s="9">
-        <v>2</v>
-      </c>
-      <c r="D46" s="9">
-        <v>1</v>
-      </c>
-      <c r="E46" s="9">
-        <v>1</v>
-      </c>
-      <c r="G46" s="9">
-        <f t="shared" si="0"/>
-        <v>5</v>
       </c>
       <c r="H46" s="1">
         <v>-1</v>
       </c>
       <c r="I46" t="s">
-        <v>181</v>
+        <v>80</v>
       </c>
       <c r="J46" t="s">
         <v>151</v>
       </c>
-      <c r="L46" s="1" t="s">
+      <c r="K46" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M46" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="M46" t="s">
+      <c r="N46" t="s">
+        <v>152</v>
+      </c>
+      <c r="O46" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>182</v>
+      </c>
+      <c r="B47" s="9">
+        <v>1</v>
+      </c>
+      <c r="C47" s="9">
+        <v>2</v>
+      </c>
+      <c r="D47" s="9">
+        <v>1</v>
+      </c>
+      <c r="E47" s="9">
+        <v>1</v>
+      </c>
+      <c r="G47" s="9">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H47" s="1">
+        <v>-1</v>
+      </c>
+      <c r="I47" t="s">
+        <v>181</v>
+      </c>
+      <c r="J47" t="s">
+        <v>151</v>
+      </c>
+      <c r="K47" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="M47" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N47" t="s">
         <v>180</v>
       </c>
-      <c r="N46" s="2" t="s">
+      <c r="O47" s="2" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
         <v>119</v>
       </c>
-      <c r="B47" s="9">
-        <v>1</v>
-      </c>
-      <c r="E47" s="9">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="I47" t="s">
+      <c r="B48" s="9">
+        <v>1</v>
+      </c>
+      <c r="E48" s="9">
+        <v>1</v>
+      </c>
+      <c r="G48" s="9">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="I48" t="s">
         <v>81</v>
-      </c>
-      <c r="J47" t="s">
-        <v>82</v>
-      </c>
-      <c r="L47" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="M47" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="N47" s="6" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>98</v>
-      </c>
-      <c r="B48" s="9">
-        <v>2</v>
-      </c>
-      <c r="C48" s="9">
-        <v>3</v>
-      </c>
-      <c r="G48" s="9">
-        <f t="shared" si="0"/>
-        <v>3</v>
-      </c>
-      <c r="H48" s="1">
-        <v>-1</v>
-      </c>
-      <c r="I48" t="s">
-        <v>84</v>
       </c>
       <c r="J48" t="s">
         <v>82</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="M48" s="2" t="s">
-        <v>215</v>
-      </c>
-      <c r="N48" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K48" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M48" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="N48" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="O48" s="6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B49" s="9">
         <v>2</v>
       </c>
       <c r="C49" s="9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G49" s="9">
-        <f t="shared" si="0"/>
-        <v>4</v>
+        <f t="shared" si="1"/>
+        <v>3</v>
       </c>
       <c r="H49" s="1">
         <v>-1</v>
@@ -2663,121 +2898,174 @@
       <c r="J49" t="s">
         <v>82</v>
       </c>
-      <c r="L49" s="1" t="s">
+      <c r="K49" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M49" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M49" s="2" t="s">
-        <v>216</v>
-      </c>
       <c r="N49" s="2" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+        <v>215</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B50" s="9">
         <v>2</v>
       </c>
       <c r="C50" s="9">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G50" s="9">
-        <f t="shared" si="0"/>
-        <v>7</v>
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H50" s="1">
+        <v>-1</v>
       </c>
       <c r="I50" t="s">
-        <v>112</v>
+        <v>84</v>
       </c>
       <c r="J50" t="s">
         <v>82</v>
       </c>
-      <c r="L50" s="1" t="s">
+      <c r="K50" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>early</v>
+      </c>
+      <c r="M50" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="M50" s="2" t="s">
-        <v>217</v>
-      </c>
       <c r="N50" s="2" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+        <v>216</v>
+      </c>
+      <c r="O50" s="2" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B51" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C51" s="9">
-        <v>4</v>
-      </c>
-      <c r="F51" s="9">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G51" s="9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="H51" s="1">
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>7</v>
       </c>
       <c r="I51" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="J51" t="s">
         <v>82</v>
       </c>
-      <c r="K51" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="L51" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="M51" t="s">
-        <v>178</v>
+      <c r="K51" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>151</v>
       </c>
       <c r="N51" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="O51" s="2" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>85</v>
+        <v>113</v>
       </c>
       <c r="B52" s="9">
         <v>1</v>
       </c>
       <c r="C52" s="9">
-        <v>7</v>
+        <v>4</v>
+      </c>
+      <c r="F52" s="9">
+        <v>1</v>
       </c>
       <c r="G52" s="9">
-        <f t="shared" si="0"/>
-        <v>9</v>
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H52" s="1">
+        <v>1</v>
       </c>
       <c r="I52" t="s">
-        <v>86</v>
+        <v>118</v>
       </c>
       <c r="J52" t="s">
         <v>82</v>
       </c>
-      <c r="K52" s="1" t="s">
+      <c r="K52" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="L52" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="L52" s="1" t="s">
+      <c r="M52" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="M52" s="6" t="s">
+      <c r="N52" t="s">
+        <v>178</v>
+      </c>
+      <c r="O52" s="2" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" s="9">
+        <v>1</v>
+      </c>
+      <c r="C53" s="9">
+        <v>7</v>
+      </c>
+      <c r="G53" s="9">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I53" t="s">
+        <v>86</v>
+      </c>
+      <c r="J53" t="s">
+        <v>82</v>
+      </c>
+      <c r="K53" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>late</v>
+      </c>
+      <c r="L53" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="M53" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="N53" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="N52" s="2" t="s">
+      <c r="O53" s="2" t="s">
         <v>173</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:M41">
-    <sortCondition ref="J2:J41"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:N42">
+    <sortCondition ref="J2:J42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
@@ -2785,21 +3073,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="7.85546875"/>
-    <col min="3" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="8.54296875"/>
+    <col min="2" max="2" width="7.81640625"/>
+    <col min="3" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
@@ -2807,7 +3095,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2815,7 +3103,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2823,7 +3111,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2831,7 +3119,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2846,22 +3134,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.5703125"/>
-    <col min="2" max="2" width="14.42578125" style="1"/>
+    <col min="1" max="1" width="8.54296875"/>
+    <col min="2" max="2" width="14.453125" style="1"/>
     <col min="3" max="3" width="14"/>
-    <col min="4" max="1025" width="8.5703125"/>
+    <col min="4" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>90</v>
       </c>
@@ -2872,56 +3160,56 @@
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <f>COUNTA(Deck!C2:C112)</f>
+        <f>COUNTA(Deck!C2:C113)</f>
         <v>22</v>
       </c>
       <c r="C2" s="1">
-        <f>SUM(Deck!C2:C111)</f>
+        <f>SUM(Deck!C2:C112)</f>
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <f>COUNTA(Deck!D2:D112)</f>
+        <f>COUNTA(Deck!D2:D113)</f>
         <v>19</v>
       </c>
       <c r="C3" s="1">
-        <f>SUM(Deck!D2:D111)</f>
+        <f>SUM(Deck!D2:D112)</f>
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="1">
-        <f>COUNTA(Deck!E2:E112)</f>
+        <f>COUNTA(Deck!E2:E113)</f>
         <v>17</v>
       </c>
       <c r="C4" s="1">
-        <f>SUM(Deck!E2:E111)</f>
+        <f>SUM(Deck!E2:E112)</f>
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="1">
-        <f>COUNTA(Deck!F2:F112)</f>
-        <v>15</v>
+        <f>COUNTA(Deck!F2:F113)</f>
+        <v>16</v>
       </c>
       <c r="C5" s="1">
-        <f>SUM(Deck!F2:F112)</f>
-        <v>31</v>
+        <f>SUM(Deck!F2:F113)</f>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new concept art, new font
</commit_message>
<xml_diff>
--- a/data/deck.xlsx
+++ b/data/deck.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\project spider monkey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D4A9948-4751-40AC-8BCA-314A686E9798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98C3246F-CB20-4229-A0EF-7A155748518B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" tabRatio="989" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="225">
   <si>
     <t>Name</t>
   </si>
@@ -701,6 +701,9 @@
   </si>
   <si>
     <t>Stage</t>
+  </si>
+  <si>
+    <t>*At game end, +2/+5 VP if you have 2/3 Ancient artifacts (count this bonus only once)</t>
   </si>
 </sst>
 </file>
@@ -1118,7 +1121,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K4" sqref="K4"/>
+      <selection pane="bottomRight" activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1425,7 +1428,7 @@
         <v>214</v>
       </c>
       <c r="N9" t="s">
-        <v>188</v>
+        <v>224</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>124</v>

</xml_diff>